<commit_message>
Verificando se o teste pega bem o problema
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4,24 +4,22 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
     <sheet name="Configs" sheetId="1" r:id="rId2"/>
-    <sheet name="Dados_Projetados" sheetId="2" r:id="rId3"/>
-    <sheet name="Cenarios" sheetId="9" r:id="rId4"/>
-    <sheet name="Parametros" sheetId="4" r:id="rId5"/>
-    <sheet name="Funcoes_Inputs" sheetId="11" r:id="rId6"/>
-    <sheet name="Funcoes_Outputs" sheetId="12" r:id="rId7"/>
-    <sheet name="Distribuições" sheetId="10" r:id="rId8"/>
-    <sheet name="Categorias" sheetId="13" r:id="rId9"/>
-    <sheet name="Custos" sheetId="8" r:id="rId10"/>
-    <sheet name="Benefícios_Capturados" sheetId="3" r:id="rId11"/>
+    <sheet name="Parametros" sheetId="4" r:id="rId3"/>
+    <sheet name="Funcoes_Inputs" sheetId="11" r:id="rId4"/>
+    <sheet name="Funcoes_Outputs" sheetId="12" r:id="rId5"/>
+    <sheet name="Distribuições" sheetId="10" r:id="rId6"/>
+    <sheet name="Categorias" sheetId="13" r:id="rId7"/>
+    <sheet name="Custos" sheetId="8" r:id="rId8"/>
+    <sheet name="Benefícios_Capturados" sheetId="3" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lista_de_Parâmetros!$A$1:$F$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Parametros!$A$1:$G$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Parametros!$A$1:$G$10</definedName>
     <definedName name="Ano_Inicial">Configs!$D$2:$D$2</definedName>
     <definedName name="Anos_a_Serem_Simulados">Configs!$A$2</definedName>
     <definedName name="CategoriaSAT">Configs!$C$2:$C$2</definedName>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="126">
   <si>
     <t>Ano</t>
   </si>
@@ -44,9 +42,6 @@
     <t>Funcionarios</t>
   </si>
   <si>
-    <t>FolhadePagamento</t>
-  </si>
-  <si>
     <t>CategoriaSAT</t>
   </si>
   <si>
@@ -56,21 +51,6 @@
     <t>AnosaSeremSimulados</t>
   </si>
   <si>
-    <t>SalarioMedio</t>
-  </si>
-  <si>
-    <t>SATProjetado</t>
-  </si>
-  <si>
-    <t>IndiceDoSAT</t>
-  </si>
-  <si>
-    <t>FAPProjetado</t>
-  </si>
-  <si>
-    <t>DespesaSATProjetada</t>
-  </si>
-  <si>
     <t>NomeVariavel</t>
   </si>
   <si>
@@ -200,30 +180,6 @@
     <t>NomeIniciativa10</t>
   </si>
   <si>
-    <t>Iniciativa3</t>
-  </si>
-  <si>
-    <t>Iniciativa4</t>
-  </si>
-  <si>
-    <t>Iniciativa5</t>
-  </si>
-  <si>
-    <t>Iniciativa6</t>
-  </si>
-  <si>
-    <t>Iniciativa7</t>
-  </si>
-  <si>
-    <t>Iniciativa8</t>
-  </si>
-  <si>
-    <t>Iniciativa9</t>
-  </si>
-  <si>
-    <t>Iniciativa10</t>
-  </si>
-  <si>
     <t>TodasIniciativas</t>
   </si>
   <si>
@@ -239,13 +195,7 @@
     <t>Replicacoes</t>
   </si>
   <si>
-    <t>Simular</t>
-  </si>
-  <si>
     <t>Cenario</t>
-  </si>
-  <si>
-    <t>CenarioASIS</t>
   </si>
   <si>
     <t>CustoTotal</t>
@@ -518,12 +468,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -531,16 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -550,12 +490,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -884,412 +822,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>29</v>
+      <c r="A1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F5"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="12">
-        <v>2017</v>
-      </c>
-      <c r="D2" s="4">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="12">
-        <v>2018</v>
-      </c>
-      <c r="D3" s="4">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="12">
-        <v>2019</v>
-      </c>
-      <c r="D4" s="4">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="12">
-        <v>2020</v>
-      </c>
-      <c r="D5" s="4">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="12">
-        <v>2021</v>
-      </c>
-      <c r="D6" s="4">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="12">
-        <v>2017</v>
-      </c>
-      <c r="D7" s="4">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="12">
-        <v>2018</v>
-      </c>
-      <c r="D8" s="4">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="12">
-        <v>2019</v>
-      </c>
-      <c r="D9" s="4">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="12">
-        <v>2020</v>
-      </c>
-      <c r="D10" s="4">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="12">
-        <v>2021</v>
-      </c>
-      <c r="D11" s="4">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="12">
-        <v>2017</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="12">
-        <v>2018</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="12">
-        <v>2019</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="12">
-        <v>2020</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="12">
-        <v>2021</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="12">
-        <v>2017</v>
-      </c>
-      <c r="D17" s="4">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="12">
-        <v>2018</v>
-      </c>
-      <c r="D18" s="4">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="12">
-        <v>2019</v>
-      </c>
-      <c r="D19" s="4">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="12">
-        <v>2020</v>
-      </c>
-      <c r="D20" s="4">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="12">
-        <v>2021</v>
-      </c>
-      <c r="D21" s="4">
-        <v>150000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
@@ -1320,58 +931,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -1401,10 +1012,10 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1418,538 +1029,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="4" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <f>Ano_Inicial</f>
-        <v>2017</v>
-      </c>
-      <c r="B2" s="2">
-        <v>3000</v>
-      </c>
-      <c r="C2" s="8">
-        <f>B2*850</f>
-        <v>2550000</v>
-      </c>
-      <c r="D2" s="5">
-        <v>750</v>
-      </c>
-      <c r="E2" s="5">
-        <f>F2*C2</f>
-        <v>153000</v>
-      </c>
-      <c r="F2" s="7">
-        <f>G2*H2</f>
-        <v>0.06</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="H2">
-        <f>CategoriaSAT</f>
-        <v>3</v>
-      </c>
-      <c r="I2" s="14">
-        <v>8</v>
-      </c>
-      <c r="J2" s="14">
-        <v>20</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M2">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <f t="shared" ref="A3:A6" si="0">IFERROR(IF(A2+1&lt;=Anos_a_Serem_Simulados+Ano_Inicial-1,A2+1,""),"")</f>
-        <v>2018</v>
-      </c>
-      <c r="B3" s="2">
-        <f>ROUND(B2*1.005,0)</f>
-        <v>3015</v>
-      </c>
-      <c r="C3" s="8">
-        <f t="shared" ref="C3:C6" si="1">B3*850</f>
-        <v>2562750</v>
-      </c>
-      <c r="D3" s="4">
-        <f>ROUND(D2*1.08,2)</f>
-        <v>810</v>
-      </c>
-      <c r="E3" s="5">
-        <f t="shared" ref="E3:E6" si="2">F3*C3</f>
-        <v>153765</v>
-      </c>
-      <c r="F3" s="7">
-        <f t="shared" ref="F3:F6" si="3">G3*H3</f>
-        <v>0.06</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H6" si="4">CategoriaSAT</f>
-        <v>3</v>
-      </c>
-      <c r="I3" s="14">
-        <v>8</v>
-      </c>
-      <c r="J3" s="14">
-        <v>20</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M3">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <f t="shared" si="0"/>
-        <v>2019</v>
-      </c>
-      <c r="B4" s="2">
-        <f t="shared" ref="B4:B6" si="5">ROUND(B3*1.005,0)</f>
-        <v>3030</v>
-      </c>
-      <c r="C4" s="8">
-        <f t="shared" si="1"/>
-        <v>2575500</v>
-      </c>
-      <c r="D4" s="4">
-        <f t="shared" ref="D4:D6" si="6">ROUND(D3*1.08,2)</f>
-        <v>874.8</v>
-      </c>
-      <c r="E4" s="5">
-        <f t="shared" si="2"/>
-        <v>154530</v>
-      </c>
-      <c r="F4" s="7">
-        <f t="shared" si="3"/>
-        <v>0.06</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="I4" s="14">
-        <v>8</v>
-      </c>
-      <c r="J4" s="14">
-        <v>20</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M4">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <f t="shared" si="0"/>
-        <v>2020</v>
-      </c>
-      <c r="B5" s="2">
-        <f t="shared" si="5"/>
-        <v>3045</v>
-      </c>
-      <c r="C5" s="8">
-        <f t="shared" si="1"/>
-        <v>2588250</v>
-      </c>
-      <c r="D5" s="4">
-        <f t="shared" si="6"/>
-        <v>944.78</v>
-      </c>
-      <c r="E5" s="5">
-        <f t="shared" si="2"/>
-        <v>155295</v>
-      </c>
-      <c r="F5" s="7">
-        <f t="shared" si="3"/>
-        <v>0.06</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="I5" s="14">
-        <v>8</v>
-      </c>
-      <c r="J5" s="14">
-        <v>20</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M5">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <f t="shared" si="0"/>
-        <v>2021</v>
-      </c>
-      <c r="B6" s="2">
-        <f t="shared" si="5"/>
-        <v>3060</v>
-      </c>
-      <c r="C6" s="8">
-        <f t="shared" si="1"/>
-        <v>2601000</v>
-      </c>
-      <c r="D6" s="4">
-        <f t="shared" si="6"/>
-        <v>1020.36</v>
-      </c>
-      <c r="E6" s="5">
-        <f t="shared" si="2"/>
-        <v>156060</v>
-      </c>
-      <c r="F6" s="7">
-        <f t="shared" si="3"/>
-        <v>0.06</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="I6" s="14">
-        <v>8</v>
-      </c>
-      <c r="J6" s="14">
-        <v>20</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M6">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C7" s="8"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="8"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="8"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="8"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="8"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="C2" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="C3" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="C4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="C5" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="C6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="C7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="C8" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="C9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="C10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="C11" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="C12" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="C13" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G26" sqref="F26:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1963,34 +1046,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="9" t="s">
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>84</v>
-      </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C2">
         <v>3.0000000000000001E-3</v>
@@ -1998,18 +1081,18 @@
       <c r="D2">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C3">
         <v>5.0000000000000001E-3</v>
@@ -2018,15 +1101,15 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C4">
         <v>2E-3</v>
@@ -2035,15 +1118,15 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C5">
         <v>2E-3</v>
@@ -2052,15 +1135,15 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C6">
         <v>1E-3</v>
@@ -2069,15 +1152,15 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <v>0.4</v>
@@ -2086,15 +1169,15 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C8">
         <v>0.3</v>
@@ -2103,15 +1186,15 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C9">
         <v>0.2</v>
@@ -2120,15 +1203,15 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C10">
         <v>0.1</v>
@@ -2137,15 +1220,15 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>84</v>
+      <c r="A11" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C11">
         <v>3.0000000000000001E-3</v>
@@ -2153,18 +1236,18 @@
       <c r="D11">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C12">
         <v>5.0000000000000001E-3</v>
@@ -2173,15 +1256,15 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C13">
         <v>2E-3</v>
@@ -2190,15 +1273,15 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C14">
         <v>2E-3</v>
@@ -2207,15 +1290,15 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C15">
         <v>1E-3</v>
@@ -2224,15 +1307,15 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G15" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C16">
         <v>0.4</v>
@@ -2241,15 +1324,15 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C17">
         <v>0.3</v>
@@ -2258,15 +1341,15 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C18">
         <v>0.2</v>
@@ -2275,15 +1358,15 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C19">
         <v>0.1</v>
@@ -2292,15 +1375,15 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C20">
         <v>100</v>
@@ -2309,15 +1392,15 @@
         <v>30</v>
       </c>
       <c r="G20" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C21">
         <v>100</v>
@@ -2326,15 +1409,15 @@
         <v>30</v>
       </c>
       <c r="G21" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -2343,15 +1426,15 @@
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -2360,15 +1443,15 @@
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -2377,15 +1460,15 @@
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C25">
         <v>5</v>
@@ -2394,15 +1477,15 @@
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C26">
         <v>5</v>
@@ -2411,15 +1494,15 @@
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C27">
         <v>5</v>
@@ -2428,15 +1511,15 @@
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C28">
         <v>5</v>
@@ -2445,15 +1528,15 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C29">
         <v>5</v>
@@ -2462,15 +1545,15 @@
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C30">
         <v>5</v>
@@ -2479,15 +1562,15 @@
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C31">
         <v>5</v>
@@ -2496,15 +1579,15 @@
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -2513,15 +1596,15 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C33">
         <v>5</v>
@@ -2530,15 +1613,15 @@
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C34">
         <v>5</v>
@@ -2547,15 +1630,15 @@
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C35">
         <v>5</v>
@@ -2564,15 +1647,15 @@
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C36">
         <v>5</v>
@@ -2581,15 +1664,15 @@
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C37">
         <v>5</v>
@@ -2598,15 +1681,15 @@
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C38">
         <v>5</v>
@@ -2615,15 +1698,15 @@
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="B39" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C39">
         <v>5</v>
@@ -2632,15 +1715,15 @@
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C40">
         <v>5</v>
@@ -2649,15 +1732,15 @@
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C41">
         <v>5</v>
@@ -2666,7 +1749,7 @@
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2676,7 +1759,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
@@ -2693,18 +1776,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2716,10 +1799,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C3" t="b">
         <f>TRUE</f>
@@ -2728,10 +1811,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C4" t="b">
         <f>TRUE</f>
@@ -2740,10 +1823,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C5" t="b">
         <f>TRUE</f>
@@ -2752,10 +1835,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C6" t="b">
         <f>TRUE</f>
@@ -2764,10 +1847,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C7" t="b">
         <f>TRUE</f>
@@ -2776,10 +1859,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C8" t="b">
         <f>TRUE</f>
@@ -2788,10 +1871,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C9" t="b">
         <f>TRUE</f>
@@ -2800,10 +1883,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="C10" t="b">
         <f>TRUE</f>
@@ -2812,10 +1895,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C11" t="b">
         <f>TRUE</f>
@@ -2824,7 +1907,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -2836,10 +1919,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C13" t="b">
         <f>FALSE</f>
@@ -2848,10 +1931,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C14" t="b">
         <f>FALSE</f>
@@ -2860,10 +1943,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="C15" t="b">
         <f>FALSE</f>
@@ -2872,10 +1955,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B16" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="C16" t="b">
         <f>FALSE</f>
@@ -2884,10 +1967,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C17" t="b">
         <f>FALSE</f>
@@ -2896,10 +1979,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C18" t="b">
         <f>FALSE</f>
@@ -2908,10 +1991,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C19" t="b">
         <f>FALSE</f>
@@ -2920,10 +2003,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="C20" t="b">
         <f>FALSE</f>
@@ -2932,10 +2015,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="C21" t="b">
         <f>TRUE</f>
@@ -2944,7 +2027,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -2956,10 +2039,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C23" t="b">
         <f>FALSE</f>
@@ -2968,10 +2051,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C24" t="b">
         <f>FALSE</f>
@@ -2980,10 +2063,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B25" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C25" t="b">
         <f>TRUE</f>
@@ -2992,10 +2075,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C26" t="b">
         <f>FALSE</f>
@@ -3004,10 +2087,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C27" t="b">
         <f>FALSE</f>
@@ -3016,10 +2099,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="C28" t="b">
         <f>FALSE</f>
@@ -3028,10 +2111,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C29" t="b">
         <f>FALSE</f>
@@ -3040,10 +2123,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B30" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C30" t="b">
         <f>FALSE</f>
@@ -3052,7 +2135,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B31" t="str">
         <f>"ProbMulta_"&amp;D31</f>
@@ -3063,12 +2146,12 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B32" t="str">
         <f>"ProbMulta_"&amp;D32</f>
@@ -3079,12 +2162,12 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B33" t="str">
         <f>"ProbMulta_"&amp;D33</f>
@@ -3095,12 +2178,12 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B34" t="str">
         <f>"CustoMedioMulta_"&amp;D34</f>
@@ -3111,12 +2194,12 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B35" t="str">
         <f>"CustoMedioMulta_"&amp;D35</f>
@@ -3127,12 +2210,12 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B36" t="str">
         <f>"CustoMedioMulta_"&amp;D36</f>
@@ -3143,12 +2226,12 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B37" t="str">
         <f>"Atendimento_"&amp;D37</f>
@@ -3159,12 +2242,12 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" ref="B38:B39" si="0">"Atendimento_"&amp;D38</f>
@@ -3175,12 +2258,12 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
@@ -3191,15 +2274,15 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B40" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="C40" t="b">
         <f>FALSE</f>
@@ -3208,10 +2291,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" t="s">
         <v>124</v>
-      </c>
-      <c r="B41" t="s">
-        <v>140</v>
       </c>
       <c r="C41" t="b">
         <f>FALSE</f>
@@ -3220,10 +2303,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B42" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="C42" t="b">
         <f>FALSE</f>
@@ -3232,10 +2315,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C43" t="b">
         <f>FALSE</f>
@@ -3244,10 +2327,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B44" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C44" t="b">
         <f>FALSE</f>
@@ -3256,10 +2339,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C45" t="b">
         <f>FALSE</f>
@@ -3268,10 +2351,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B46" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C46" t="b">
         <f>FALSE</f>
@@ -3280,10 +2363,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C47" t="b">
         <f>FALSE</f>
@@ -3292,10 +2375,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C48" t="b">
         <f>FALSE</f>
@@ -3304,10 +2387,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B49" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="C49" t="b">
         <f>FALSE</f>
@@ -3316,10 +2399,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C50" t="b">
         <f>FALSE</f>
@@ -3332,7 +2415,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -3349,261 +2432,261 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B22" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B24" t="str">
         <f>"NumeroMultas_"&amp;C24</f>
         <v>NumeroMultas_Lei1</v>
       </c>
       <c r="C24" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" ref="B25:B26" si="0">"NumeroMultas_"&amp;C25</f>
         <v>NumeroMultas_Lei2</v>
       </c>
       <c r="C25" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
         <v>NumeroMultas_Lei3</v>
       </c>
       <c r="C26" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B27" t="str">
         <f>"ProbMultaAjustada_"&amp;C27</f>
         <v>ProbMultaAjustada_Lei1</v>
       </c>
       <c r="C27" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B28" t="str">
         <f>"ProbMultaAjustada_"&amp;C28</f>
         <v>ProbMultaAjustada_Lei2</v>
       </c>
       <c r="C28" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B29" t="str">
         <f>"ProbMultaAjustada_"&amp;C29</f>
         <v>ProbMultaAjustada_Lei3</v>
       </c>
       <c r="C29" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -3611,7 +2694,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -3629,55 +2712,55 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -3685,7 +2768,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -3697,25 +2780,352 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="7">
+        <v>2017</v>
+      </c>
+      <c r="D2" s="3">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2018</v>
+      </c>
+      <c r="D3" s="3">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2019</v>
+      </c>
+      <c r="D4" s="3">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2020</v>
+      </c>
+      <c r="D5" s="3">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="7">
+        <v>2021</v>
+      </c>
+      <c r="D6" s="3">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="7">
+        <v>2017</v>
+      </c>
+      <c r="D7" s="3">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="7">
+        <v>2018</v>
+      </c>
+      <c r="D8" s="3">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="7">
+        <v>2019</v>
+      </c>
+      <c r="D9" s="3">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="7">
+        <v>2020</v>
+      </c>
+      <c r="D10" s="3">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="7">
+        <v>2021</v>
+      </c>
+      <c r="D11" s="3">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="7">
+        <v>2017</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2018</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="7">
+        <v>2019</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2020</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="7">
+        <v>2021</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="7">
+        <v>2017</v>
+      </c>
+      <c r="D17" s="3">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="7">
+        <v>2018</v>
+      </c>
+      <c r="D18" s="3">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2019</v>
+      </c>
+      <c r="D19" s="3">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="7">
+        <v>2020</v>
+      </c>
+      <c r="D20" s="3">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="7">
+        <v>2021</v>
+      </c>
+      <c r="D21" s="3">
+        <v>150000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Voltando ao arquivo de dados original.
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4,22 +4,24 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
     <sheet name="Configs" sheetId="1" r:id="rId2"/>
-    <sheet name="Parametros" sheetId="4" r:id="rId3"/>
-    <sheet name="Funcoes_Inputs" sheetId="11" r:id="rId4"/>
-    <sheet name="Funcoes_Outputs" sheetId="12" r:id="rId5"/>
-    <sheet name="Distribuições" sheetId="10" r:id="rId6"/>
-    <sheet name="Categorias" sheetId="13" r:id="rId7"/>
-    <sheet name="Custos" sheetId="8" r:id="rId8"/>
-    <sheet name="Benefícios_Capturados" sheetId="3" r:id="rId9"/>
+    <sheet name="Dados_Projetados" sheetId="2" r:id="rId3"/>
+    <sheet name="Cenarios" sheetId="9" r:id="rId4"/>
+    <sheet name="Parametros" sheetId="4" r:id="rId5"/>
+    <sheet name="Funcoes_Inputs" sheetId="11" r:id="rId6"/>
+    <sheet name="Funcoes_Outputs" sheetId="12" r:id="rId7"/>
+    <sheet name="Distribuições" sheetId="10" r:id="rId8"/>
+    <sheet name="Categorias" sheetId="13" r:id="rId9"/>
+    <sheet name="Custos" sheetId="8" r:id="rId10"/>
+    <sheet name="Benefícios_Capturados" sheetId="3" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lista_de_Parâmetros!$A$1:$F$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Parametros!$A$1:$G$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Parametros!$A$1:$G$10</definedName>
     <definedName name="Ano_Inicial">Configs!$D$2:$D$2</definedName>
     <definedName name="Anos_a_Serem_Simulados">Configs!$A$2</definedName>
     <definedName name="CategoriaSAT">Configs!$C$2:$C$2</definedName>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="142">
   <si>
     <t>Ano</t>
   </si>
@@ -42,6 +44,9 @@
     <t>Funcionarios</t>
   </si>
   <si>
+    <t>FolhadePagamento</t>
+  </si>
+  <si>
     <t>CategoriaSAT</t>
   </si>
   <si>
@@ -51,6 +56,21 @@
     <t>AnosaSeremSimulados</t>
   </si>
   <si>
+    <t>SalarioMedio</t>
+  </si>
+  <si>
+    <t>SATProjetado</t>
+  </si>
+  <si>
+    <t>IndiceDoSAT</t>
+  </si>
+  <si>
+    <t>FAPProjetado</t>
+  </si>
+  <si>
+    <t>DespesaSATProjetada</t>
+  </si>
+  <si>
     <t>NomeVariavel</t>
   </si>
   <si>
@@ -180,6 +200,30 @@
     <t>NomeIniciativa10</t>
   </si>
   <si>
+    <t>Iniciativa3</t>
+  </si>
+  <si>
+    <t>Iniciativa4</t>
+  </si>
+  <si>
+    <t>Iniciativa5</t>
+  </si>
+  <si>
+    <t>Iniciativa6</t>
+  </si>
+  <si>
+    <t>Iniciativa7</t>
+  </si>
+  <si>
+    <t>Iniciativa8</t>
+  </si>
+  <si>
+    <t>Iniciativa9</t>
+  </si>
+  <si>
+    <t>Iniciativa10</t>
+  </si>
+  <si>
     <t>TodasIniciativas</t>
   </si>
   <si>
@@ -195,7 +239,13 @@
     <t>Replicacoes</t>
   </si>
   <si>
+    <t>Simular</t>
+  </si>
+  <si>
     <t>Cenario</t>
+  </si>
+  <si>
+    <t>CenarioASIS</t>
   </si>
   <si>
     <t>CustoTotal</t>
@@ -468,11 +518,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -480,7 +531,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -490,10 +550,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -822,85 +884,412 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>23</v>
+      <c r="A1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
         <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F5"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="12">
+        <v>2017</v>
+      </c>
+      <c r="D2" s="4">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="12">
+        <v>2018</v>
+      </c>
+      <c r="D3" s="4">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="12">
+        <v>2019</v>
+      </c>
+      <c r="D4" s="4">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="12">
+        <v>2020</v>
+      </c>
+      <c r="D5" s="4">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="12">
+        <v>2021</v>
+      </c>
+      <c r="D6" s="4">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="12">
+        <v>2017</v>
+      </c>
+      <c r="D7" s="4">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="12">
+        <v>2018</v>
+      </c>
+      <c r="D8" s="4">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="12">
+        <v>2019</v>
+      </c>
+      <c r="D9" s="4">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="12">
+        <v>2020</v>
+      </c>
+      <c r="D10" s="4">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="12">
+        <v>2021</v>
+      </c>
+      <c r="D11" s="4">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="12">
+        <v>2017</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="12">
+        <v>2018</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="12">
+        <v>2019</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="12">
+        <v>2020</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="12">
+        <v>2021</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="12">
+        <v>2017</v>
+      </c>
+      <c r="D17" s="4">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="12">
+        <v>2018</v>
+      </c>
+      <c r="D18" s="4">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="12">
+        <v>2019</v>
+      </c>
+      <c r="D19" s="4">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="12">
+        <v>2020</v>
+      </c>
+      <c r="D20" s="4">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="12">
+        <v>2021</v>
+      </c>
+      <c r="D21" s="4">
+        <v>150000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
@@ -931,58 +1320,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -1012,10 +1401,10 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1029,10 +1418,538 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <f>Ano_Inicial</f>
+        <v>2017</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3000</v>
+      </c>
+      <c r="C2" s="8">
+        <f>B2*850</f>
+        <v>2550000</v>
+      </c>
+      <c r="D2" s="5">
+        <v>750</v>
+      </c>
+      <c r="E2" s="5">
+        <f>F2*C2</f>
+        <v>153000</v>
+      </c>
+      <c r="F2" s="7">
+        <f>G2*H2</f>
+        <v>0.06</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="H2">
+        <f>CategoriaSAT</f>
+        <v>3</v>
+      </c>
+      <c r="I2" s="14">
+        <v>8</v>
+      </c>
+      <c r="J2" s="14">
+        <v>20</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <f t="shared" ref="A3:A6" si="0">IFERROR(IF(A2+1&lt;=Anos_a_Serem_Simulados+Ano_Inicial-1,A2+1,""),"")</f>
+        <v>2018</v>
+      </c>
+      <c r="B3" s="2">
+        <f>ROUND(B2*1.005,0)</f>
+        <v>3015</v>
+      </c>
+      <c r="C3" s="8">
+        <f t="shared" ref="C3:C6" si="1">B3*850</f>
+        <v>2562750</v>
+      </c>
+      <c r="D3" s="4">
+        <f>ROUND(D2*1.08,2)</f>
+        <v>810</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E6" si="2">F3*C3</f>
+        <v>153765</v>
+      </c>
+      <c r="F3" s="7">
+        <f t="shared" ref="F3:F6" si="3">G3*H3</f>
+        <v>0.06</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H6" si="4">CategoriaSAT</f>
+        <v>3</v>
+      </c>
+      <c r="I3" s="14">
+        <v>8</v>
+      </c>
+      <c r="J3" s="14">
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <f t="shared" si="0"/>
+        <v>2019</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" ref="B4:B6" si="5">ROUND(B3*1.005,0)</f>
+        <v>3030</v>
+      </c>
+      <c r="C4" s="8">
+        <f t="shared" si="1"/>
+        <v>2575500</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" ref="D4:D6" si="6">ROUND(D3*1.08,2)</f>
+        <v>874.8</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="2"/>
+        <v>154530</v>
+      </c>
+      <c r="F4" s="7">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="I4" s="14">
+        <v>8</v>
+      </c>
+      <c r="J4" s="14">
+        <v>20</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="5"/>
+        <v>3045</v>
+      </c>
+      <c r="C5" s="8">
+        <f t="shared" si="1"/>
+        <v>2588250</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="6"/>
+        <v>944.78</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="2"/>
+        <v>155295</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="I5" s="14">
+        <v>8</v>
+      </c>
+      <c r="J5" s="14">
+        <v>20</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <f t="shared" si="0"/>
+        <v>2021</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="5"/>
+        <v>3060</v>
+      </c>
+      <c r="C6" s="8">
+        <f t="shared" si="1"/>
+        <v>2601000</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="6"/>
+        <v>1020.36</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="2"/>
+        <v>156060</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="I6" s="14">
+        <v>8</v>
+      </c>
+      <c r="J6" s="14">
+        <v>20</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C7" s="8"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C8" s="8"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C9" s="8"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C10" s="8"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C11" s="8"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C2" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="C4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="C6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="C7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="C8" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="C9" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="C10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="C11" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="C12" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="C13" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="F26:G26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,34 +1963,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>53</v>
+      <c r="D1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>68</v>
+      <c r="A2" s="13" t="s">
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C2">
         <v>3.0000000000000001E-3</v>
@@ -1081,18 +1998,18 @@
       <c r="D2">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C3">
         <v>5.0000000000000001E-3</v>
@@ -1101,15 +2018,15 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C4">
         <v>2E-3</v>
@@ -1118,15 +2035,15 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C5">
         <v>2E-3</v>
@@ -1135,15 +2052,15 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C6">
         <v>1E-3</v>
@@ -1152,15 +2069,15 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C7">
         <v>0.4</v>
@@ -1169,15 +2086,15 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C8">
         <v>0.3</v>
@@ -1186,15 +2103,15 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C9">
         <v>0.2</v>
@@ -1203,15 +2120,15 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C10">
         <v>0.1</v>
@@ -1220,15 +2137,15 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>68</v>
+      <c r="A11" s="13" t="s">
+        <v>84</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C11">
         <v>3.0000000000000001E-3</v>
@@ -1236,18 +2153,18 @@
       <c r="D11">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C12">
         <v>5.0000000000000001E-3</v>
@@ -1256,15 +2173,15 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C13">
         <v>2E-3</v>
@@ -1273,15 +2190,15 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G13" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C14">
         <v>2E-3</v>
@@ -1290,15 +2207,15 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G14" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C15">
         <v>1E-3</v>
@@ -1307,15 +2224,15 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G15" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C16">
         <v>0.4</v>
@@ -1324,15 +2241,15 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C17">
         <v>0.3</v>
@@ -1341,15 +2258,15 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C18">
         <v>0.2</v>
@@ -1358,15 +2275,15 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C19">
         <v>0.1</v>
@@ -1375,15 +2292,15 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C20">
         <v>100</v>
@@ -1392,15 +2309,15 @@
         <v>30</v>
       </c>
       <c r="G20" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C21">
         <v>100</v>
@@ -1409,15 +2326,15 @@
         <v>30</v>
       </c>
       <c r="G21" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -1426,15 +2343,15 @@
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -1443,15 +2360,15 @@
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -1460,15 +2377,15 @@
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C25">
         <v>5</v>
@@ -1477,15 +2394,15 @@
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C26">
         <v>5</v>
@@ -1494,15 +2411,15 @@
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C27">
         <v>5</v>
@@ -1511,15 +2428,15 @@
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C28">
         <v>5</v>
@@ -1528,15 +2445,15 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C29">
         <v>5</v>
@@ -1545,15 +2462,15 @@
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C30">
         <v>5</v>
@@ -1562,15 +2479,15 @@
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C31">
         <v>5</v>
@@ -1579,15 +2496,15 @@
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -1596,15 +2513,15 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="B33" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C33">
         <v>5</v>
@@ -1613,15 +2530,15 @@
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C34">
         <v>5</v>
@@ -1630,15 +2547,15 @@
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="B35" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C35">
         <v>5</v>
@@ -1647,15 +2564,15 @@
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C36">
         <v>5</v>
@@ -1664,15 +2581,15 @@
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C37">
         <v>5</v>
@@ -1681,15 +2598,15 @@
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C38">
         <v>5</v>
@@ -1698,15 +2615,15 @@
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C39">
         <v>5</v>
@@ -1715,15 +2632,15 @@
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C40">
         <v>5</v>
@@ -1732,15 +2649,15 @@
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C41">
         <v>5</v>
@@ -1749,7 +2666,7 @@
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1759,7 +2676,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
@@ -1776,18 +2693,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1799,10 +2716,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C3" t="b">
         <f>TRUE</f>
@@ -1811,10 +2728,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C4" t="b">
         <f>TRUE</f>
@@ -1823,10 +2740,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="C5" t="b">
         <f>TRUE</f>
@@ -1835,10 +2752,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="C6" t="b">
         <f>TRUE</f>
@@ -1847,10 +2764,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="C7" t="b">
         <f>TRUE</f>
@@ -1859,10 +2776,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="C8" t="b">
         <f>TRUE</f>
@@ -1871,10 +2788,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="C9" t="b">
         <f>TRUE</f>
@@ -1883,10 +2800,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="C10" t="b">
         <f>TRUE</f>
@@ -1895,10 +2812,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="C11" t="b">
         <f>TRUE</f>
@@ -1907,7 +2824,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -1919,10 +2836,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" t="s">
         <v>100</v>
-      </c>
-      <c r="B13" t="s">
-        <v>84</v>
       </c>
       <c r="C13" t="b">
         <f>FALSE</f>
@@ -1931,10 +2848,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="C14" t="b">
         <f>FALSE</f>
@@ -1943,10 +2860,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="C15" t="b">
         <f>FALSE</f>
@@ -1955,10 +2872,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="C16" t="b">
         <f>FALSE</f>
@@ -1967,10 +2884,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="C17" t="b">
         <f>FALSE</f>
@@ -1979,10 +2896,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C18" t="b">
         <f>FALSE</f>
@@ -1991,10 +2908,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="C19" t="b">
         <f>FALSE</f>
@@ -2003,10 +2920,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="C20" t="b">
         <f>FALSE</f>
@@ -2015,10 +2932,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="C21" t="b">
         <f>TRUE</f>
@@ -2027,7 +2944,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -2039,10 +2956,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C23" t="b">
         <f>FALSE</f>
@@ -2051,10 +2968,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C24" t="b">
         <f>FALSE</f>
@@ -2063,10 +2980,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="C25" t="b">
         <f>TRUE</f>
@@ -2075,10 +2992,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="C26" t="b">
         <f>FALSE</f>
@@ -2087,10 +3004,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C27" t="b">
         <f>FALSE</f>
@@ -2099,10 +3016,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="C28" t="b">
         <f>FALSE</f>
@@ -2111,10 +3028,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="C29" t="b">
         <f>FALSE</f>
@@ -2123,10 +3040,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C30" t="b">
         <f>FALSE</f>
@@ -2135,7 +3052,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B31" t="str">
         <f>"ProbMulta_"&amp;D31</f>
@@ -2146,12 +3063,12 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B32" t="str">
         <f>"ProbMulta_"&amp;D32</f>
@@ -2162,12 +3079,12 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B33" t="str">
         <f>"ProbMulta_"&amp;D33</f>
@@ -2178,12 +3095,12 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B34" t="str">
         <f>"CustoMedioMulta_"&amp;D34</f>
@@ -2194,12 +3111,12 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B35" t="str">
         <f>"CustoMedioMulta_"&amp;D35</f>
@@ -2210,12 +3127,12 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B36" t="str">
         <f>"CustoMedioMulta_"&amp;D36</f>
@@ -2226,12 +3143,12 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B37" t="str">
         <f>"Atendimento_"&amp;D37</f>
@@ -2242,12 +3159,12 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" ref="B38:B39" si="0">"Atendimento_"&amp;D38</f>
@@ -2258,12 +3175,12 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
@@ -2274,15 +3191,15 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B40" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="C40" t="b">
         <f>FALSE</f>
@@ -2291,10 +3208,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B41" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="C41" t="b">
         <f>FALSE</f>
@@ -2303,10 +3220,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B42" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="C42" t="b">
         <f>FALSE</f>
@@ -2315,10 +3232,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C43" t="b">
         <f>FALSE</f>
@@ -2327,10 +3244,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C44" t="b">
         <f>FALSE</f>
@@ -2339,10 +3256,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="C45" t="b">
         <f>FALSE</f>
@@ -2351,10 +3268,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B46" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="C46" t="b">
         <f>FALSE</f>
@@ -2363,10 +3280,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="C47" t="b">
         <f>FALSE</f>
@@ -2375,10 +3292,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>124</v>
+      </c>
+      <c r="B48" t="s">
         <v>108</v>
-      </c>
-      <c r="B48" t="s">
-        <v>92</v>
       </c>
       <c r="C48" t="b">
         <f>FALSE</f>
@@ -2387,10 +3304,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B49" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C49" t="b">
         <f>FALSE</f>
@@ -2399,10 +3316,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B50" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C50" t="b">
         <f>FALSE</f>
@@ -2415,7 +3332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -2432,261 +3349,261 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
         <v>99</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B21" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B23" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B24" t="str">
         <f>"NumeroMultas_"&amp;C24</f>
         <v>NumeroMultas_Lei1</v>
       </c>
       <c r="C24" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" ref="B25:B26" si="0">"NumeroMultas_"&amp;C25</f>
         <v>NumeroMultas_Lei2</v>
       </c>
       <c r="C25" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
         <v>NumeroMultas_Lei3</v>
       </c>
       <c r="C26" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B27" t="str">
         <f>"ProbMultaAjustada_"&amp;C27</f>
         <v>ProbMultaAjustada_Lei1</v>
       </c>
       <c r="C27" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B28" t="str">
         <f>"ProbMultaAjustada_"&amp;C28</f>
         <v>ProbMultaAjustada_Lei2</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B29" t="str">
         <f>"ProbMultaAjustada_"&amp;C29</f>
         <v>ProbMultaAjustada_Lei3</v>
       </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2694,7 +3611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2712,55 +3629,55 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2768,7 +3685,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -2780,352 +3697,25 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="7">
-        <v>2017</v>
-      </c>
-      <c r="D2" s="3">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="7">
-        <v>2018</v>
-      </c>
-      <c r="D3" s="3">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="7">
-        <v>2019</v>
-      </c>
-      <c r="D4" s="3">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="7">
-        <v>2020</v>
-      </c>
-      <c r="D5" s="3">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="7">
-        <v>2021</v>
-      </c>
-      <c r="D6" s="3">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="7">
-        <v>2017</v>
-      </c>
-      <c r="D7" s="3">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="7">
-        <v>2018</v>
-      </c>
-      <c r="D8" s="3">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="7">
-        <v>2019</v>
-      </c>
-      <c r="D9" s="3">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="7">
-        <v>2020</v>
-      </c>
-      <c r="D10" s="3">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="7">
-        <v>2021</v>
-      </c>
-      <c r="D11" s="3">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="7">
-        <v>2017</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="7">
-        <v>2018</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="7">
-        <v>2019</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="7">
-        <v>2020</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="7">
-        <v>2021</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="7">
-        <v>2017</v>
-      </c>
-      <c r="D17" s="3">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="7">
-        <v>2018</v>
-      </c>
-      <c r="D18" s="3">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="7">
-        <v>2019</v>
-      </c>
-      <c r="D19" s="3">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="7">
-        <v>2020</v>
-      </c>
-      <c r="D20" s="3">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="7">
-        <v>2021</v>
-      </c>
-      <c r="D21" s="3">
-        <v>150000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Calcular Multas (Com vari[avel Multas como Aleatória)
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="134">
   <si>
     <t>Ano</t>
   </si>
@@ -428,40 +428,16 @@
     <t>Lei3</t>
   </si>
   <si>
-    <t>ProbMulta_Lei1</t>
-  </si>
-  <si>
-    <t>ProbMulta_Lei2</t>
-  </si>
-  <si>
-    <t>ProbMulta_Lei3</t>
-  </si>
-  <si>
-    <t>CustoMedioMulta_Lei1</t>
-  </si>
-  <si>
-    <t>CustoMedioMulta_Lei2</t>
-  </si>
-  <si>
-    <t>CustoMedioMulta_Lei3</t>
-  </si>
-  <si>
     <t>Atendimento_Lei1</t>
   </si>
   <si>
-    <t>Atendimento_Lei2</t>
-  </si>
-  <si>
-    <t>Atendimento_Lei3</t>
-  </si>
-  <si>
     <t>Crise</t>
   </si>
   <si>
     <t>FatorCrise</t>
   </si>
   <si>
-    <t>FatorMultiplicativoMultas</t>
+    <t>NumeroMultasAPriori_Lei1</t>
   </si>
 </sst>
 </file>
@@ -1420,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,13 +1448,14 @@
         <v>21</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>141</v>
+        <v>132</v>
+      </c>
+      <c r="M1" s="9" t="str">
+        <f>"CustoMedioMulta_Lei1"</f>
+        <v>CustoMedioMulta_Lei1</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1518,13 +1495,13 @@
         <v>20</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>0.05</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1566,13 +1543,13 @@
         <v>20</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>0.05</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1617,10 +1594,10 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>0.05</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1665,10 +1642,10 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>0.05</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1713,10 +1690,10 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>0.05</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1946,15 +1923,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -2365,16 +2342,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B24" t="s">
         <v>71</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G24" t="s">
         <v>43</v>
@@ -2382,16 +2359,16 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B25" t="s">
         <v>71</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" t="s">
         <v>43</v>
@@ -2399,273 +2376,35 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B26" t="s">
         <v>71</v>
       </c>
       <c r="C26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G26" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
         <v>71</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>134</v>
-      </c>
-      <c r="B28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28">
-        <v>5</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="G28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>135</v>
-      </c>
-      <c r="B29" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29">
-        <v>5</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="G29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>136</v>
-      </c>
-      <c r="B30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30">
-        <v>5</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="G30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>137</v>
-      </c>
-      <c r="B31" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31">
-        <v>5</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="G31" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>138</v>
-      </c>
-      <c r="B32" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32">
-        <v>5</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="G32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>130</v>
-      </c>
-      <c r="B33" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33">
-        <v>5</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="G33" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>131</v>
-      </c>
-      <c r="B34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34">
-        <v>5</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="G34" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>132</v>
-      </c>
-      <c r="B35" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35">
-        <v>5</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="G35" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>133</v>
-      </c>
-      <c r="B36" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36">
-        <v>5</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="G36" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>134</v>
-      </c>
-      <c r="B37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37">
-        <v>5</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="G37" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>135</v>
-      </c>
-      <c r="B38" t="s">
-        <v>71</v>
-      </c>
-      <c r="C38">
-        <v>5</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="G38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>136</v>
-      </c>
-      <c r="B39" t="s">
-        <v>71</v>
-      </c>
-      <c r="C39">
-        <v>5</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="G39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>137</v>
-      </c>
-      <c r="B40" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40">
-        <v>5</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="G40" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>138</v>
-      </c>
-      <c r="B41" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41">
-        <v>5</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="G41" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2678,10 +2417,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B33" activeCellId="1" sqref="B31 B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3055,8 +2794,8 @@
         <v>124</v>
       </c>
       <c r="B31" t="str">
-        <f>"ProbMulta_"&amp;D31</f>
-        <v>ProbMulta_Lei1</v>
+        <f>"NumeroMultasAPriori_"&amp;D31</f>
+        <v>NumeroMultasAPriori_Lei1</v>
       </c>
       <c r="C31" t="b">
         <f>TRUE</f>
@@ -3071,15 +2810,15 @@
         <v>124</v>
       </c>
       <c r="B32" t="str">
-        <f>"ProbMulta_"&amp;D32</f>
-        <v>ProbMulta_Lei2</v>
+        <f>"CustoMedioMulta_"&amp;D32</f>
+        <v>CustoMedioMulta_Lei1</v>
       </c>
       <c r="C32" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3087,241 +2826,37 @@
         <v>124</v>
       </c>
       <c r="B33" t="str">
-        <f>"ProbMulta_"&amp;D33</f>
-        <v>ProbMulta_Lei3</v>
+        <f>"Atendimento_"&amp;D33</f>
+        <v>Atendimento_Lei1</v>
       </c>
       <c r="C33" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>124</v>
       </c>
-      <c r="B34" t="str">
-        <f>"CustoMedioMulta_"&amp;D34</f>
-        <v>CustoMedioMulta_Lei1</v>
+      <c r="B34" t="s">
+        <v>131</v>
       </c>
       <c r="C34" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>127</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>124</v>
       </c>
-      <c r="B35" t="str">
-        <f>"CustoMedioMulta_"&amp;D35</f>
-        <v>CustoMedioMulta_Lei2</v>
+      <c r="B35" t="s">
+        <v>132</v>
       </c>
       <c r="C35" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="D35" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>124</v>
-      </c>
-      <c r="B36" t="str">
-        <f>"CustoMedioMulta_"&amp;D36</f>
-        <v>CustoMedioMulta_Lei3</v>
-      </c>
-      <c r="C36" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>124</v>
-      </c>
-      <c r="B37" t="str">
-        <f>"Atendimento_"&amp;D37</f>
-        <v>Atendimento_Lei1</v>
-      </c>
-      <c r="C37" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>124</v>
-      </c>
-      <c r="B38" t="str">
-        <f t="shared" ref="B38:B39" si="0">"Atendimento_"&amp;D38</f>
-        <v>Atendimento_Lei2</v>
-      </c>
-      <c r="C38" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>124</v>
-      </c>
-      <c r="B39" t="str">
-        <f t="shared" si="0"/>
-        <v>Atendimento_Lei3</v>
-      </c>
-      <c r="C39" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>124</v>
-      </c>
-      <c r="B40" t="s">
-        <v>139</v>
-      </c>
-      <c r="C40" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>124</v>
-      </c>
-      <c r="B41" t="s">
-        <v>140</v>
-      </c>
-      <c r="C41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>124</v>
-      </c>
-      <c r="B42" t="s">
-        <v>141</v>
-      </c>
-      <c r="C42" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>124</v>
-      </c>
-      <c r="B43" t="s">
-        <v>99</v>
-      </c>
-      <c r="C43" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>124</v>
-      </c>
-      <c r="B44" t="s">
-        <v>100</v>
-      </c>
-      <c r="C44" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>124</v>
-      </c>
-      <c r="B45" t="s">
-        <v>101</v>
-      </c>
-      <c r="C45" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>124</v>
-      </c>
-      <c r="B46" t="s">
-        <v>102</v>
-      </c>
-      <c r="C46" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>124</v>
-      </c>
-      <c r="B47" t="s">
-        <v>107</v>
-      </c>
-      <c r="C47" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>124</v>
-      </c>
-      <c r="B48" t="s">
-        <v>108</v>
-      </c>
-      <c r="C48" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>124</v>
-      </c>
-      <c r="B49" t="s">
-        <v>109</v>
-      </c>
-      <c r="C49" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>124</v>
-      </c>
-      <c r="B50" t="s">
-        <v>110</v>
-      </c>
-      <c r="C50" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
@@ -3334,10 +2869,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B18"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3544,66 +3079,6 @@
       </c>
       <c r="C24" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>124</v>
-      </c>
-      <c r="B25" t="str">
-        <f t="shared" ref="B25:B26" si="0">"NumeroMultas_"&amp;C25</f>
-        <v>NumeroMultas_Lei2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>124</v>
-      </c>
-      <c r="B26" t="str">
-        <f t="shared" si="0"/>
-        <v>NumeroMultas_Lei3</v>
-      </c>
-      <c r="C26" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>124</v>
-      </c>
-      <c r="B27" t="str">
-        <f>"ProbMultaAjustada_"&amp;C27</f>
-        <v>ProbMultaAjustada_Lei1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>124</v>
-      </c>
-      <c r="B28" t="str">
-        <f>"ProbMultaAjustada_"&amp;C28</f>
-        <v>ProbMultaAjustada_Lei2</v>
-      </c>
-      <c r="C28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>124</v>
-      </c>
-      <c r="B29" t="str">
-        <f>"ProbMultaAjustada_"&amp;C29</f>
-        <v>ProbMultaAjustada_Lei3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ações Regressivas - Passando no Teste
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="143">
   <si>
     <t>Ano</t>
   </si>
@@ -438,6 +438,33 @@
   </si>
   <si>
     <t>NumeroMultasAPriori_Lei1</t>
+  </si>
+  <si>
+    <t>calcular_acoes_regressivas_inss</t>
+  </si>
+  <si>
+    <t>Nev_AcaoRegressivaINSS</t>
+  </si>
+  <si>
+    <t>Nev_AcaoRegressivaInicial</t>
+  </si>
+  <si>
+    <t>PAcaoRegressiva</t>
+  </si>
+  <si>
+    <t>CustoMedioAcaoRegressivaINSS</t>
+  </si>
+  <si>
+    <t>DespesaAcoesRegressivasINSS</t>
+  </si>
+  <si>
+    <t>AcoesRegressivasINSS</t>
+  </si>
+  <si>
+    <t>Nev_AcaoRegressivaINSSAcumulado</t>
+  </si>
+  <si>
+    <t>PInvalidez</t>
   </si>
 </sst>
 </file>
@@ -1394,10 +1421,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L6"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,9 +1441,10 @@
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1457,8 +1485,11 @@
         <f>"CustoMedioMulta_Lei1"</f>
         <v>CustoMedioMulta_Lei1</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <f>Ano_Inicial</f>
         <v>2017</v>
@@ -1503,8 +1534,11 @@
       <c r="M2">
         <v>1200</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f t="shared" ref="A3:A6" si="0">IFERROR(IF(A2+1&lt;=Anos_a_Serem_Simulados+Ano_Inicial-1,A2+1,""),"")</f>
         <v>2018</v>
@@ -1551,8 +1585,11 @@
       <c r="M3">
         <v>1200</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -1599,8 +1636,11 @@
       <c r="M4">
         <v>1200</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -1647,8 +1687,11 @@
       <c r="M5">
         <v>1200</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -1695,32 +1738,35 @@
       <c r="M6">
         <v>1200</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C7" s="8"/>
       <c r="E7" s="5"/>
       <c r="F7" s="7"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C8" s="8"/>
       <c r="E8" s="5"/>
       <c r="F8" s="7"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C9" s="8"/>
       <c r="E9" s="5"/>
       <c r="F9" s="7"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C10" s="8"/>
       <c r="E10" s="5"/>
       <c r="F10" s="7"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C11" s="8"/>
       <c r="E11" s="5"/>
       <c r="F11" s="7"/>
@@ -1923,15 +1969,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -2408,6 +2454,108 @@
         <v>17</v>
       </c>
     </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28">
+        <v>0.5</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29">
+        <v>0.5</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32">
+        <v>0.01</v>
+      </c>
+      <c r="D32">
+        <v>1E-3</v>
+      </c>
+      <c r="G32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33">
+        <v>0.01</v>
+      </c>
+      <c r="D33">
+        <v>1E-3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G10"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2417,10 +2565,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B33" activeCellId="1" sqref="B31 B33"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2861,6 +3009,78 @@
         <v>0</v>
       </c>
     </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>134</v>
+      </c>
+      <c r="B38" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>134</v>
+      </c>
+      <c r="B39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>134</v>
+      </c>
+      <c r="B42" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2869,10 +3089,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3079,6 +3299,38 @@
       </c>
       <c r="C24" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculo do BCR Fechou (Arredondando Eventos para Cima)
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Benefícios_Capturados" sheetId="3" r:id="rId11"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Custos!$A$1:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lista_de_Parâmetros!$A$1:$F$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Parametros!$A$1:$G$10</definedName>
     <definedName name="Ano_Inicial">Configs!$D$2:$D$2</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="143">
   <si>
     <t>Ano</t>
   </si>
@@ -971,11 +972,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1029,257 +1028,34 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
         <v>65</v>
       </c>
       <c r="C4" s="12">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="D4" s="4">
-        <v>50000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
         <v>65</v>
       </c>
       <c r="C5" s="12">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="D5" s="4">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="12">
-        <v>2021</v>
-      </c>
-      <c r="D6" s="4">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="12">
-        <v>2017</v>
-      </c>
-      <c r="D7" s="4">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="12">
-        <v>2018</v>
-      </c>
-      <c r="D8" s="4">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="12">
-        <v>2019</v>
-      </c>
-      <c r="D9" s="4">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="12">
-        <v>2020</v>
-      </c>
-      <c r="D10" s="4">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="12">
-        <v>2021</v>
-      </c>
-      <c r="D11" s="4">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="12">
-        <v>2017</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="12">
-        <v>2018</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="12">
-        <v>2019</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="12">
-        <v>2020</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="12">
-        <v>2021</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="12">
-        <v>2017</v>
-      </c>
-      <c r="D17" s="4">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="12">
-        <v>2018</v>
-      </c>
-      <c r="D18" s="4">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="12">
-        <v>2019</v>
-      </c>
-      <c r="D19" s="4">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="12">
-        <v>2020</v>
-      </c>
-      <c r="D20" s="4">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="12">
-        <v>2021</v>
-      </c>
-      <c r="D21" s="4">
-        <v>150000</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D5"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -1301,7 +1077,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,7 +1155,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>1000</v>
@@ -1423,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,16 +1299,16 @@
         <v>8</v>
       </c>
       <c r="J2" s="14">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="M2">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="N2">
         <v>15000</v>
@@ -1540,207 +1316,77 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <f t="shared" ref="A3:A6" si="0">IFERROR(IF(A2+1&lt;=Anos_a_Serem_Simulados+Ano_Inicial-1,A2+1,""),"")</f>
+        <f t="shared" ref="A3" si="0">IFERROR(IF(A2+1&lt;=Anos_a_Serem_Simulados+Ano_Inicial-1,A2+1,""),"")</f>
         <v>2018</v>
       </c>
       <c r="B3" s="2">
-        <f>ROUND(B2*1.005,0)</f>
-        <v>3015</v>
+        <v>3000</v>
       </c>
       <c r="C3" s="8">
-        <f t="shared" ref="C3:C6" si="1">B3*850</f>
-        <v>2562750</v>
+        <f t="shared" ref="C3" si="1">B3*850</f>
+        <v>2550000</v>
       </c>
       <c r="D3" s="4">
         <f>ROUND(D2*1.08,2)</f>
         <v>810</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E6" si="2">F3*C3</f>
-        <v>153765</v>
+        <f t="shared" ref="E3" si="2">F3*C3</f>
+        <v>153000</v>
       </c>
       <c r="F3" s="7">
-        <f t="shared" ref="F3:F6" si="3">G3*H3</f>
+        <f t="shared" ref="F3" si="3">G3*H3</f>
         <v>0.06</v>
       </c>
       <c r="G3" s="6">
         <v>0.02</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H6" si="4">CategoriaSAT</f>
+        <f t="shared" ref="H3" si="4">CategoriaSAT</f>
         <v>3</v>
       </c>
       <c r="I3" s="14">
         <v>8</v>
       </c>
       <c r="J3" s="14">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="M3">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="N3">
         <v>15000</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <f t="shared" si="0"/>
-        <v>2019</v>
-      </c>
-      <c r="B4" s="2">
-        <f t="shared" ref="B4:B6" si="5">ROUND(B3*1.005,0)</f>
-        <v>3030</v>
-      </c>
-      <c r="C4" s="8">
-        <f t="shared" si="1"/>
-        <v>2575500</v>
-      </c>
-      <c r="D4" s="4">
-        <f t="shared" ref="D4:D6" si="6">ROUND(D3*1.08,2)</f>
-        <v>874.8</v>
-      </c>
-      <c r="E4" s="5">
-        <f t="shared" si="2"/>
-        <v>154530</v>
-      </c>
-      <c r="F4" s="7">
-        <f t="shared" si="3"/>
-        <v>0.06</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="I4" s="14">
-        <v>8</v>
-      </c>
-      <c r="J4" s="14">
-        <v>20</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>1200</v>
-      </c>
-      <c r="N4">
-        <v>15000</v>
-      </c>
+      <c r="C4" s="8"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="6"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <f t="shared" si="0"/>
-        <v>2020</v>
-      </c>
-      <c r="B5" s="2">
-        <f t="shared" si="5"/>
-        <v>3045</v>
-      </c>
-      <c r="C5" s="8">
-        <f t="shared" si="1"/>
-        <v>2588250</v>
-      </c>
-      <c r="D5" s="4">
-        <f t="shared" si="6"/>
-        <v>944.78</v>
-      </c>
-      <c r="E5" s="5">
-        <f t="shared" si="2"/>
-        <v>155295</v>
-      </c>
-      <c r="F5" s="7">
-        <f t="shared" si="3"/>
-        <v>0.06</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="I5" s="14">
-        <v>8</v>
-      </c>
-      <c r="J5" s="14">
-        <v>20</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>1200</v>
-      </c>
-      <c r="N5">
-        <v>15000</v>
-      </c>
+      <c r="C5" s="8"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="6"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <f t="shared" si="0"/>
-        <v>2021</v>
-      </c>
-      <c r="B6" s="2">
-        <f t="shared" si="5"/>
-        <v>3060</v>
-      </c>
-      <c r="C6" s="8">
-        <f t="shared" si="1"/>
-        <v>2601000</v>
-      </c>
-      <c r="D6" s="4">
-        <f t="shared" si="6"/>
-        <v>1020.36</v>
-      </c>
-      <c r="E6" s="5">
-        <f t="shared" si="2"/>
-        <v>156060</v>
-      </c>
-      <c r="F6" s="7">
-        <f t="shared" si="3"/>
-        <v>0.06</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="I6" s="14">
-        <v>8</v>
-      </c>
-      <c r="J6" s="14">
-        <v>20</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>1200</v>
-      </c>
-      <c r="N6">
-        <v>15000</v>
-      </c>
+      <c r="C6" s="8"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="6"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C7" s="8"/>
@@ -1971,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2016,10 +1662,11 @@
         <v>71</v>
       </c>
       <c r="C2">
-        <v>3.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D2">
-        <v>9.9999999999999995E-7</v>
+        <f>C2*0.01</f>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -2038,7 +1685,8 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D3">
-        <v>9.9999999999999995E-7</v>
+        <f t="shared" ref="D3:D33" si="0">C3*0.01</f>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="G3" t="s">
         <v>43</v>
@@ -2052,10 +1700,11 @@
         <v>71</v>
       </c>
       <c r="C4">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D4">
-        <v>9.9999999999999995E-7</v>
+        <f t="shared" si="0"/>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="G4" t="s">
         <v>43</v>
@@ -2069,10 +1718,11 @@
         <v>71</v>
       </c>
       <c r="C5">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D5">
-        <v>9.9999999999999995E-7</v>
+        <f t="shared" si="0"/>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="G5" t="s">
         <v>43</v>
@@ -2086,10 +1736,11 @@
         <v>71</v>
       </c>
       <c r="C6">
-        <v>1E-3</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>9.9999999999999995E-7</v>
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
       <c r="G6" t="s">
         <v>43</v>
@@ -2106,7 +1757,8 @@
         <v>0.4</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="G7" t="s">
         <v>43</v>
@@ -2123,7 +1775,8 @@
         <v>0.3</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="G8" t="s">
         <v>43</v>
@@ -2140,7 +1793,8 @@
         <v>0.2</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2E-3</v>
       </c>
       <c r="G9" t="s">
         <v>43</v>
@@ -2157,7 +1811,8 @@
         <v>0.1</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1E-3</v>
       </c>
       <c r="G10" t="s">
         <v>43</v>
@@ -2171,10 +1826,12 @@
         <v>71</v>
       </c>
       <c r="C11">
+        <f>C2-0.002</f>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D11">
-        <v>9.9999999999999995E-7</v>
+        <f t="shared" si="0"/>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
@@ -2190,10 +1847,12 @@
         <v>71</v>
       </c>
       <c r="C12">
-        <v>5.0000000000000001E-3</v>
+        <f t="shared" ref="C12:C14" si="1">C3-0.002</f>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D12">
-        <v>9.9999999999999995E-7</v>
+        <f t="shared" si="0"/>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="G12" t="s">
         <v>17</v>
@@ -2207,10 +1866,12 @@
         <v>71</v>
       </c>
       <c r="C13">
-        <v>2E-3</v>
+        <f t="shared" si="1"/>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D13">
-        <v>9.9999999999999995E-7</v>
+        <f t="shared" si="0"/>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="G13" t="s">
         <v>17</v>
@@ -2224,10 +1885,12 @@
         <v>71</v>
       </c>
       <c r="C14">
-        <v>2E-3</v>
+        <f t="shared" si="1"/>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D14">
-        <v>9.9999999999999995E-7</v>
+        <f t="shared" si="0"/>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="G14" t="s">
         <v>17</v>
@@ -2241,10 +1904,12 @@
         <v>71</v>
       </c>
       <c r="C15">
-        <v>1E-3</v>
+        <f>C6-1</f>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>9.9999999999999995E-7</v>
+        <f t="shared" si="0"/>
+        <v>0.04</v>
       </c>
       <c r="G15" t="s">
         <v>17</v>
@@ -2261,7 +1926,8 @@
         <v>0.4</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="G16" t="s">
         <v>17</v>
@@ -2278,7 +1944,8 @@
         <v>0.3</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="G17" t="s">
         <v>17</v>
@@ -2295,7 +1962,8 @@
         <v>0.2</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2E-3</v>
       </c>
       <c r="G18" t="s">
         <v>17</v>
@@ -2312,7 +1980,8 @@
         <v>0.1</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1E-3</v>
       </c>
       <c r="G19" t="s">
         <v>17</v>
@@ -2326,10 +1995,11 @@
         <v>71</v>
       </c>
       <c r="C20">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="D20">
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="G20" t="s">
         <v>17</v>
@@ -2343,10 +2013,11 @@
         <v>71</v>
       </c>
       <c r="C21">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="D21">
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="G21" t="s">
         <v>43</v>
@@ -2363,7 +2034,8 @@
         <v>5</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
       <c r="G22" t="s">
         <v>43</v>
@@ -2380,7 +2052,8 @@
         <v>5</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
       <c r="G23" t="s">
         <v>17</v>
@@ -2397,7 +2070,8 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.02</v>
       </c>
       <c r="G24" t="s">
         <v>43</v>
@@ -2414,6 +2088,7 @@
         <v>0</v>
       </c>
       <c r="D25">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G25" t="s">
@@ -2431,7 +2106,8 @@
         <v>2</v>
       </c>
       <c r="D26">
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.02</v>
       </c>
       <c r="G26" t="s">
         <v>17</v>
@@ -2448,7 +2124,8 @@
         <v>1</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.01</v>
       </c>
       <c r="G27" t="s">
         <v>17</v>
@@ -2465,7 +2142,8 @@
         <v>0.5</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G28" t="s">
         <v>43</v>
@@ -2482,7 +2160,8 @@
         <v>0.5</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G29" t="s">
         <v>17</v>
@@ -2499,7 +2178,8 @@
         <v>10</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.1</v>
       </c>
       <c r="G30" t="s">
         <v>43</v>
@@ -2516,7 +2196,8 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.1</v>
       </c>
       <c r="G31" t="s">
         <v>17</v>
@@ -2530,9 +2211,10 @@
         <v>71</v>
       </c>
       <c r="C32">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="D32">
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
       <c r="G32" t="s">
@@ -2547,9 +2229,10 @@
         <v>71</v>
       </c>
       <c r="C33">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="D33">
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
       <c r="G33" t="s">
@@ -3091,8 +2774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implementação da Função calcular_beneficios_inss
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="150">
   <si>
     <t>Ano</t>
   </si>
@@ -466,12 +466,33 @@
   </si>
   <si>
     <t>PInvalidez</t>
+  </si>
+  <si>
+    <t>calcular_beneficios_inss</t>
+  </si>
+  <si>
+    <t>NB_91</t>
+  </si>
+  <si>
+    <t>NB_92</t>
+  </si>
+  <si>
+    <t>NB_93</t>
+  </si>
+  <si>
+    <t>NB_94</t>
+  </si>
+  <si>
+    <t>NB_31</t>
+  </si>
+  <si>
+    <t>NB_32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -870,7 +891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -964,14 +985,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F5"/>
+  <autoFilter ref="A1:F5" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
@@ -1055,13 +1076,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D5"/>
+  <autoFilter ref="A1:D5" xr:uid="{00000000-0009-0000-0000-000009000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1073,7 +1094,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1196,7 +1217,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1425,7 +1446,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1614,11 +1635,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2240,18 +2261,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G10"/>
+  <autoFilter ref="A1:G10" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2764,6 +2785,134 @@
         <v>136</v>
       </c>
     </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>143</v>
+      </c>
+      <c r="B46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>143</v>
+      </c>
+      <c r="B47" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>143</v>
+      </c>
+      <c r="B48" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>143</v>
+      </c>
+      <c r="B50" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>143</v>
+      </c>
+      <c r="B51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>143</v>
+      </c>
+      <c r="B52" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>143</v>
+      </c>
+      <c r="B53" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>143</v>
+      </c>
+      <c r="B54" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>143</v>
+      </c>
+      <c r="B55" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>143</v>
+      </c>
+      <c r="B57" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>143</v>
+      </c>
+      <c r="B58" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>143</v>
+      </c>
+      <c r="B59" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>143</v>
+      </c>
+      <c r="B60" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2771,11 +2920,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3016,13 +3165,61 @@
         <v>135</v>
       </c>
     </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>143</v>
+      </c>
+      <c r="B29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>143</v>
+      </c>
+      <c r="B31" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>143</v>
+      </c>
+      <c r="B33" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" t="s">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3096,7 +3293,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Tentativa para o calculo acumulado
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="156">
   <si>
     <t>Ano</t>
   </si>
@@ -487,6 +487,24 @@
   </si>
   <si>
     <t>NB_32</t>
+  </si>
+  <si>
+    <t>NB_91_Inicial</t>
+  </si>
+  <si>
+    <t>NB_92_Inicial</t>
+  </si>
+  <si>
+    <t>NB_93_Inicial</t>
+  </si>
+  <si>
+    <t>NB_94_Inicial</t>
+  </si>
+  <si>
+    <t>NB_31_Inicial</t>
+  </si>
+  <si>
+    <t>NB_32_Inicial</t>
   </si>
 </sst>
 </file>
@@ -1218,10 +1236,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,9 +1257,10 @@
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1285,8 +1304,26 @@
       <c r="N1" s="9" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <f>Ano_Inicial</f>
         <v>2017</v>
@@ -1334,8 +1371,26 @@
       <c r="N2">
         <v>15000</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f t="shared" ref="A3" si="0">IFERROR(IF(A2+1&lt;=Anos_a_Serem_Simulados+Ano_Inicial-1,A2+1,""),"")</f>
         <v>2018</v>
@@ -1384,8 +1439,32 @@
       <c r="N3">
         <v>15000</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <f>O2</f>
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:T3" si="5">P2</f>
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C4" s="8"/>
       <c r="E4" s="5"/>
       <c r="F4" s="7"/>
@@ -1393,7 +1472,7 @@
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C5" s="8"/>
       <c r="E5" s="5"/>
       <c r="F5" s="7"/>
@@ -1401,7 +1480,7 @@
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C6" s="8"/>
       <c r="E6" s="5"/>
       <c r="F6" s="7"/>
@@ -1409,31 +1488,31 @@
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C7" s="8"/>
       <c r="E7" s="5"/>
       <c r="F7" s="7"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C8" s="8"/>
       <c r="E8" s="5"/>
       <c r="F8" s="7"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C9" s="8"/>
       <c r="E9" s="5"/>
       <c r="F9" s="7"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C10" s="8"/>
       <c r="E10" s="5"/>
       <c r="F10" s="7"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C11" s="8"/>
       <c r="E11" s="5"/>
       <c r="F11" s="7"/>
@@ -1638,7 +1717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -2269,10 +2348,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2913,6 +2992,54 @@
         <v>112</v>
       </c>
     </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>143</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>143</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>143</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>143</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>143</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>143</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2923,8 +3050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Índice de Frequência Ampliado
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="181">
   <si>
     <t>Ano</t>
   </si>
@@ -571,6 +571,15 @@
   </si>
   <si>
     <t>DespesasMPInsumos</t>
+  </si>
+  <si>
+    <t>calcular_indices_ampliados</t>
+  </si>
+  <si>
+    <t>EventosIndiceFrequenciaAmpliado</t>
+  </si>
+  <si>
+    <t>IndiceFrequenciaAmpliado</t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1314,7 @@
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,9 +1792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A41" sqref="A40:A41"/>
-    </sheetView>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2558,10 +2565,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3490,6 +3497,142 @@
         <v>108</v>
       </c>
     </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>178</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>178</v>
+      </c>
+      <c r="B98" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>178</v>
+      </c>
+      <c r="B99" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>178</v>
+      </c>
+      <c r="B100" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>178</v>
+      </c>
+      <c r="B101" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>178</v>
+      </c>
+      <c r="B102" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>178</v>
+      </c>
+      <c r="B103" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>178</v>
+      </c>
+      <c r="B104" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>178</v>
+      </c>
+      <c r="B105" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>178</v>
+      </c>
+      <c r="B106" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>178</v>
+      </c>
+      <c r="B107" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>178</v>
+      </c>
+      <c r="B108" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>178</v>
+      </c>
+      <c r="B109" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>178</v>
+      </c>
+      <c r="B110" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>178</v>
+      </c>
+      <c r="B111" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>178</v>
+      </c>
+      <c r="B112" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>178</v>
+      </c>
+      <c r="B113" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3498,10 +3641,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3900,6 +4043,22 @@
       </c>
       <c r="B48" t="s">
         <v>177</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>178</v>
+      </c>
+      <c r="B49" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>178</v>
+      </c>
+      <c r="B50" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifucações (apenas salvando caso algo dê errado)
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="209">
   <si>
     <t>Ano</t>
   </si>
@@ -643,6 +643,27 @@
   </si>
   <si>
     <t>DespesasReclamatorias</t>
+  </si>
+  <si>
+    <t>calcular_reajustes_plano</t>
+  </si>
+  <si>
+    <t>DespesasPlanoInicial</t>
+  </si>
+  <si>
+    <t>Beta0ReajustePlano</t>
+  </si>
+  <si>
+    <t>BetaFreqReajustePlano</t>
+  </si>
+  <si>
+    <t>BetaGravReajustePlano</t>
+  </si>
+  <si>
+    <t>ReajustePlanoEstimado</t>
+  </si>
+  <si>
+    <t>DespesasPlanodeSaude</t>
   </si>
 </sst>
 </file>
@@ -1382,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AA11"/>
+  <dimension ref="A1:AE11"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,9 +1430,12 @@
     <col min="24" max="24" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="20.85546875" customWidth="1"/>
+    <col min="28" max="28" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1494,8 +1518,20 @@
       <c r="AA1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB1" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <f>Ano_Inicial</f>
         <v>2017</v>
@@ -1582,8 +1618,20 @@
       <c r="AA2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB2">
+        <v>10000</v>
+      </c>
+      <c r="AC2">
+        <v>1E-4</v>
+      </c>
+      <c r="AD2">
+        <v>1E-4</v>
+      </c>
+      <c r="AE2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f t="shared" ref="A3" si="0">IFERROR(IF(A2+1&lt;=Anos_a_Serem_Simulados+Ano_Inicial-1,A2+1,""),"")</f>
         <v>2018</v>
@@ -1677,8 +1725,20 @@
       <c r="AA3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB3">
+        <v>10000</v>
+      </c>
+      <c r="AC3">
+        <v>1E-4</v>
+      </c>
+      <c r="AD3">
+        <v>1E-4</v>
+      </c>
+      <c r="AE3">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C4" s="8"/>
       <c r="E4" s="5"/>
       <c r="F4" s="7"/>
@@ -1686,7 +1746,7 @@
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C5" s="8"/>
       <c r="E5" s="5"/>
       <c r="F5" s="7"/>
@@ -1694,7 +1754,7 @@
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C6" s="8"/>
       <c r="E6" s="5"/>
       <c r="F6" s="7"/>
@@ -1702,31 +1762,31 @@
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C7" s="8"/>
       <c r="E7" s="5"/>
       <c r="F7" s="7"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C8" s="8"/>
       <c r="E8" s="5"/>
       <c r="F8" s="7"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C9" s="8"/>
       <c r="E9" s="5"/>
       <c r="F9" s="7"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C10" s="8"/>
       <c r="E10" s="5"/>
       <c r="F10" s="7"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C11" s="8"/>
       <c r="E11" s="5"/>
       <c r="F11" s="7"/>
@@ -2778,10 +2838,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D138"/>
+  <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="A138" sqref="A138"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4046,6 +4106,54 @@
         <v>199</v>
       </c>
     </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>202</v>
+      </c>
+      <c r="B139" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>202</v>
+      </c>
+      <c r="B140" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>202</v>
+      </c>
+      <c r="B141" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>202</v>
+      </c>
+      <c r="B142" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>202</v>
+      </c>
+      <c r="B143" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>202</v>
+      </c>
+      <c r="B144" t="s">
+        <v>181</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4054,10 +4162,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4544,6 +4652,22 @@
       </c>
       <c r="B59" t="s">
         <v>201</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>202</v>
+      </c>
+      <c r="B60" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>202</v>
+      </c>
+      <c r="B61" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integrando FAP ao Cálculo
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -1590,7 +1590,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
@@ -2335,7 +2335,7 @@
         <v>CustoMedio_NB_91</v>
       </c>
       <c r="J1" t="str">
-        <f t="shared" ref="J1:M1" si="0">"CustoMedio_"&amp;C1</f>
+        <f t="shared" ref="J1:L1" si="0">"CustoMedio_"&amp;C1</f>
         <v>CustoMedio_NB_92</v>
       </c>
       <c r="K1" t="str">

</xml_diff>

<commit_message>
Dados Obrigatórios e Não Obrigatórios
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4335,9 +4335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4838,7 +4836,7 @@
       </c>
       <c r="D31" t="b">
         <f>VLOOKUP(A31,Módulos!A:B,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -4854,7 +4852,7 @@
       </c>
       <c r="D32" t="b">
         <f>VLOOKUP(A32,Módulos!A:B,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -4870,7 +4868,7 @@
       </c>
       <c r="D33" t="b">
         <f>VLOOKUP(A33,Módulos!A:B,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -4886,7 +4884,7 @@
       </c>
       <c r="D34" t="b">
         <f>VLOOKUP(A34,Módulos!A:B,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -4902,7 +4900,7 @@
       </c>
       <c r="D35" t="b">
         <f>VLOOKUP(A35,Módulos!A:B,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -4918,7 +4916,7 @@
       </c>
       <c r="D36" t="b">
         <f>VLOOKUP(A36,Módulos!A:B,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -4934,7 +4932,7 @@
       </c>
       <c r="D37" t="b">
         <f>VLOOKUP(A37,Módulos!A:B,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -4950,7 +4948,7 @@
       </c>
       <c r="D38" t="b">
         <f>VLOOKUP(A38,Módulos!A:B,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -4966,7 +4964,7 @@
       </c>
       <c r="D39" t="b">
         <f>VLOOKUP(A39,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4982,7 +4980,7 @@
       </c>
       <c r="D40" t="b">
         <f>VLOOKUP(A40,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -4998,7 +4996,7 @@
       </c>
       <c r="D41" t="b">
         <f>VLOOKUP(A41,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -5014,7 +5012,7 @@
       </c>
       <c r="D42" t="b">
         <f>VLOOKUP(A42,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -5030,7 +5028,7 @@
       </c>
       <c r="D43" t="b">
         <f>VLOOKUP(A43,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -5046,7 +5044,7 @@
       </c>
       <c r="D44" t="b">
         <f>VLOOKUP(A44,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -5062,7 +5060,7 @@
       </c>
       <c r="D45" t="b">
         <f>VLOOKUP(A45,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -5078,7 +5076,7 @@
       </c>
       <c r="D46" t="b">
         <f>VLOOKUP(A46,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -5094,7 +5092,7 @@
       </c>
       <c r="D47" t="b">
         <f>VLOOKUP(A47,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -5110,7 +5108,7 @@
       </c>
       <c r="D48" t="b">
         <f>VLOOKUP(A48,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -5126,7 +5124,7 @@
       </c>
       <c r="D49" t="b">
         <f>VLOOKUP(A49,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -5142,7 +5140,7 @@
       </c>
       <c r="D50" t="b">
         <f>VLOOKUP(A50,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -5158,7 +5156,7 @@
       </c>
       <c r="D51" t="b">
         <f>VLOOKUP(A51,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -5174,7 +5172,7 @@
       </c>
       <c r="D52" t="b">
         <f>VLOOKUP(A52,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -5190,7 +5188,7 @@
       </c>
       <c r="D53" t="b">
         <f>VLOOKUP(A53,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -5206,7 +5204,7 @@
       </c>
       <c r="D54" t="b">
         <f>VLOOKUP(A54,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -5222,7 +5220,7 @@
       </c>
       <c r="D55" t="b">
         <f>VLOOKUP(A55,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -5238,7 +5236,7 @@
       </c>
       <c r="D56" t="b">
         <f>VLOOKUP(A56,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -5254,7 +5252,7 @@
       </c>
       <c r="D57" t="b">
         <f>VLOOKUP(A57,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -5270,7 +5268,7 @@
       </c>
       <c r="D58" t="b">
         <f>VLOOKUP(A58,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -5286,7 +5284,7 @@
       </c>
       <c r="D59" t="b">
         <f>VLOOKUP(A59,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -5302,7 +5300,7 @@
       </c>
       <c r="D60" t="b">
         <f>VLOOKUP(A60,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -5318,7 +5316,7 @@
       </c>
       <c r="D61" t="b">
         <f>VLOOKUP(A61,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -7668,11 +7666,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A637D1-2310-439A-BD02-4B96D1435E85}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7725,8 +7725,8 @@
         <v>129</v>
       </c>
       <c r="B6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -7734,8 +7734,8 @@
         <v>134</v>
       </c>
       <c r="B7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Batentes na regressão do FAP, arquivo de dados ajustado.
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="304">
   <si>
     <t>Ano</t>
   </si>
@@ -2735,9 +2735,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F112" sqref="F112"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4480,7 +4482,7 @@
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="D96">
-        <f t="shared" ref="D96:D107" si="17">C96*0.01</f>
+        <f t="shared" ref="D96:D108" si="17">C96*0.01</f>
         <v>2.5000000000000002E-6</v>
       </c>
       <c r="G96" t="s">
@@ -4694,6 +4696,78 @@
       </c>
       <c r="G107" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>266</v>
+      </c>
+      <c r="B108" t="s">
+        <v>65</v>
+      </c>
+      <c r="C108">
+        <v>1000</v>
+      </c>
+      <c r="D108">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="G108" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>197</v>
+      </c>
+      <c r="B109" t="s">
+        <v>65</v>
+      </c>
+      <c r="C109">
+        <v>1000</v>
+      </c>
+      <c r="D109">
+        <f t="shared" ref="D109:D110" si="18">C109*0.01</f>
+        <v>10</v>
+      </c>
+      <c r="G109" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>266</v>
+      </c>
+      <c r="B110" t="s">
+        <v>65</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G110" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>197</v>
+      </c>
+      <c r="B111" t="s">
+        <v>65</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <f t="shared" ref="D111" si="19">C111*0.01</f>
+        <v>0</v>
+      </c>
+      <c r="G111" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -4707,7 +4781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A637D1-2310-439A-BD02-4B96D1435E85}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Poisson com numero de funcionários fixo (apenas para teste)
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -3773,7 +3773,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6260,7 +6262,7 @@
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Correção do Erro no calculo da Despesa FAP
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -2502,7 +2502,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2568,6 +2568,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2794,10 +2795,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>3</v>
+        <v>0.03</v>
       </c>
       <c r="D2" s="1">
         <v>2017</v>
@@ -2835,8 +2836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BB11"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3052,7 +3053,7 @@
       </c>
       <c r="D2">
         <f>CategoriaSAT</f>
-        <v>3</v>
+        <v>0.03</v>
       </c>
       <c r="E2" s="11">
         <v>8</v>
@@ -3219,7 +3220,7 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3" si="2">CategoriaSAT</f>
-        <v>3</v>
+        <v>0.03</v>
       </c>
       <c r="E3" s="11">
         <v>8</v>
@@ -3582,7 +3583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -3773,8 +3774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Tirar do modelo exigência do Funcionário Desligados Iniciais
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Custos!$A$1:$D$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Funcoes_Inputs!$A$1:$E$223</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Funcoes_Inputs!$A$1:$E$222</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lista_de_Parâmetros!$A$1:$F$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Módulos!$A$1:$B$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Parametros!$A$1:$G$54</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="303">
   <si>
     <t>Ano</t>
   </si>
@@ -569,16 +569,10 @@
     <t>DesligamentosInvoluntarios</t>
   </si>
   <si>
-    <t>FuncDesligadosInicial</t>
-  </si>
-  <si>
     <t>TurnoverGeral</t>
   </si>
   <si>
     <t>FuncionariosDesligados</t>
-  </si>
-  <si>
-    <t>FuncionariosDesligadosAcumulado</t>
   </si>
   <si>
     <t>calcular_reclamatorias</t>
@@ -1467,9 +1461,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1488,7 +1484,7 @@
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1511,7 +1507,7 @@
         <v>85</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D66" si="0">A3</f>
+        <f t="shared" ref="D3:D65" si="0">A3</f>
         <v>calcular_eventos</v>
       </c>
     </row>
@@ -1800,7 +1796,7 @@
         <v>120</v>
       </c>
       <c r="B27" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
@@ -1812,7 +1808,7 @@
         <v>120</v>
       </c>
       <c r="B28" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -2136,7 +2132,7 @@
         <v>173</v>
       </c>
       <c r="B55" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
@@ -2148,7 +2144,7 @@
         <v>173</v>
       </c>
       <c r="B56" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
@@ -2157,22 +2153,22 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B57" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
-        <v>calcular_turnovergeral</v>
+        <v>calcular_reclamatorias</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B58" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
@@ -2181,22 +2177,22 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B59" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D59" t="str">
         <f t="shared" si="0"/>
-        <v>calcular_reclamatorias</v>
+        <v>calcular_reajustes_plano</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B60" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" si="0"/>
@@ -2205,22 +2201,22 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B61" t="s">
         <v>190</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>calcular_reajustes_plano</v>
+        <v>calcular_reabilitacao</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>189</v>
+      </c>
+      <c r="B62" t="s">
         <v>191</v>
-      </c>
-      <c r="B62" t="s">
-        <v>192</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
@@ -2229,70 +2225,70 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B63" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>calcular_reabilitacao</v>
+        <v>calcular_produtividade</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B64" t="s">
-        <v>197</v>
+        <v>264</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>calcular_produtividade</v>
+        <v>calcular_qualidade</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B65" t="s">
-        <v>266</v>
+        <v>207</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>calcular_qualidade</v>
+        <v>calcular_imagem_contracacao</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>206</v>
+      </c>
+      <c r="B66" t="s">
         <v>208</v>
       </c>
-      <c r="B66" t="s">
-        <v>209</v>
-      </c>
       <c r="D66" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D66:D83" si="1">A66</f>
         <v>calcular_imagem_contracacao</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B67" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:D84" si="1">A67</f>
-        <v>calcular_imagem_contracacao</v>
+        <f t="shared" si="1"/>
+        <v>calcular_imagem_receita</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B68" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="1"/>
@@ -2301,22 +2297,22 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>212</v>
+        <v>254</v>
       </c>
       <c r="B69" t="s">
-        <v>217</v>
+        <v>258</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="1"/>
-        <v>calcular_imagem_receita</v>
+        <v>calcular_interrupcao_acidentes</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B70" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="1"/>
@@ -2325,34 +2321,34 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B71" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="1"/>
-        <v>calcular_interrupcao_acidentes</v>
+        <v>calcular_interdicao_fiscalizacao</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="B72" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="1"/>
-        <v>calcular_interdicao_fiscalizacao</v>
+        <v>calcular_fap</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B73" t="s">
-        <v>241</v>
+        <v>287</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="1"/>
@@ -2361,10 +2357,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>286</v>
+      </c>
+      <c r="B74" t="s">
         <v>288</v>
-      </c>
-      <c r="B74" t="s">
-        <v>289</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="1"/>
@@ -2373,10 +2369,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B75" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="1"/>
@@ -2385,10 +2381,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B76" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="1"/>
@@ -2397,10 +2393,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B77" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="1"/>
@@ -2409,10 +2405,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B78" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="1"/>
@@ -2421,10 +2417,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="1"/>
@@ -2433,10 +2429,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B80" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="1"/>
@@ -2445,10 +2441,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B81" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="1"/>
@@ -2457,10 +2453,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B82" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="1"/>
@@ -2469,24 +2465,12 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B83" t="s">
-        <v>298</v>
+        <v>24</v>
       </c>
       <c r="D83" t="str">
-        <f t="shared" si="1"/>
-        <v>calcular_fap</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>288</v>
-      </c>
-      <c r="B84" t="s">
-        <v>24</v>
-      </c>
-      <c r="D84" t="str">
         <f t="shared" si="1"/>
         <v>calcular_fap</v>
       </c>
@@ -2667,7 +2651,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
@@ -2681,7 +2665,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B5" t="s">
         <v>59</v>
@@ -2715,7 +2699,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2795,7 +2781,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C2" s="2">
         <v>0.03</v>
@@ -2834,11 +2820,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BB11"/>
+  <dimension ref="A1:BA11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2854,28 +2838,27 @@
     <col min="16" max="17" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.85546875" customWidth="1"/>
-    <col min="22" max="22" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="25" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18.28515625" customWidth="1"/>
-    <col min="34" max="34" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="44" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="45" max="48" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="25" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.28515625" customWidth="1"/>
+    <col min="33" max="33" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="43" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="47" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2886,7 +2869,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>15</v>
@@ -2937,109 +2920,106 @@
         <v>174</v>
       </c>
       <c r="U1" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="V1" t="s">
+        <v>184</v>
+      </c>
+      <c r="W1" t="s">
         <v>185</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>186</v>
       </c>
-      <c r="X1" t="s">
-        <v>187</v>
-      </c>
       <c r="Y1" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="Z1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AA1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB1" t="s">
         <v>202</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>203</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>204</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>205</v>
       </c>
-      <c r="AE1" t="s">
-        <v>206</v>
-      </c>
       <c r="AF1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="AG1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AH1" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="AI1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>231</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>232</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>233</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>234</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>235</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>236</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>237</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>238</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>239</v>
       </c>
       <c r="AR1" t="s">
         <v>240</v>
       </c>
       <c r="AS1" t="s">
+        <v>241</v>
+      </c>
+      <c r="AT1" t="s">
         <v>242</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>243</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>244</v>
       </c>
       <c r="AV1" t="s">
         <v>245</v>
       </c>
       <c r="AW1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AX1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="AY1" t="s">
         <v>246</v>
       </c>
       <c r="AZ1" t="s">
+        <v>247</v>
+      </c>
+      <c r="BA1" t="s">
         <v>248</v>
       </c>
-      <c r="BA1" t="s">
-        <v>249</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <f>Ano_Inicial</f>
         <v>2017</v>
@@ -3104,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="U2">
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="V2">
-        <v>10000</v>
+        <v>1E-4</v>
       </c>
       <c r="W2">
         <v>1E-4</v>
@@ -3116,13 +3096,13 @@
         <v>1E-4</v>
       </c>
       <c r="Y2">
-        <v>1E-4</v>
+        <v>10000</v>
       </c>
       <c r="Z2">
-        <v>10000</v>
+        <v>3</v>
       </c>
       <c r="AA2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB2">
         <v>1</v>
@@ -3137,13 +3117,13 @@
         <v>1</v>
       </c>
       <c r="AF2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AG2">
         <v>10</v>
       </c>
       <c r="AH2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AI2">
         <v>1</v>
@@ -3173,7 +3153,7 @@
         <v>1</v>
       </c>
       <c r="AR2">
-        <v>1</v>
+        <v>50000</v>
       </c>
       <c r="AS2">
         <v>50000</v>
@@ -3185,7 +3165,7 @@
         <v>50000</v>
       </c>
       <c r="AV2">
-        <v>50000</v>
+        <v>1</v>
       </c>
       <c r="AW2">
         <v>1</v>
@@ -3202,11 +3182,8 @@
       <c r="BA2">
         <v>1</v>
       </c>
-      <c r="BB2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f t="shared" ref="A3" si="0">IFERROR(IF(A2+1&lt;=Anos_a_Serem_Simulados+Ano_Inicial-1,A2+1,""),"")</f>
         <v>2018</v>
@@ -3277,10 +3254,10 @@
         <v>10</v>
       </c>
       <c r="U3">
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="V3">
-        <v>10000</v>
+        <v>1E-4</v>
       </c>
       <c r="W3">
         <v>1E-4</v>
@@ -3289,13 +3266,13 @@
         <v>1E-4</v>
       </c>
       <c r="Y3">
-        <v>1E-4</v>
+        <v>10040</v>
       </c>
       <c r="Z3">
-        <v>10040</v>
+        <v>3</v>
       </c>
       <c r="AA3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB3">
         <v>1</v>
@@ -3310,13 +3287,13 @@
         <v>1</v>
       </c>
       <c r="AF3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AG3">
         <v>10</v>
       </c>
       <c r="AH3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AI3">
         <v>1</v>
@@ -3346,7 +3323,7 @@
         <v>1</v>
       </c>
       <c r="AR3">
-        <v>1</v>
+        <v>50000</v>
       </c>
       <c r="AS3">
         <v>50000</v>
@@ -3358,7 +3335,7 @@
         <v>50000</v>
       </c>
       <c r="AV3">
-        <v>50000</v>
+        <v>1</v>
       </c>
       <c r="AW3">
         <v>1</v>
@@ -3375,38 +3352,35 @@
       <c r="BA3">
         <v>1</v>
       </c>
-      <c r="BB3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="C4" s="6"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="C5" s="6"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="C6" s="6"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="C11" s="6"/>
     </row>
   </sheetData>
@@ -3456,7 +3430,7 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I1" t="str">
         <f>"CustoMedio_"&amp;B1</f>
@@ -3475,10 +3449,10 @@
         <v>CustoMedio_NB_94</v>
       </c>
       <c r="M1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="N1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -3583,7 +3557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -3607,7 +3581,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B2" t="b">
         <f>TRUE</f>
@@ -3812,7 +3786,7 @@
         <v>62</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3830,7 +3804,7 @@
         <v>0.05</v>
       </c>
       <c r="G2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H2" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A2)&gt;0,FALSE,TRUE)</f>
@@ -3852,7 +3826,7 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H3" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A3)&gt;0,FALSE,TRUE)</f>
@@ -3874,7 +3848,7 @@
         <v>0.05</v>
       </c>
       <c r="G4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H4" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A4)&gt;0,FALSE,TRUE)</f>
@@ -3896,7 +3870,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H5" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A5)&gt;0,FALSE,TRUE)</f>
@@ -3918,7 +3892,7 @@
         <v>1E-3</v>
       </c>
       <c r="G6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H6" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A6)&gt;0,FALSE,TRUE)</f>
@@ -3940,7 +3914,7 @@
         <v>1E-4</v>
       </c>
       <c r="G7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H7" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A7)&gt;0,FALSE,TRUE)</f>
@@ -3962,7 +3936,7 @@
         <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H8" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A8)&gt;0,FALSE,TRUE)</f>
@@ -3984,7 +3958,7 @@
         <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H9" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A9)&gt;0,FALSE,TRUE)</f>
@@ -4006,7 +3980,7 @@
         <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H10" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A10)&gt;0,FALSE,TRUE)</f>
@@ -4015,7 +3989,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B11" t="s">
         <v>65</v>
@@ -4028,7 +4002,7 @@
         <v>1E-3</v>
       </c>
       <c r="G11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H11" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A11)&gt;0,FALSE,TRUE)</f>
@@ -4037,7 +4011,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B12" t="s">
         <v>65</v>
@@ -4050,7 +4024,7 @@
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H12" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A12)&gt;0,FALSE,TRUE)</f>
@@ -4059,7 +4033,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B13" t="s">
         <v>65</v>
@@ -4072,7 +4046,7 @@
         <v>1E-3</v>
       </c>
       <c r="G13" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H13" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A13)&gt;0,FALSE,TRUE)</f>
@@ -4081,7 +4055,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B14" t="s">
         <v>65</v>
@@ -4094,7 +4068,7 @@
         <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H14" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A14)&gt;0,FALSE,TRUE)</f>
@@ -4103,7 +4077,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B15" t="s">
         <v>65</v>
@@ -4116,7 +4090,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H15" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A15)&gt;0,FALSE,TRUE)</f>
@@ -4125,7 +4099,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B16" t="s">
         <v>65</v>
@@ -4138,7 +4112,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H16" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A16)&gt;0,FALSE,TRUE)</f>
@@ -4147,7 +4121,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B17" t="s">
         <v>65</v>
@@ -4160,7 +4134,7 @@
         <v>0.1</v>
       </c>
       <c r="G17" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H17" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A17)&gt;0,FALSE,TRUE)</f>
@@ -4169,7 +4143,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B18" t="s">
         <v>65</v>
@@ -4182,7 +4156,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H18" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A18)&gt;0,FALSE,TRUE)</f>
@@ -4204,7 +4178,7 @@
         <v>0.02</v>
       </c>
       <c r="G19" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A19)&gt;0,FALSE,TRUE)</f>
@@ -4213,7 +4187,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B20" t="s">
         <v>65</v>
@@ -4226,7 +4200,7 @@
         <v>0.02</v>
       </c>
       <c r="G20" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H20" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A20)&gt;0,FALSE,TRUE)</f>
@@ -4235,7 +4209,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B21" t="s">
         <v>65</v>
@@ -4248,7 +4222,7 @@
         <v>0.02</v>
       </c>
       <c r="G21" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H21" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A21)&gt;0,FALSE,TRUE)</f>
@@ -4257,7 +4231,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B22" t="s">
         <v>65</v>
@@ -4270,7 +4244,7 @@
         <v>0.02</v>
       </c>
       <c r="G22" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H22" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A22)&gt;0,FALSE,TRUE)</f>
@@ -4279,7 +4253,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B23" t="s">
         <v>65</v>
@@ -4292,7 +4266,7 @@
         <v>0.02</v>
       </c>
       <c r="G23" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H23" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A23)&gt;0,FALSE,TRUE)</f>
@@ -4301,7 +4275,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B24" t="s">
         <v>65</v>
@@ -4314,7 +4288,7 @@
         <v>5</v>
       </c>
       <c r="G24" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H24" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A24)&gt;0,FALSE,TRUE)</f>
@@ -4323,7 +4297,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B25" t="s">
         <v>65</v>
@@ -4336,7 +4310,7 @@
         <v>5</v>
       </c>
       <c r="G25" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H25" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A25)&gt;0,FALSE,TRUE)</f>
@@ -4345,7 +4319,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B26" t="s">
         <v>65</v>
@@ -4358,7 +4332,7 @@
         <v>5</v>
       </c>
       <c r="G26" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H26" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A26)&gt;0,FALSE,TRUE)</f>
@@ -4367,7 +4341,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B27" t="s">
         <v>65</v>
@@ -4380,7 +4354,7 @@
         <v>5</v>
       </c>
       <c r="G27" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H27" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A27)&gt;0,FALSE,TRUE)</f>
@@ -4389,7 +4363,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B28" t="s">
         <v>65</v>
@@ -4402,7 +4376,7 @@
         <v>5</v>
       </c>
       <c r="G28" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H28" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A28)&gt;0,FALSE,TRUE)</f>
@@ -4424,7 +4398,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H29" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A29)&gt;0,FALSE,TRUE)</f>
@@ -4433,7 +4407,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B30" t="s">
         <v>65</v>
@@ -4446,7 +4420,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H30" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A30)&gt;0,FALSE,TRUE)</f>
@@ -4455,7 +4429,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B31" t="s">
         <v>65</v>
@@ -4468,7 +4442,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H31" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A31)&gt;0,FALSE,TRUE)</f>
@@ -4477,7 +4451,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B32" t="s">
         <v>65</v>
@@ -4490,7 +4464,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H32" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A32)&gt;0,FALSE,TRUE)</f>
@@ -4499,7 +4473,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B33" t="s">
         <v>65</v>
@@ -4512,7 +4486,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H33" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A33)&gt;0,FALSE,TRUE)</f>
@@ -4521,7 +4495,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B34" t="s">
         <v>65</v>
@@ -4534,7 +4508,7 @@
         <v>0.1</v>
       </c>
       <c r="G34" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H34" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A34)&gt;0,FALSE,TRUE)</f>
@@ -4543,7 +4517,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B35" t="s">
         <v>65</v>
@@ -4556,7 +4530,7 @@
         <v>0.01</v>
       </c>
       <c r="G35" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H35" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A35)&gt;0,FALSE,TRUE)</f>
@@ -4565,7 +4539,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B36" t="s">
         <v>65</v>
@@ -4578,7 +4552,7 @@
         <v>10</v>
       </c>
       <c r="G36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H36" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A36)&gt;0,FALSE,TRUE)</f>
@@ -4587,7 +4561,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B37" t="s">
         <v>65</v>
@@ -4600,7 +4574,7 @@
         <v>0.02</v>
       </c>
       <c r="G37" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H37" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A37)&gt;0,FALSE,TRUE)</f>
@@ -4609,7 +4583,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B38" t="s">
         <v>65</v>
@@ -4622,7 +4596,7 @@
         <v>0.1</v>
       </c>
       <c r="G38" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H38" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A38)&gt;0,FALSE,TRUE)</f>
@@ -4631,7 +4605,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B39" t="s">
         <v>65</v>
@@ -4644,7 +4618,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G39" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H39" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A39)&gt;0,FALSE,TRUE)</f>
@@ -4653,7 +4627,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B40" t="s">
         <v>65</v>
@@ -4666,7 +4640,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G40" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H40" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A40)&gt;0,FALSE,TRUE)</f>
@@ -4675,7 +4649,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B41" t="s">
         <v>65</v>
@@ -4688,7 +4662,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G41" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H41" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A41)&gt;0,FALSE,TRUE)</f>
@@ -4697,7 +4671,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B42" t="s">
         <v>65</v>
@@ -4710,7 +4684,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G42" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H42" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A42)&gt;0,FALSE,TRUE)</f>
@@ -4719,7 +4693,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B43" t="s">
         <v>65</v>
@@ -4732,7 +4706,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G43" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H43" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A43)&gt;0,FALSE,TRUE)</f>
@@ -4741,7 +4715,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B44" t="s">
         <v>65</v>
@@ -4754,7 +4728,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G44" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H44" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A44)&gt;0,FALSE,TRUE)</f>
@@ -4763,7 +4737,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B45" t="s">
         <v>65</v>
@@ -4776,7 +4750,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G45" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H45" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A45)&gt;0,FALSE,TRUE)</f>
@@ -4785,7 +4759,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B46" t="s">
         <v>65</v>
@@ -4798,7 +4772,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G46" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H46" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A46)&gt;0,FALSE,TRUE)</f>
@@ -4807,7 +4781,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B47" t="s">
         <v>65</v>
@@ -4820,7 +4794,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G47" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H47" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A47)&gt;0,FALSE,TRUE)</f>
@@ -4829,7 +4803,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B48" t="s">
         <v>65</v>
@@ -4842,7 +4816,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G48" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H48" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A48)&gt;0,FALSE,TRUE)</f>
@@ -4851,7 +4825,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B49" t="s">
         <v>65</v>
@@ -4864,7 +4838,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G49" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H49" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A49)&gt;0,FALSE,TRUE)</f>
@@ -4873,7 +4847,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B50" t="s">
         <v>65</v>
@@ -4886,7 +4860,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G50" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H50" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A50)&gt;0,FALSE,TRUE)</f>
@@ -4895,7 +4869,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B51" t="s">
         <v>65</v>
@@ -4908,7 +4882,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G51" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H51" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A51)&gt;0,FALSE,TRUE)</f>
@@ -4917,7 +4891,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B52" t="s">
         <v>65</v>
@@ -4930,7 +4904,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G52" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H52" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A52)&gt;0,FALSE,TRUE)</f>
@@ -4939,7 +4913,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B53" t="s">
         <v>65</v>
@@ -4952,7 +4926,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G53" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H53" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A53)&gt;0,FALSE,TRUE)</f>
@@ -4961,7 +4935,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B54" t="s">
         <v>65</v>
@@ -4974,7 +4948,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G54" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H54" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A54)&gt;0,FALSE,TRUE)</f>
@@ -5181,7 +5155,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B64" t="s">
         <v>65</v>
@@ -5203,7 +5177,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B65" t="s">
         <v>65</v>
@@ -5225,7 +5199,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B66" t="s">
         <v>65</v>
@@ -5247,7 +5221,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B67" t="s">
         <v>65</v>
@@ -5269,7 +5243,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B68" t="s">
         <v>65</v>
@@ -5291,7 +5265,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B69" t="s">
         <v>65</v>
@@ -5313,7 +5287,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B70" t="s">
         <v>65</v>
@@ -5335,7 +5309,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B71" t="s">
         <v>65</v>
@@ -5379,7 +5353,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B73" t="s">
         <v>65</v>
@@ -5401,7 +5375,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B74" t="s">
         <v>65</v>
@@ -5423,7 +5397,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B75" t="s">
         <v>65</v>
@@ -5445,7 +5419,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B76" t="s">
         <v>65</v>
@@ -5467,7 +5441,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B77" t="s">
         <v>65</v>
@@ -5489,7 +5463,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B78" t="s">
         <v>65</v>
@@ -5511,7 +5485,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B79" t="s">
         <v>65</v>
@@ -5533,7 +5507,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B80" t="s">
         <v>65</v>
@@ -5555,7 +5529,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B81" t="s">
         <v>65</v>
@@ -5599,7 +5573,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B83" t="s">
         <v>65</v>
@@ -5621,7 +5595,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B84" t="s">
         <v>65</v>
@@ -5643,7 +5617,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B85" t="s">
         <v>65</v>
@@ -5665,7 +5639,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B86" t="s">
         <v>65</v>
@@ -5687,7 +5661,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B87" t="s">
         <v>65</v>
@@ -5709,7 +5683,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B88" t="s">
         <v>65</v>
@@ -5731,7 +5705,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B89" t="s">
         <v>65</v>
@@ -5753,7 +5727,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B90" t="s">
         <v>65</v>
@@ -5775,7 +5749,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B91" t="s">
         <v>65</v>
@@ -5797,7 +5771,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B92" t="s">
         <v>65</v>
@@ -5820,7 +5794,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B93" t="s">
         <v>65</v>
@@ -5843,7 +5817,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B94" t="s">
         <v>65</v>
@@ -5866,7 +5840,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B95" t="s">
         <v>65</v>
@@ -5889,7 +5863,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B96" t="s">
         <v>65</v>
@@ -5912,7 +5886,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B97" t="s">
         <v>65</v>
@@ -5935,7 +5909,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B98" t="s">
         <v>65</v>
@@ -5958,7 +5932,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B99" t="s">
         <v>65</v>
@@ -5981,7 +5955,7 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B100" t="s">
         <v>65</v>
@@ -6004,7 +5978,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B101" t="s">
         <v>65</v>
@@ -6027,7 +6001,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B102" t="s">
         <v>65</v>
@@ -6050,7 +6024,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B103" t="s">
         <v>65</v>
@@ -6073,7 +6047,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B104" t="s">
         <v>65</v>
@@ -6096,7 +6070,7 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B105" t="s">
         <v>65</v>
@@ -6119,7 +6093,7 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B106" t="s">
         <v>65</v>
@@ -6142,7 +6116,7 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B107" t="s">
         <v>65</v>
@@ -6165,7 +6139,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B108" t="s">
         <v>65</v>
@@ -6187,7 +6161,7 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B109" t="s">
         <v>65</v>
@@ -6209,7 +6183,7 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B110" t="s">
         <v>65</v>
@@ -6222,7 +6196,7 @@
         <v>0</v>
       </c>
       <c r="G110" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H110" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A110)&gt;0,FALSE,TRUE)</f>
@@ -6231,7 +6205,7 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B111" t="s">
         <v>65</v>
@@ -6244,7 +6218,7 @@
         <v>0</v>
       </c>
       <c r="G111" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H111" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A111)&gt;0,FALSE,TRUE)</f>
@@ -6283,87 +6257,87 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -6388,13 +6362,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6424,7 +6398,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -6436,7 +6410,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -6448,7 +6422,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -6460,7 +6434,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6481,7 +6455,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6493,7 +6467,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -6505,7 +6479,7 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -6517,7 +6491,7 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -6529,7 +6503,7 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -6543,7 +6517,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B15" t="b">
         <f>FALSE</f>
@@ -6552,7 +6526,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B16" t="b">
         <f>FALSE</f>
@@ -6561,7 +6535,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B17" t="b">
         <f>FALSE</f>
@@ -6570,7 +6544,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B18" t="b">
         <f>FALSE</f>
@@ -6579,7 +6553,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B19" t="b">
         <f>FALSE</f>
@@ -6588,7 +6562,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B20" t="b">
         <f>FALSE</f>
@@ -6597,7 +6571,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B21" t="b">
         <f>FALSE</f>
@@ -6615,7 +6589,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B23" t="b">
         <f>FALSE</f>
@@ -6624,7 +6598,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B24" t="b">
         <f>FALSE</f>
@@ -6633,7 +6607,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B25" t="b">
         <f>FALSE</f>
@@ -6648,9 +6622,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E234"/>
+  <dimension ref="A1:E233"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="B138" sqref="B138"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6672,10 +6648,10 @@
         <v>79</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6723,7 +6699,7 @@
         <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C4" t="b">
         <f>TRUE</f>
@@ -6743,7 +6719,7 @@
         <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C5" t="b">
         <f>TRUE</f>
@@ -6763,7 +6739,7 @@
         <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C6" t="b">
         <f>TRUE</f>
@@ -6783,7 +6759,7 @@
         <v>101</v>
       </c>
       <c r="B7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C7" t="b">
         <f>TRUE</f>
@@ -6803,7 +6779,7 @@
         <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C8" t="b">
         <f>TRUE</f>
@@ -6823,7 +6799,7 @@
         <v>101</v>
       </c>
       <c r="B9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C9" t="b">
         <f>TRUE</f>
@@ -6843,7 +6819,7 @@
         <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C10" t="b">
         <f>TRUE</f>
@@ -6863,7 +6839,7 @@
         <v>101</v>
       </c>
       <c r="B11" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C11" t="b">
         <f>TRUE</f>
@@ -6883,7 +6859,7 @@
         <v>101</v>
       </c>
       <c r="B12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C12" t="b">
         <f>TRUE</f>
@@ -6903,7 +6879,7 @@
         <v>101</v>
       </c>
       <c r="B13" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C13" t="b">
         <f>TRUE</f>
@@ -6923,7 +6899,7 @@
         <v>101</v>
       </c>
       <c r="B14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C14" t="b">
         <f>TRUE</f>
@@ -6943,7 +6919,7 @@
         <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C15" t="b">
         <f>TRUE</f>
@@ -6963,7 +6939,7 @@
         <v>101</v>
       </c>
       <c r="B16" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C16" t="b">
         <f>TRUE</f>
@@ -6983,7 +6959,7 @@
         <v>101</v>
       </c>
       <c r="B17" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C17" t="b">
         <f>TRUE</f>
@@ -7003,7 +6979,7 @@
         <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C18" t="b">
         <f>TRUE</f>
@@ -7023,7 +6999,7 @@
         <v>101</v>
       </c>
       <c r="B19" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C19" t="b">
         <f>TRUE</f>
@@ -7503,7 +7479,7 @@
         <v>120</v>
       </c>
       <c r="B43" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C43" t="b">
         <f>TRUE</f>
@@ -7523,7 +7499,7 @@
         <v>120</v>
       </c>
       <c r="B44" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C44" t="b">
         <f>TRUE</f>
@@ -7543,7 +7519,7 @@
         <v>120</v>
       </c>
       <c r="B45" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C45" t="b">
         <f>TRUE</f>
@@ -7563,7 +7539,7 @@
         <v>120</v>
       </c>
       <c r="B46" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C46" t="b">
         <f>TRUE</f>
@@ -9363,7 +9339,7 @@
         <v>173</v>
       </c>
       <c r="B136" t="s">
-        <v>175</v>
+        <v>1</v>
       </c>
       <c r="C136" t="b">
         <f>TRUE</f>
@@ -9380,34 +9356,34 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B137" t="s">
-        <v>1</v>
+        <v>176</v>
       </c>
       <c r="C137" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D137" t="b">
         <f>VLOOKUP(A137,Módulos!A:B,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E137" t="str">
         <f>IF(C137,"Nenhuma",VLOOKUP(B137,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_turnovergeral</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B138" t="s">
         <v>178</v>
       </c>
       <c r="C138" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D138" t="b">
         <f>VLOOKUP(A138,Módulos!A:B,2,FALSE)</f>
@@ -9415,15 +9391,15 @@
       </c>
       <c r="E138" t="str">
         <f>IF(C138,"Nenhuma",VLOOKUP(B138,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_turnovergeral</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>177</v>
+      </c>
+      <c r="B139" t="s">
         <v>179</v>
-      </c>
-      <c r="B139" t="s">
-        <v>180</v>
       </c>
       <c r="C139" t="b">
         <f>TRUE</f>
@@ -9440,10 +9416,10 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B140" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C140" t="b">
         <f>TRUE</f>
@@ -9460,10 +9436,10 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>182</v>
+      </c>
+      <c r="B141" t="s">
         <v>184</v>
-      </c>
-      <c r="B141" t="s">
-        <v>185</v>
       </c>
       <c r="C141" t="b">
         <f>TRUE</f>
@@ -9480,10 +9456,10 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B142" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C142" t="b">
         <f>TRUE</f>
@@ -9500,10 +9476,10 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B143" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C143" t="b">
         <f>TRUE</f>
@@ -9520,14 +9496,14 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B144" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="C144" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D144" t="b">
         <f>VLOOKUP(A144,Módulos!A:B,2,FALSE)</f>
@@ -9535,15 +9511,15 @@
       </c>
       <c r="E144" t="str">
         <f>IF(C144,"Nenhuma",VLOOKUP(B144,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_indices_ampliados</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B145" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C145" t="b">
         <f>FALSE</f>
@@ -9560,10 +9536,10 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B146" t="s">
-        <v>163</v>
+        <v>86</v>
       </c>
       <c r="C146" t="b">
         <f>FALSE</f>
@@ -9575,15 +9551,15 @@
       </c>
       <c r="E146" t="str">
         <f>IF(C146,"Nenhuma",VLOOKUP(B146,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_indices_ampliados</v>
+        <v>calcular_eventos</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B147" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C147" t="b">
         <f>FALSE</f>
@@ -9600,10 +9576,10 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B148" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C148" t="b">
         <f>FALSE</f>
@@ -9620,10 +9596,10 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B149" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C149" t="b">
         <f>FALSE</f>
@@ -9640,10 +9616,10 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B150" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C150" t="b">
         <f>FALSE</f>
@@ -9660,10 +9636,10 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B151" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C151" t="b">
         <f>FALSE</f>
@@ -9680,10 +9656,10 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B152" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C152" t="b">
         <f>FALSE</f>
@@ -9700,10 +9676,10 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B153" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C153" t="b">
         <f>FALSE</f>
@@ -9720,14 +9696,14 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B154" t="s">
-        <v>97</v>
+        <v>192</v>
       </c>
       <c r="C154" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D154" t="b">
         <f>VLOOKUP(A154,Módulos!A:B,2,FALSE)</f>
@@ -9735,15 +9711,15 @@
       </c>
       <c r="E154" t="str">
         <f>IF(C154,"Nenhuma",VLOOKUP(B154,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_eventos</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B155" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C155" t="b">
         <f>TRUE</f>
@@ -9760,10 +9736,10 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B156" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C156" t="b">
         <f>TRUE</f>
@@ -9780,7 +9756,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B157" t="s">
         <v>199</v>
@@ -9800,10 +9776,10 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>198</v>
+      </c>
+      <c r="B158" t="s">
         <v>200</v>
-      </c>
-      <c r="B158" t="s">
-        <v>201</v>
       </c>
       <c r="C158" t="b">
         <f>TRUE</f>
@@ -9820,10 +9796,10 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B159" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C159" t="b">
         <f>TRUE</f>
@@ -9840,10 +9816,10 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B160" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C160" t="b">
         <f>TRUE</f>
@@ -9860,10 +9836,10 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B161" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C161" t="b">
         <f>TRUE</f>
@@ -9880,10 +9856,10 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B162" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C162" t="b">
         <f>TRUE</f>
@@ -9900,10 +9876,10 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B163" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C163" t="b">
         <f>TRUE</f>
@@ -9920,10 +9896,10 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B164" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C164" t="b">
         <f>TRUE</f>
@@ -9940,10 +9916,10 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B165" t="s">
-        <v>207</v>
+        <v>168</v>
       </c>
       <c r="C165" t="b">
         <f>TRUE</f>
@@ -9960,14 +9936,14 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B166" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C166" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D166" t="b">
         <f>VLOOKUP(A166,Módulos!A:B,2,FALSE)</f>
@@ -9975,15 +9951,15 @@
       </c>
       <c r="E166" t="str">
         <f>IF(C166,"Nenhuma",VLOOKUP(B166,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_indices_ampliados</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B167" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C167" t="b">
         <f>FALSE</f>
@@ -10000,14 +9976,14 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B168" t="s">
-        <v>163</v>
+        <v>1</v>
       </c>
       <c r="C168" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D168" t="b">
         <f>VLOOKUP(A168,Módulos!A:B,2,FALSE)</f>
@@ -10015,15 +9991,15 @@
       </c>
       <c r="E168" t="str">
         <f>IF(C168,"Nenhuma",VLOOKUP(B168,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_indices_ampliados</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B169" t="s">
-        <v>1</v>
+        <v>209</v>
       </c>
       <c r="C169" t="b">
         <f>TRUE</f>
@@ -10040,14 +10016,14 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B170" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
       <c r="C170" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D170" t="b">
         <f>VLOOKUP(A170,Módulos!A:B,2,FALSE)</f>
@@ -10055,15 +10031,15 @@
       </c>
       <c r="E170" t="str">
         <f>IF(C170,"Nenhuma",VLOOKUP(B170,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_turnovergeral</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B171" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="C171" t="b">
         <f>FALSE</f>
@@ -10075,19 +10051,19 @@
       </c>
       <c r="E171" t="str">
         <f>IF(C171,"Nenhuma",VLOOKUP(B171,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_turnovergeral</v>
+        <v>calcular_indices_ampliados</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B172" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="C172" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D172" t="b">
         <f>VLOOKUP(A172,Módulos!A:B,2,FALSE)</f>
@@ -10095,19 +10071,19 @@
       </c>
       <c r="E172" t="str">
         <f>IF(C172,"Nenhuma",VLOOKUP(B172,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_indices_ampliados</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B173" t="s">
-        <v>213</v>
+        <v>163</v>
       </c>
       <c r="C173" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D173" t="b">
         <f>VLOOKUP(A173,Módulos!A:B,2,FALSE)</f>
@@ -10115,19 +10091,19 @@
       </c>
       <c r="E173" t="str">
         <f>IF(C173,"Nenhuma",VLOOKUP(B173,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_indices_ampliados</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>210</v>
+      </c>
+      <c r="B174" t="s">
         <v>212</v>
       </c>
-      <c r="B174" t="s">
-        <v>163</v>
-      </c>
       <c r="C174" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D174" t="b">
         <f>VLOOKUP(A174,Módulos!A:B,2,FALSE)</f>
@@ -10135,15 +10111,15 @@
       </c>
       <c r="E174" t="str">
         <f>IF(C174,"Nenhuma",VLOOKUP(B174,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_indices_ampliados</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B175" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C175" t="b">
         <f>TRUE</f>
@@ -10160,10 +10136,10 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>212</v>
+        <v>110</v>
       </c>
       <c r="B176" t="s">
-        <v>215</v>
+        <v>119</v>
       </c>
       <c r="C176" t="b">
         <f>TRUE</f>
@@ -10183,7 +10159,7 @@
         <v>110</v>
       </c>
       <c r="B177" t="s">
-        <v>119</v>
+        <v>225</v>
       </c>
       <c r="C177" t="b">
         <f>TRUE</f>
@@ -10203,7 +10179,7 @@
         <v>110</v>
       </c>
       <c r="B178" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C178" t="b">
         <f>TRUE</f>
@@ -10223,7 +10199,7 @@
         <v>110</v>
       </c>
       <c r="B179" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C179" t="b">
         <f>TRUE</f>
@@ -10243,7 +10219,7 @@
         <v>110</v>
       </c>
       <c r="B180" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C180" t="b">
         <f>TRUE</f>
@@ -10263,7 +10239,7 @@
         <v>110</v>
       </c>
       <c r="B181" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="C181" t="b">
         <f>TRUE</f>
@@ -10283,7 +10259,7 @@
         <v>110</v>
       </c>
       <c r="B182" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C182" t="b">
         <f>TRUE</f>
@@ -10303,7 +10279,7 @@
         <v>110</v>
       </c>
       <c r="B183" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C183" t="b">
         <f>TRUE</f>
@@ -10323,7 +10299,7 @@
         <v>110</v>
       </c>
       <c r="B184" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C184" t="b">
         <f>TRUE</f>
@@ -10343,7 +10319,7 @@
         <v>110</v>
       </c>
       <c r="B185" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C185" t="b">
         <f>TRUE</f>
@@ -10363,7 +10339,7 @@
         <v>110</v>
       </c>
       <c r="B186" t="s">
-        <v>226</v>
+        <v>116</v>
       </c>
       <c r="C186" t="b">
         <f>TRUE</f>
@@ -10383,7 +10359,7 @@
         <v>110</v>
       </c>
       <c r="B187" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="C187" t="b">
         <f>TRUE</f>
@@ -10403,7 +10379,7 @@
         <v>110</v>
       </c>
       <c r="B188" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C188" t="b">
         <f>TRUE</f>
@@ -10423,7 +10399,7 @@
         <v>110</v>
       </c>
       <c r="B189" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C189" t="b">
         <f>TRUE</f>
@@ -10443,7 +10419,7 @@
         <v>110</v>
       </c>
       <c r="B190" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C190" t="b">
         <f>TRUE</f>
@@ -10463,7 +10439,7 @@
         <v>110</v>
       </c>
       <c r="B191" t="s">
-        <v>222</v>
+        <v>117</v>
       </c>
       <c r="C191" t="b">
         <f>TRUE</f>
@@ -10483,7 +10459,7 @@
         <v>110</v>
       </c>
       <c r="B192" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C192" t="b">
         <f>TRUE</f>
@@ -10503,7 +10479,7 @@
         <v>110</v>
       </c>
       <c r="B193" t="s">
-        <v>118</v>
+        <v>229</v>
       </c>
       <c r="C193" t="b">
         <f>TRUE</f>
@@ -10523,7 +10499,7 @@
         <v>110</v>
       </c>
       <c r="B194" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C194" t="b">
         <f>TRUE</f>
@@ -10543,7 +10519,7 @@
         <v>110</v>
       </c>
       <c r="B195" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C195" t="b">
         <f>TRUE</f>
@@ -10563,7 +10539,7 @@
         <v>110</v>
       </c>
       <c r="B196" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C196" t="b">
         <f>TRUE</f>
@@ -10583,7 +10559,7 @@
         <v>110</v>
       </c>
       <c r="B197" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C197" t="b">
         <f>TRUE</f>
@@ -10603,7 +10579,7 @@
         <v>110</v>
       </c>
       <c r="B198" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C198" t="b">
         <f>TRUE</f>
@@ -10623,7 +10599,7 @@
         <v>110</v>
       </c>
       <c r="B199" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C199" t="b">
         <f>TRUE</f>
@@ -10643,7 +10619,7 @@
         <v>110</v>
       </c>
       <c r="B200" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C200" t="b">
         <f>TRUE</f>
@@ -10663,7 +10639,7 @@
         <v>110</v>
       </c>
       <c r="B201" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C201" t="b">
         <f>TRUE</f>
@@ -10683,10 +10659,9 @@
         <v>110</v>
       </c>
       <c r="B202" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C202" t="b">
-        <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="D202" t="b">
@@ -10703,10 +10678,11 @@
         <v>110</v>
       </c>
       <c r="B203" t="s">
-        <v>240</v>
+        <v>87</v>
       </c>
       <c r="C203" t="b">
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D203" t="b">
         <f>VLOOKUP(A203,Módulos!A:B,2,FALSE)</f>
@@ -10714,7 +10690,7 @@
       </c>
       <c r="E203" t="str">
         <f>IF(C203,"Nenhuma",VLOOKUP(B203,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_eventos</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -10722,7 +10698,7 @@
         <v>110</v>
       </c>
       <c r="B204" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C204" t="b">
         <f>FALSE</f>
@@ -10742,7 +10718,7 @@
         <v>110</v>
       </c>
       <c r="B205" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C205" t="b">
         <f>FALSE</f>
@@ -10762,7 +10738,7 @@
         <v>110</v>
       </c>
       <c r="B206" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C206" t="b">
         <f>FALSE</f>
@@ -10782,7 +10758,7 @@
         <v>110</v>
       </c>
       <c r="B207" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C207" t="b">
         <f>FALSE</f>
@@ -10802,7 +10778,7 @@
         <v>110</v>
       </c>
       <c r="B208" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C208" t="b">
         <f>FALSE</f>
@@ -10822,7 +10798,7 @@
         <v>110</v>
       </c>
       <c r="B209" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C209" t="b">
         <f>FALSE</f>
@@ -10842,7 +10818,7 @@
         <v>110</v>
       </c>
       <c r="B210" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C210" t="b">
         <f>FALSE</f>
@@ -10859,14 +10835,14 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>110</v>
+        <v>254</v>
       </c>
       <c r="B211" t="s">
-        <v>94</v>
+        <v>255</v>
       </c>
       <c r="C211" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D211" t="b">
         <f>VLOOKUP(A211,Módulos!A:B,2,FALSE)</f>
@@ -10874,15 +10850,15 @@
       </c>
       <c r="E211" t="str">
         <f>IF(C211,"Nenhuma",VLOOKUP(B211,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_eventos</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
+        <v>254</v>
+      </c>
+      <c r="B212" t="s">
         <v>256</v>
-      </c>
-      <c r="B212" t="s">
-        <v>257</v>
       </c>
       <c r="C212" t="b">
         <f>TRUE</f>
@@ -10899,14 +10875,14 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B213" t="s">
-        <v>258</v>
+        <v>87</v>
       </c>
       <c r="C213" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D213" t="b">
         <f>VLOOKUP(A213,Módulos!A:B,2,FALSE)</f>
@@ -10914,15 +10890,15 @@
       </c>
       <c r="E213" t="str">
         <f>IF(C213,"Nenhuma",VLOOKUP(B213,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_eventos</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B214" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C214" t="b">
         <f>FALSE</f>
@@ -10939,10 +10915,10 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B215" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C215" t="b">
         <f>FALSE</f>
@@ -10959,10 +10935,10 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B216" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C216" t="b">
         <f>FALSE</f>
@@ -10979,14 +10955,14 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B217" t="s">
-        <v>86</v>
+        <v>257</v>
       </c>
       <c r="C217" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D217" t="b">
         <f>VLOOKUP(A217,Módulos!A:B,2,FALSE)</f>
@@ -10994,15 +10970,15 @@
       </c>
       <c r="E217" t="str">
         <f>IF(C217,"Nenhuma",VLOOKUP(B217,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_eventos</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B218" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C218" t="b">
         <f>TRUE</f>
@@ -11019,10 +10995,10 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B219" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C219" t="b">
         <f>TRUE</f>
@@ -11039,10 +11015,10 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B220" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C220" t="b">
         <f>TRUE</f>
@@ -11059,10 +11035,10 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B221" t="s">
-        <v>259</v>
+        <v>117</v>
       </c>
       <c r="C221" t="b">
         <f>TRUE</f>
@@ -11079,10 +11055,10 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B222" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C222" t="b">
         <f>TRUE</f>
@@ -11099,14 +11075,14 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="B223" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="C223" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D223" t="b">
         <f>VLOOKUP(A223,Módulos!A:B,2,FALSE)</f>
@@ -11114,15 +11090,15 @@
       </c>
       <c r="E223" t="str">
         <f>IF(C223,"Nenhuma",VLOOKUP(B223,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_beneficios_inss</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B224" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C224" t="b">
         <f>FALSE</f>
@@ -11139,10 +11115,10 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B225" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C225" t="b">
         <f>FALSE</f>
@@ -11159,10 +11135,10 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B226" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C226" t="b">
         <f>FALSE</f>
@@ -11179,14 +11155,14 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B227" t="s">
-        <v>129</v>
+        <v>240</v>
       </c>
       <c r="C227" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D227" t="b">
         <f>VLOOKUP(A227,Módulos!A:B,2,FALSE)</f>
@@ -11194,15 +11170,15 @@
       </c>
       <c r="E227" t="str">
         <f>IF(C227,"Nenhuma",VLOOKUP(B227,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_beneficios_inss</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B228" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C228" t="b">
         <f>TRUE</f>
@@ -11219,10 +11195,10 @@
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B229" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C229" t="b">
         <f>TRUE</f>
@@ -11239,10 +11215,10 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B230" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C230" t="b">
         <f>TRUE</f>
@@ -11259,10 +11235,10 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B231" t="s">
-        <v>245</v>
+        <v>2</v>
       </c>
       <c r="C231" t="b">
         <f>TRUE</f>
@@ -11279,10 +11255,10 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B232" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C232" t="b">
         <f>TRUE</f>
@@ -11299,14 +11275,14 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B233" t="s">
-        <v>1</v>
+        <v>175</v>
       </c>
       <c r="C233" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D233" t="b">
         <f>VLOOKUP(A233,Módulos!A:B,2,FALSE)</f>
@@ -11314,31 +11290,11 @@
       </c>
       <c r="E233" t="str">
         <f>IF(C233,"Nenhuma",VLOOKUP(B233,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
-      </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
-        <v>288</v>
-      </c>
-      <c r="B234" t="s">
-        <v>176</v>
-      </c>
-      <c r="C234" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="D234" t="b">
-        <f>VLOOKUP(A234,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="E234" t="str">
-        <f>IF(C234,"Nenhuma",VLOOKUP(B234,Funcoes_Outputs!B:D,3,FALSE))</f>
         <v>calcular_turnovergeral</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E223" xr:uid="{D8C2AD8A-D29B-4ECE-B686-2DDAE10A4D17}"/>
+  <autoFilter ref="A1:E222" xr:uid="{D8C2AD8A-D29B-4ECE-B686-2DDAE10A4D17}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Remover Produção Projetada do modelo
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Custos!$A$1:$D$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Funcoes_Inputs!$A$1:$E$222</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Funcoes_Inputs!$A$1:$E$219</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lista_de_Parâmetros!$A$1:$F$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Módulos!$A$1:$B$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Parametros!$A$1:$G$54</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="303">
   <si>
     <t>Ano</t>
   </si>
@@ -1463,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3748,8 +3748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6622,10 +6622,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E233"/>
+  <dimension ref="A1:E230"/>
   <sheetViews>
-    <sheetView topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138"/>
+    <sheetView topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="B155" sqref="B155:B156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9719,7 +9719,7 @@
         <v>194</v>
       </c>
       <c r="B155" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C155" t="b">
         <f>TRUE</f>
@@ -9736,10 +9736,10 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B156" t="s">
-        <v>197</v>
+        <v>264</v>
       </c>
       <c r="C156" t="b">
         <f>TRUE</f>
@@ -9756,10 +9756,10 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B157" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C157" t="b">
         <f>TRUE</f>
@@ -9776,10 +9776,10 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B158" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C158" t="b">
         <f>TRUE</f>
@@ -9796,10 +9796,10 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B159" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C159" t="b">
         <f>TRUE</f>
@@ -9819,7 +9819,7 @@
         <v>206</v>
       </c>
       <c r="B160" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C160" t="b">
         <f>TRUE</f>
@@ -9839,7 +9839,7 @@
         <v>206</v>
       </c>
       <c r="B161" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C161" t="b">
         <f>TRUE</f>
@@ -9859,7 +9859,7 @@
         <v>206</v>
       </c>
       <c r="B162" t="s">
-        <v>203</v>
+        <v>168</v>
       </c>
       <c r="C162" t="b">
         <f>TRUE</f>
@@ -9879,11 +9879,11 @@
         <v>206</v>
       </c>
       <c r="B163" t="s">
-        <v>204</v>
+        <v>162</v>
       </c>
       <c r="C163" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D163" t="b">
         <f>VLOOKUP(A163,Módulos!A:B,2,FALSE)</f>
@@ -9891,7 +9891,7 @@
       </c>
       <c r="E163" t="str">
         <f>IF(C163,"Nenhuma",VLOOKUP(B163,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_indices_ampliados</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -9899,11 +9899,11 @@
         <v>206</v>
       </c>
       <c r="B164" t="s">
-        <v>205</v>
+        <v>163</v>
       </c>
       <c r="C164" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D164" t="b">
         <f>VLOOKUP(A164,Módulos!A:B,2,FALSE)</f>
@@ -9911,7 +9911,7 @@
       </c>
       <c r="E164" t="str">
         <f>IF(C164,"Nenhuma",VLOOKUP(B164,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_indices_ampliados</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -9919,7 +9919,7 @@
         <v>206</v>
       </c>
       <c r="B165" t="s">
-        <v>168</v>
+        <v>1</v>
       </c>
       <c r="C165" t="b">
         <f>TRUE</f>
@@ -9939,11 +9939,11 @@
         <v>206</v>
       </c>
       <c r="B166" t="s">
-        <v>162</v>
+        <v>209</v>
       </c>
       <c r="C166" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D166" t="b">
         <f>VLOOKUP(A166,Módulos!A:B,2,FALSE)</f>
@@ -9951,7 +9951,7 @@
       </c>
       <c r="E166" t="str">
         <f>IF(C166,"Nenhuma",VLOOKUP(B166,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_indices_ampliados</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -9959,7 +9959,7 @@
         <v>206</v>
       </c>
       <c r="B167" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="C167" t="b">
         <f>FALSE</f>
@@ -9971,19 +9971,19 @@
       </c>
       <c r="E167" t="str">
         <f>IF(C167,"Nenhuma",VLOOKUP(B167,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_indices_ampliados</v>
+        <v>calcular_turnovergeral</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B168" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="C168" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D168" t="b">
         <f>VLOOKUP(A168,Módulos!A:B,2,FALSE)</f>
@@ -9991,15 +9991,15 @@
       </c>
       <c r="E168" t="str">
         <f>IF(C168,"Nenhuma",VLOOKUP(B168,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_indices_ampliados</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B169" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C169" t="b">
         <f>TRUE</f>
@@ -10016,10 +10016,10 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B170" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="C170" t="b">
         <f>FALSE</f>
@@ -10031,7 +10031,7 @@
       </c>
       <c r="E170" t="str">
         <f>IF(C170,"Nenhuma",VLOOKUP(B170,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_turnovergeral</v>
+        <v>calcular_indices_ampliados</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -10039,11 +10039,11 @@
         <v>210</v>
       </c>
       <c r="B171" t="s">
-        <v>162</v>
+        <v>212</v>
       </c>
       <c r="C171" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D171" t="b">
         <f>VLOOKUP(A171,Módulos!A:B,2,FALSE)</f>
@@ -10051,7 +10051,7 @@
       </c>
       <c r="E171" t="str">
         <f>IF(C171,"Nenhuma",VLOOKUP(B171,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_indices_ampliados</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -10059,7 +10059,7 @@
         <v>210</v>
       </c>
       <c r="B172" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C172" t="b">
         <f>TRUE</f>
@@ -10076,14 +10076,14 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>210</v>
+        <v>110</v>
       </c>
       <c r="B173" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
       <c r="C173" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D173" t="b">
         <f>VLOOKUP(A173,Módulos!A:B,2,FALSE)</f>
@@ -10091,15 +10091,15 @@
       </c>
       <c r="E173" t="str">
         <f>IF(C173,"Nenhuma",VLOOKUP(B173,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_indices_ampliados</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>210</v>
+        <v>110</v>
       </c>
       <c r="B174" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="C174" t="b">
         <f>TRUE</f>
@@ -10116,10 +10116,10 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>210</v>
+        <v>110</v>
       </c>
       <c r="B175" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="C175" t="b">
         <f>TRUE</f>
@@ -10139,7 +10139,7 @@
         <v>110</v>
       </c>
       <c r="B176" t="s">
-        <v>119</v>
+        <v>227</v>
       </c>
       <c r="C176" t="b">
         <f>TRUE</f>
@@ -10159,7 +10159,7 @@
         <v>110</v>
       </c>
       <c r="B177" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C177" t="b">
         <f>TRUE</f>
@@ -10179,7 +10179,7 @@
         <v>110</v>
       </c>
       <c r="B178" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C178" t="b">
         <f>TRUE</f>
@@ -10199,7 +10199,7 @@
         <v>110</v>
       </c>
       <c r="B179" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C179" t="b">
         <f>TRUE</f>
@@ -10219,7 +10219,7 @@
         <v>110</v>
       </c>
       <c r="B180" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C180" t="b">
         <f>TRUE</f>
@@ -10239,7 +10239,7 @@
         <v>110</v>
       </c>
       <c r="B181" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="C181" t="b">
         <f>TRUE</f>
@@ -10259,7 +10259,7 @@
         <v>110</v>
       </c>
       <c r="B182" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C182" t="b">
         <f>TRUE</f>
@@ -10279,7 +10279,7 @@
         <v>110</v>
       </c>
       <c r="B183" t="s">
-        <v>222</v>
+        <v>116</v>
       </c>
       <c r="C183" t="b">
         <f>TRUE</f>
@@ -10299,7 +10299,7 @@
         <v>110</v>
       </c>
       <c r="B184" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C184" t="b">
         <f>TRUE</f>
@@ -10319,7 +10319,7 @@
         <v>110</v>
       </c>
       <c r="B185" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C185" t="b">
         <f>TRUE</f>
@@ -10339,7 +10339,7 @@
         <v>110</v>
       </c>
       <c r="B186" t="s">
-        <v>116</v>
+        <v>219</v>
       </c>
       <c r="C186" t="b">
         <f>TRUE</f>
@@ -10359,7 +10359,7 @@
         <v>110</v>
       </c>
       <c r="B187" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C187" t="b">
         <f>TRUE</f>
@@ -10379,7 +10379,7 @@
         <v>110</v>
       </c>
       <c r="B188" t="s">
-        <v>218</v>
+        <v>117</v>
       </c>
       <c r="C188" t="b">
         <f>TRUE</f>
@@ -10399,7 +10399,7 @@
         <v>110</v>
       </c>
       <c r="B189" t="s">
-        <v>219</v>
+        <v>118</v>
       </c>
       <c r="C189" t="b">
         <f>TRUE</f>
@@ -10419,7 +10419,7 @@
         <v>110</v>
       </c>
       <c r="B190" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="C190" t="b">
         <f>TRUE</f>
@@ -10439,7 +10439,7 @@
         <v>110</v>
       </c>
       <c r="B191" t="s">
-        <v>117</v>
+        <v>230</v>
       </c>
       <c r="C191" t="b">
         <f>TRUE</f>
@@ -10459,7 +10459,7 @@
         <v>110</v>
       </c>
       <c r="B192" t="s">
-        <v>118</v>
+        <v>231</v>
       </c>
       <c r="C192" t="b">
         <f>TRUE</f>
@@ -10479,7 +10479,7 @@
         <v>110</v>
       </c>
       <c r="B193" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C193" t="b">
         <f>TRUE</f>
@@ -10499,7 +10499,7 @@
         <v>110</v>
       </c>
       <c r="B194" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C194" t="b">
         <f>TRUE</f>
@@ -10519,7 +10519,7 @@
         <v>110</v>
       </c>
       <c r="B195" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C195" t="b">
         <f>TRUE</f>
@@ -10539,7 +10539,7 @@
         <v>110</v>
       </c>
       <c r="B196" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C196" t="b">
         <f>TRUE</f>
@@ -10559,7 +10559,7 @@
         <v>110</v>
       </c>
       <c r="B197" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C197" t="b">
         <f>TRUE</f>
@@ -10579,7 +10579,7 @@
         <v>110</v>
       </c>
       <c r="B198" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C198" t="b">
         <f>TRUE</f>
@@ -10599,10 +10599,9 @@
         <v>110</v>
       </c>
       <c r="B199" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C199" t="b">
-        <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="D199" t="b">
@@ -10619,11 +10618,11 @@
         <v>110</v>
       </c>
       <c r="B200" t="s">
-        <v>236</v>
+        <v>87</v>
       </c>
       <c r="C200" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D200" t="b">
         <f>VLOOKUP(A200,Módulos!A:B,2,FALSE)</f>
@@ -10631,7 +10630,7 @@
       </c>
       <c r="E200" t="str">
         <f>IF(C200,"Nenhuma",VLOOKUP(B200,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_eventos</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -10639,11 +10638,11 @@
         <v>110</v>
       </c>
       <c r="B201" t="s">
-        <v>237</v>
+        <v>95</v>
       </c>
       <c r="C201" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D201" t="b">
         <f>VLOOKUP(A201,Módulos!A:B,2,FALSE)</f>
@@ -10651,7 +10650,7 @@
       </c>
       <c r="E201" t="str">
         <f>IF(C201,"Nenhuma",VLOOKUP(B201,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_eventos</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -10659,10 +10658,11 @@
         <v>110</v>
       </c>
       <c r="B202" t="s">
-        <v>238</v>
+        <v>88</v>
       </c>
       <c r="C202" t="b">
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D202" t="b">
         <f>VLOOKUP(A202,Módulos!A:B,2,FALSE)</f>
@@ -10670,7 +10670,7 @@
       </c>
       <c r="E202" t="str">
         <f>IF(C202,"Nenhuma",VLOOKUP(B202,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_eventos</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -10678,7 +10678,7 @@
         <v>110</v>
       </c>
       <c r="B203" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C203" t="b">
         <f>FALSE</f>
@@ -10698,7 +10698,7 @@
         <v>110</v>
       </c>
       <c r="B204" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C204" t="b">
         <f>FALSE</f>
@@ -10718,7 +10718,7 @@
         <v>110</v>
       </c>
       <c r="B205" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C205" t="b">
         <f>FALSE</f>
@@ -10738,7 +10738,7 @@
         <v>110</v>
       </c>
       <c r="B206" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C206" t="b">
         <f>FALSE</f>
@@ -10758,7 +10758,7 @@
         <v>110</v>
       </c>
       <c r="B207" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C207" t="b">
         <f>FALSE</f>
@@ -10775,14 +10775,14 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>110</v>
+        <v>254</v>
       </c>
       <c r="B208" t="s">
-        <v>93</v>
+        <v>255</v>
       </c>
       <c r="C208" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D208" t="b">
         <f>VLOOKUP(A208,Módulos!A:B,2,FALSE)</f>
@@ -10790,19 +10790,19 @@
       </c>
       <c r="E208" t="str">
         <f>IF(C208,"Nenhuma",VLOOKUP(B208,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_eventos</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>110</v>
+        <v>254</v>
       </c>
       <c r="B209" t="s">
-        <v>86</v>
+        <v>256</v>
       </c>
       <c r="C209" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D209" t="b">
         <f>VLOOKUP(A209,Módulos!A:B,2,FALSE)</f>
@@ -10810,15 +10810,15 @@
       </c>
       <c r="E209" t="str">
         <f>IF(C209,"Nenhuma",VLOOKUP(B209,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_eventos</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>110</v>
+        <v>254</v>
       </c>
       <c r="B210" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C210" t="b">
         <f>FALSE</f>
@@ -10838,11 +10838,11 @@
         <v>254</v>
       </c>
       <c r="B211" t="s">
-        <v>255</v>
+        <v>88</v>
       </c>
       <c r="C211" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D211" t="b">
         <f>VLOOKUP(A211,Módulos!A:B,2,FALSE)</f>
@@ -10850,7 +10850,7 @@
       </c>
       <c r="E211" t="str">
         <f>IF(C211,"Nenhuma",VLOOKUP(B211,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_eventos</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -10858,11 +10858,11 @@
         <v>254</v>
       </c>
       <c r="B212" t="s">
-        <v>256</v>
+        <v>85</v>
       </c>
       <c r="C212" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D212" t="b">
         <f>VLOOKUP(A212,Módulos!A:B,2,FALSE)</f>
@@ -10870,7 +10870,7 @@
       </c>
       <c r="E212" t="str">
         <f>IF(C212,"Nenhuma",VLOOKUP(B212,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_eventos</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -10878,7 +10878,7 @@
         <v>254</v>
       </c>
       <c r="B213" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C213" t="b">
         <f>FALSE</f>
@@ -10898,11 +10898,11 @@
         <v>254</v>
       </c>
       <c r="B214" t="s">
-        <v>88</v>
+        <v>257</v>
       </c>
       <c r="C214" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D214" t="b">
         <f>VLOOKUP(A214,Módulos!A:B,2,FALSE)</f>
@@ -10910,19 +10910,19 @@
       </c>
       <c r="E214" t="str">
         <f>IF(C214,"Nenhuma",VLOOKUP(B214,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_eventos</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="B215" t="s">
-        <v>85</v>
+        <v>260</v>
       </c>
       <c r="C215" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D215" t="b">
         <f>VLOOKUP(A215,Módulos!A:B,2,FALSE)</f>
@@ -10930,19 +10930,19 @@
       </c>
       <c r="E215" t="str">
         <f>IF(C215,"Nenhuma",VLOOKUP(B215,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_eventos</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="B216" t="s">
-        <v>86</v>
+        <v>261</v>
       </c>
       <c r="C216" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D216" t="b">
         <f>VLOOKUP(A216,Módulos!A:B,2,FALSE)</f>
@@ -10950,12 +10950,12 @@
       </c>
       <c r="E216" t="str">
         <f>IF(C216,"Nenhuma",VLOOKUP(B216,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_eventos</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="B217" t="s">
         <v>257</v>
@@ -10978,7 +10978,7 @@
         <v>262</v>
       </c>
       <c r="B218" t="s">
-        <v>260</v>
+        <v>117</v>
       </c>
       <c r="C218" t="b">
         <f>TRUE</f>
@@ -10998,7 +10998,7 @@
         <v>262</v>
       </c>
       <c r="B219" t="s">
-        <v>261</v>
+        <v>118</v>
       </c>
       <c r="C219" t="b">
         <f>TRUE</f>
@@ -11015,14 +11015,14 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="B220" t="s">
-        <v>257</v>
+        <v>126</v>
       </c>
       <c r="C220" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D220" t="b">
         <f>VLOOKUP(A220,Módulos!A:B,2,FALSE)</f>
@@ -11030,19 +11030,19 @@
       </c>
       <c r="E220" t="str">
         <f>IF(C220,"Nenhuma",VLOOKUP(B220,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_beneficios_inss</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="B221" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="C221" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D221" t="b">
         <f>VLOOKUP(A221,Módulos!A:B,2,FALSE)</f>
@@ -11050,19 +11050,19 @@
       </c>
       <c r="E221" t="str">
         <f>IF(C221,"Nenhuma",VLOOKUP(B221,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_beneficios_inss</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="B222" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="C222" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D222" t="b">
         <f>VLOOKUP(A222,Módulos!A:B,2,FALSE)</f>
@@ -11070,7 +11070,7 @@
       </c>
       <c r="E222" t="str">
         <f>IF(C222,"Nenhuma",VLOOKUP(B222,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_beneficios_inss</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -11078,7 +11078,7 @@
         <v>286</v>
       </c>
       <c r="B223" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C223" t="b">
         <f>FALSE</f>
@@ -11098,11 +11098,11 @@
         <v>286</v>
       </c>
       <c r="B224" t="s">
-        <v>127</v>
+        <v>240</v>
       </c>
       <c r="C224" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D224" t="b">
         <f>VLOOKUP(A224,Módulos!A:B,2,FALSE)</f>
@@ -11110,7 +11110,7 @@
       </c>
       <c r="E224" t="str">
         <f>IF(C224,"Nenhuma",VLOOKUP(B224,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_beneficios_inss</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -11118,11 +11118,11 @@
         <v>286</v>
       </c>
       <c r="B225" t="s">
-        <v>128</v>
+        <v>241</v>
       </c>
       <c r="C225" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D225" t="b">
         <f>VLOOKUP(A225,Módulos!A:B,2,FALSE)</f>
@@ -11130,7 +11130,7 @@
       </c>
       <c r="E225" t="str">
         <f>IF(C225,"Nenhuma",VLOOKUP(B225,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_beneficios_inss</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
@@ -11138,11 +11138,11 @@
         <v>286</v>
       </c>
       <c r="B226" t="s">
-        <v>129</v>
+        <v>242</v>
       </c>
       <c r="C226" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D226" t="b">
         <f>VLOOKUP(A226,Módulos!A:B,2,FALSE)</f>
@@ -11150,7 +11150,7 @@
       </c>
       <c r="E226" t="str">
         <f>IF(C226,"Nenhuma",VLOOKUP(B226,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_beneficios_inss</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -11158,7 +11158,7 @@
         <v>286</v>
       </c>
       <c r="B227" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C227" t="b">
         <f>TRUE</f>
@@ -11178,7 +11178,7 @@
         <v>286</v>
       </c>
       <c r="B228" t="s">
-        <v>241</v>
+        <v>2</v>
       </c>
       <c r="C228" t="b">
         <f>TRUE</f>
@@ -11198,7 +11198,7 @@
         <v>286</v>
       </c>
       <c r="B229" t="s">
-        <v>242</v>
+        <v>1</v>
       </c>
       <c r="C229" t="b">
         <f>TRUE</f>
@@ -11218,11 +11218,11 @@
         <v>286</v>
       </c>
       <c r="B230" t="s">
-        <v>243</v>
+        <v>175</v>
       </c>
       <c r="C230" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D230" t="b">
         <f>VLOOKUP(A230,Módulos!A:B,2,FALSE)</f>
@@ -11230,71 +11230,11 @@
       </c>
       <c r="E230" t="str">
         <f>IF(C230,"Nenhuma",VLOOKUP(B230,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
-      </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
-        <v>286</v>
-      </c>
-      <c r="B231" t="s">
-        <v>2</v>
-      </c>
-      <c r="C231" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="D231" t="b">
-        <f>VLOOKUP(A231,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="E231" t="str">
-        <f>IF(C231,"Nenhuma",VLOOKUP(B231,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>286</v>
-      </c>
-      <c r="B232" t="s">
-        <v>1</v>
-      </c>
-      <c r="C232" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="D232" t="b">
-        <f>VLOOKUP(A232,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="E232" t="str">
-        <f>IF(C232,"Nenhuma",VLOOKUP(B232,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
-        <v>286</v>
-      </c>
-      <c r="B233" t="s">
-        <v>175</v>
-      </c>
-      <c r="C233" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="D233" t="b">
-        <f>VLOOKUP(A233,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="E233" t="str">
-        <f>IF(C233,"Nenhuma",VLOOKUP(B233,Funcoes_Outputs!B:D,3,FALSE))</f>
         <v>calcular_turnovergeral</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E222" xr:uid="{D8C2AD8A-D29B-4ECE-B686-2DDAE10A4D17}"/>
+  <autoFilter ref="A1:E219" xr:uid="{D8C2AD8A-D29B-4ECE-B686-2DDAE10A4D17}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Mudança #14 Implementada (Lucro Cessante isolado por caso, e sem dias).
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -24,10 +24,10 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Custos!$A$1:$D$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Funcoes_Inputs!$A$1:$E$219</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Funcoes_Inputs!$A$1:$E$217</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lista_de_Parâmetros!$A$1:$F$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Módulos!$A$1:$B$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Parametros!$A$1:$G$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Parametros!$A$1:$G$53</definedName>
     <definedName name="Ano_Inicial">Configs!$D$2:$D$2</definedName>
     <definedName name="Anos_a_Serem_Simulados">Configs!$A$2</definedName>
     <definedName name="CategoriaSAT">Configs!$C$2:$C$2</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="306">
   <si>
     <t>Ano</t>
   </si>
@@ -815,9 +815,6 @@
     <t>DiasInterrupcaoAcidenteOutros</t>
   </si>
   <si>
-    <t>LucroCessanteDiario</t>
-  </si>
-  <si>
     <t>DiasTotaisInterrupcaoAcidente</t>
   </si>
   <si>
@@ -951,6 +948,18 @@
   </si>
   <si>
     <t>SeedFixa</t>
+  </si>
+  <si>
+    <t>LucroCessanteAcidenteObito</t>
+  </si>
+  <si>
+    <t>LucroCessanteAcidenteOutros</t>
+  </si>
+  <si>
+    <t>LucroCessanteInterdicaoFiscalizacao</t>
+  </si>
+  <si>
+    <t>normaltruncada</t>
   </si>
 </sst>
 </file>
@@ -963,7 +972,22 @@
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1010,7 +1034,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1043,6 +1067,8 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -1484,7 +1510,7 @@
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2240,7 +2266,7 @@
         <v>198</v>
       </c>
       <c r="B64" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
@@ -2300,7 +2326,7 @@
         <v>254</v>
       </c>
       <c r="B69" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="1"/>
@@ -2312,7 +2338,7 @@
         <v>254</v>
       </c>
       <c r="B70" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="1"/>
@@ -2321,10 +2347,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>261</v>
+      </c>
+      <c r="B71" t="s">
         <v>262</v>
-      </c>
-      <c r="B71" t="s">
-        <v>263</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="1"/>
@@ -2333,7 +2359,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B72" t="s">
         <v>239</v>
@@ -2345,10 +2371,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>285</v>
+      </c>
+      <c r="B73" t="s">
         <v>286</v>
-      </c>
-      <c r="B73" t="s">
-        <v>287</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="1"/>
@@ -2357,10 +2383,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B74" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="1"/>
@@ -2369,10 +2395,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B75" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="1"/>
@@ -2381,10 +2407,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B76" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="1"/>
@@ -2393,10 +2419,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B77" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="1"/>
@@ -2405,10 +2431,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B78" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="1"/>
@@ -2417,10 +2443,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="1"/>
@@ -2429,10 +2455,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B80" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="1"/>
@@ -2441,10 +2467,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B81" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="1"/>
@@ -2453,10 +2479,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B82" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="1"/>
@@ -2465,7 +2491,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B83" t="s">
         <v>24</v>
@@ -2651,7 +2677,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
@@ -2665,7 +2691,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B5" t="s">
         <v>59</v>
@@ -3581,7 +3607,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B2" t="b">
         <f>TRUE</f>
@@ -3746,2487 +3772,2612 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H111"/>
+  <dimension ref="A1:H115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="19" customWidth="1"/>
+    <col min="5" max="6" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" style="19" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>302</v>
+      <c r="H1" s="18" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="19">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="19">
         <f t="shared" ref="D2:D9" si="0">C2*0.01</f>
         <v>0.05</v>
       </c>
-      <c r="G2" t="s">
-        <v>283</v>
-      </c>
-      <c r="H2" t="b">
+      <c r="G2" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H2" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A2)&gt;0,FALSE,TRUE)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="19">
         <v>1000</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="19">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G3" t="s">
-        <v>283</v>
-      </c>
-      <c r="H3" t="b">
+      <c r="G3" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H3" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A3)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="19">
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="19">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="G4" t="s">
-        <v>283</v>
-      </c>
-      <c r="H4" t="b">
+      <c r="G4" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H4" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A4)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="19">
         <v>0.5</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="19">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G5" t="s">
-        <v>283</v>
-      </c>
-      <c r="H5" t="b">
+      <c r="G5" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H5" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A5)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="19">
         <v>0.1</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="19">
         <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
-      <c r="G6" t="s">
-        <v>283</v>
-      </c>
-      <c r="H6" t="b">
+      <c r="G6" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H6" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A6)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="19">
         <v>0.01</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="19">
         <f t="shared" si="0"/>
         <v>1E-4</v>
       </c>
-      <c r="G7" t="s">
-        <v>283</v>
-      </c>
-      <c r="H7" t="b">
+      <c r="G7" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H7" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A7)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="19">
         <v>2500</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="19">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="G8" t="s">
-        <v>283</v>
-      </c>
-      <c r="H8" t="b">
+      <c r="G8" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H8" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A8)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="19">
         <v>2000</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G9" t="s">
-        <v>283</v>
-      </c>
-      <c r="H9" t="b">
+      <c r="G9" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H9" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A9)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="19">
         <v>2000</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="19">
         <f t="shared" ref="D10" si="1">C10*0.01</f>
         <v>20</v>
       </c>
-      <c r="G10" t="s">
-        <v>283</v>
-      </c>
-      <c r="H10" t="b">
+      <c r="G10" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H10" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A10)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="19">
         <v>0.1</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="19">
         <f t="shared" ref="D11" si="2">C11*0.01</f>
         <v>1E-3</v>
       </c>
-      <c r="G11" t="s">
-        <v>283</v>
-      </c>
-      <c r="H11" t="b">
+      <c r="G11" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H11" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A11)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="19">
         <v>1000</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="19">
         <f t="shared" ref="D12" si="3">C12*0.01</f>
         <v>10</v>
       </c>
-      <c r="G12" t="s">
-        <v>283</v>
-      </c>
-      <c r="H12" t="b">
+      <c r="G12" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H12" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A12)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="19">
         <v>0.1</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="19">
         <f t="shared" ref="D13:D14" si="4">C13*0.01</f>
         <v>1E-3</v>
       </c>
-      <c r="G13" t="s">
-        <v>283</v>
-      </c>
-      <c r="H13" t="b">
+      <c r="G13" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H13" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A13)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="19">
         <v>1000</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="19">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="G14" t="s">
-        <v>283</v>
-      </c>
-      <c r="H14" t="b">
+      <c r="G14" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H14" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A14)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
+      <c r="C15" s="19">
+        <v>0</v>
+      </c>
+      <c r="D15" s="19">
         <f t="shared" ref="D15" si="5">C15*0.01</f>
         <v>0</v>
       </c>
-      <c r="G15" t="s">
-        <v>283</v>
-      </c>
-      <c r="H15" t="b">
+      <c r="G15" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H15" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A15)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
+      <c r="C16" s="19">
+        <v>0</v>
+      </c>
+      <c r="D16" s="19">
         <f t="shared" ref="D16" si="6">C16*0.01</f>
         <v>0</v>
       </c>
-      <c r="G16" t="s">
-        <v>283</v>
-      </c>
-      <c r="H16" t="b">
+      <c r="G16" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H16" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A16)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="19">
         <v>10</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="19">
         <f t="shared" ref="D17" si="7">C17*0.01</f>
         <v>0.1</v>
       </c>
-      <c r="G17" t="s">
-        <v>283</v>
-      </c>
-      <c r="H17" t="b">
+      <c r="G17" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H17" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A17)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
+      <c r="C18" s="19">
+        <v>0</v>
+      </c>
+      <c r="D18" s="19">
         <f t="shared" ref="D18:D19" si="8">C18*0.01</f>
         <v>0</v>
       </c>
-      <c r="G18" t="s">
-        <v>283</v>
-      </c>
-      <c r="H18" t="b">
+      <c r="G18" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H18" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A18)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="19">
         <v>2</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="19">
         <f t="shared" si="8"/>
         <v>0.02</v>
       </c>
-      <c r="G19" t="s">
-        <v>283</v>
-      </c>
-      <c r="H19" t="b">
+      <c r="G19" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H19" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A19)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="19">
         <v>2</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="19">
         <f t="shared" ref="D20:D24" si="9">C20*0.01</f>
         <v>0.02</v>
       </c>
-      <c r="G20" t="s">
-        <v>283</v>
-      </c>
-      <c r="H20" t="b">
+      <c r="G20" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H20" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A20)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="19">
         <v>2</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="19">
         <f t="shared" si="9"/>
         <v>0.02</v>
       </c>
-      <c r="G21" t="s">
-        <v>283</v>
-      </c>
-      <c r="H21" t="b">
+      <c r="G21" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H21" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A21)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="19">
         <v>2</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="19">
         <f t="shared" si="9"/>
         <v>0.02</v>
       </c>
-      <c r="G22" t="s">
-        <v>283</v>
-      </c>
-      <c r="H22" t="b">
+      <c r="G22" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H22" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A22)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="19">
         <v>2</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="19">
         <f t="shared" si="9"/>
         <v>0.02</v>
       </c>
-      <c r="G23" t="s">
-        <v>283</v>
-      </c>
-      <c r="H23" t="b">
+      <c r="G23" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H23" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A23)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="19">
         <v>500</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="19">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="G24" t="s">
-        <v>283</v>
-      </c>
-      <c r="H24" t="b">
+      <c r="G24" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H24" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A24)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="19">
         <v>500</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="19">
         <f t="shared" ref="D25:D33" si="10">C25*0.01</f>
         <v>5</v>
       </c>
-      <c r="G25" t="s">
-        <v>283</v>
-      </c>
-      <c r="H25" t="b">
+      <c r="G25" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H25" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A25)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="19">
         <v>500</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="19">
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
-      <c r="G26" t="s">
-        <v>283</v>
-      </c>
-      <c r="H26" t="b">
+      <c r="G26" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H26" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A26)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="19">
         <v>500</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="19">
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
-      <c r="G27" t="s">
-        <v>283</v>
-      </c>
-      <c r="H27" t="b">
+      <c r="G27" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H27" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A27)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="19">
         <v>500</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="19">
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
-      <c r="G28" t="s">
-        <v>283</v>
-      </c>
-      <c r="H28" t="b">
+      <c r="G28" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H28" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A28)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
+      <c r="C29" s="19">
+        <v>0</v>
+      </c>
+      <c r="D29" s="19">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G29" t="s">
-        <v>283</v>
-      </c>
-      <c r="H29" t="b">
+      <c r="G29" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H29" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A29)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
+      <c r="C30" s="19">
+        <v>0</v>
+      </c>
+      <c r="D30" s="19">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G30" t="s">
-        <v>283</v>
-      </c>
-      <c r="H30" t="b">
+      <c r="G30" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H30" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A30)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
+      <c r="C31" s="19">
+        <v>0</v>
+      </c>
+      <c r="D31" s="19">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G31" t="s">
-        <v>283</v>
-      </c>
-      <c r="H31" t="b">
+      <c r="G31" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H31" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A31)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
+      <c r="C32" s="19">
+        <v>0</v>
+      </c>
+      <c r="D32" s="19">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G32" t="s">
-        <v>283</v>
-      </c>
-      <c r="H32" t="b">
+      <c r="G32" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H32" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A32)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
+      <c r="C33" s="19">
+        <v>0</v>
+      </c>
+      <c r="D33" s="19">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G33" t="s">
-        <v>283</v>
-      </c>
-      <c r="H33" t="b">
+      <c r="G33" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H33" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A33)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="19">
         <v>10</v>
       </c>
-      <c r="D34">
-        <f t="shared" ref="D34:D36" si="11">C34*0.01</f>
+      <c r="D34" s="19">
+        <f t="shared" ref="D34:D35" si="11">C34*0.01</f>
         <v>0.1</v>
       </c>
-      <c r="G34" t="s">
-        <v>283</v>
-      </c>
-      <c r="H34" t="b">
+      <c r="G34" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H34" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A34)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35">
+      <c r="C35" s="19">
+        <v>1</v>
+      </c>
+      <c r="D35" s="19">
         <f t="shared" si="11"/>
         <v>0.01</v>
       </c>
-      <c r="G35" t="s">
-        <v>283</v>
-      </c>
-      <c r="H35" t="b">
+      <c r="G35" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H35" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A35)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>257</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="A36" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="B36" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C36">
-        <v>1000</v>
-      </c>
-      <c r="D36">
-        <f t="shared" si="11"/>
+      <c r="C36" s="19">
+        <v>2</v>
+      </c>
+      <c r="D36" s="19">
+        <f t="shared" ref="D36:D37" si="12">C36*0.01</f>
+        <v>0.02</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H36" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A36)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="19">
         <v>10</v>
       </c>
-      <c r="G36" t="s">
-        <v>283</v>
-      </c>
-      <c r="H36" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A36)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>260</v>
-      </c>
-      <c r="B37" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37">
-        <f t="shared" ref="D37:D38" si="12">C37*0.01</f>
-        <v>0.02</v>
-      </c>
-      <c r="G37" t="s">
-        <v>283</v>
-      </c>
-      <c r="H37" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A37)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>261</v>
-      </c>
-      <c r="B38" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38">
-        <v>10</v>
-      </c>
-      <c r="D38">
+      <c r="D37" s="19">
         <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
-      <c r="G38" t="s">
-        <v>283</v>
-      </c>
-      <c r="H38" t="b">
+      <c r="G37" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H37" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A37)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="19">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D38" s="19">
+        <f t="shared" ref="D38" si="13">C38*0.01</f>
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H38" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A38)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="19">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D39">
-        <f t="shared" ref="D39" si="13">C39*0.01</f>
+      <c r="D39" s="19">
+        <f t="shared" ref="D39:D41" si="14">C39*0.01</f>
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="G39" t="s">
-        <v>283</v>
-      </c>
-      <c r="H39" t="b">
+      <c r="G39" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H39" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A39)&gt;0,FALSE,TRUE)</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="19">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D40">
-        <f t="shared" ref="D40:D42" si="14">C40*0.01</f>
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="G40" t="s">
-        <v>283</v>
-      </c>
-      <c r="H40" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A40)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>269</v>
-      </c>
-      <c r="B41" t="s">
-        <v>65</v>
-      </c>
-      <c r="C41">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="D41">
+      <c r="D40" s="19">
         <f t="shared" si="14"/>
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="G41" t="s">
-        <v>283</v>
-      </c>
-      <c r="H41" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A41)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>270</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="G40" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H40" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A40)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="B41" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C42">
+      <c r="C41" s="19">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D42">
+      <c r="D41" s="19">
         <f t="shared" si="14"/>
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="G42" t="s">
-        <v>283</v>
-      </c>
-      <c r="H42" t="b">
+      <c r="G41" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H41" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A41)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="19">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D42" s="19">
+        <f t="shared" ref="D42:D93" si="15">C42*0.01</f>
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="G42" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H42" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A42)&gt;0,FALSE,TRUE)</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="19">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D43">
-        <f t="shared" ref="D43:D95" si="15">C43*0.01</f>
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="G43" t="s">
-        <v>283</v>
-      </c>
-      <c r="H43" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A43)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>272</v>
-      </c>
-      <c r="B44" t="s">
-        <v>65</v>
-      </c>
-      <c r="C44">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="D44">
+      <c r="D43" s="19">
         <f t="shared" si="15"/>
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="G44" t="s">
-        <v>283</v>
-      </c>
-      <c r="H44" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A44)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>273</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="G43" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H43" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A43)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C45">
+      <c r="C44" s="19">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D45">
+      <c r="D44" s="19">
         <f t="shared" si="15"/>
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="G45" t="s">
-        <v>283</v>
-      </c>
-      <c r="H45" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A45)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>274</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="G44" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H44" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A44)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C46">
+      <c r="C45" s="19">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D46">
+      <c r="D45" s="19">
         <f t="shared" si="15"/>
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="G46" t="s">
-        <v>283</v>
-      </c>
-      <c r="H46" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A46)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>275</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="G45" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H45" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A45)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C47">
+      <c r="C46" s="19">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D47">
+      <c r="D46" s="19">
         <f t="shared" si="15"/>
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="G47" t="s">
-        <v>283</v>
-      </c>
-      <c r="H47" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A47)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>276</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="G46" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H46" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A46)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="B47" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C48">
+      <c r="C47" s="19">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D48">
+      <c r="D47" s="19">
         <f t="shared" si="15"/>
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="G48" t="s">
-        <v>283</v>
-      </c>
-      <c r="H48" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A48)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>277</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="G47" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H47" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A47)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="B48" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C49">
+      <c r="C48" s="19">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D49">
+      <c r="D48" s="19">
         <f t="shared" si="15"/>
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="G49" t="s">
-        <v>283</v>
-      </c>
-      <c r="H49" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A49)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>278</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="G48" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H48" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A48)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="B49" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C50">
+      <c r="C49" s="19">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D50">
+      <c r="D49" s="19">
         <f t="shared" si="15"/>
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="G50" t="s">
-        <v>283</v>
-      </c>
-      <c r="H50" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A50)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>279</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="G49" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H49" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A49)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="B50" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C51">
+      <c r="C50" s="19">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D51">
+      <c r="D50" s="19">
         <f t="shared" si="15"/>
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="G51" t="s">
-        <v>283</v>
-      </c>
-      <c r="H51" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A51)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>280</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="G50" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H50" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A50)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C52">
+      <c r="C51" s="19">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D52">
+      <c r="D51" s="19">
         <f t="shared" si="15"/>
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="G52" t="s">
-        <v>283</v>
-      </c>
-      <c r="H52" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A52)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>281</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="G51" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H51" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A51)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="B52" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C53">
+      <c r="C52" s="19">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D53">
+      <c r="D52" s="19">
         <f t="shared" si="15"/>
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="G53" t="s">
-        <v>283</v>
-      </c>
-      <c r="H53" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A53)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="G52" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="B54" t="s">
+      <c r="H52" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A52)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="B53" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C54">
+      <c r="C53" s="19">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D54">
+      <c r="D53" s="19">
         <f t="shared" si="15"/>
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="G54" t="s">
-        <v>283</v>
-      </c>
-      <c r="H54" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A54)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="G53" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H53" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A53)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B54" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C55">
+      <c r="C54" s="19">
         <v>3</v>
       </c>
-      <c r="D55">
+      <c r="D54" s="19">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G54" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H55" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A55)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="H54" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A54)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B55" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C56">
+      <c r="C55" s="19">
         <v>800</v>
       </c>
-      <c r="D56">
+      <c r="D55" s="19">
         <f t="shared" si="15"/>
         <v>8</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G55" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H56" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A56)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="H55" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A55)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B56" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C57">
+      <c r="C56" s="19">
         <v>3</v>
       </c>
-      <c r="D57">
+      <c r="D56" s="19">
         <f t="shared" si="15"/>
         <v>0.03</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G56" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H57" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A57)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="H56" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A56)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B57" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C58">
+      <c r="C57" s="19">
         <v>0.2</v>
       </c>
-      <c r="D58">
+      <c r="D57" s="19">
         <f t="shared" si="15"/>
         <v>2E-3</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G57" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H58" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A58)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="H57" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A57)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B58" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C59">
+      <c r="C58" s="19">
         <v>0.05</v>
       </c>
-      <c r="D59">
+      <c r="D58" s="19">
         <f t="shared" si="15"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G58" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H59" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A59)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="17" t="s">
+      <c r="H58" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A58)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B59" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C60">
+      <c r="C59" s="19">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D60">
+      <c r="D59" s="19">
         <f t="shared" si="15"/>
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G59" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H60" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A60)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
+      <c r="H59" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A59)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B60" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C61">
+      <c r="C60" s="19">
         <v>1500</v>
       </c>
-      <c r="D61">
+      <c r="D60" s="19">
         <f t="shared" si="15"/>
         <v>15</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G60" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H61" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A61)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="17" t="s">
+      <c r="H60" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A60)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B61" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C62">
+      <c r="C61" s="19">
         <v>1500</v>
       </c>
-      <c r="D62">
+      <c r="D61" s="19">
         <f t="shared" si="15"/>
         <v>15</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G61" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H62" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A62)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="H61" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A61)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B62" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C63">
+      <c r="C62" s="19">
         <v>1500</v>
       </c>
-      <c r="D63">
+      <c r="D62" s="19">
         <f t="shared" si="15"/>
         <v>15</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G62" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H63" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A63)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="H62" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A62)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B63" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C64">
+      <c r="C63" s="19">
         <v>0.01</v>
       </c>
-      <c r="D64">
+      <c r="D63" s="19">
         <f t="shared" si="15"/>
         <v>1E-4</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G63" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H64" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A64)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="H63" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A63)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B64" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C65">
+      <c r="C64" s="19">
         <v>800</v>
       </c>
-      <c r="D65">
+      <c r="D64" s="19">
         <f t="shared" si="15"/>
         <v>8</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G64" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H65" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A65)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="H64" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A64)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B65" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C66">
+      <c r="C65" s="19">
         <v>0.05</v>
       </c>
-      <c r="D66">
+      <c r="D65" s="19">
         <f t="shared" si="15"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G65" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H66" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A66)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="H65" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A65)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B66" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C67">
+      <c r="C66" s="19">
         <v>800</v>
       </c>
-      <c r="D67">
+      <c r="D66" s="19">
         <f t="shared" si="15"/>
         <v>8</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G66" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H67" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A67)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="H66" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A66)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B67" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C68">
+      <c r="C67" s="19">
         <v>0.1</v>
       </c>
-      <c r="D68">
+      <c r="D67" s="19">
         <f t="shared" si="15"/>
         <v>1E-3</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G67" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H68" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A68)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="H67" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A67)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B68" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C69">
+      <c r="C68" s="19">
         <v>0.1</v>
       </c>
-      <c r="D69">
+      <c r="D68" s="19">
         <f t="shared" si="15"/>
         <v>1E-3</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G68" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H69" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A69)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="H68" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A68)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B69" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C70">
+      <c r="C69" s="19">
         <v>8</v>
       </c>
-      <c r="D70">
+      <c r="D69" s="19">
         <f t="shared" si="15"/>
         <v>0.08</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G69" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H70" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A70)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="H69" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A69)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B70" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C71">
+      <c r="C70" s="19">
         <v>10000</v>
       </c>
-      <c r="D71">
+      <c r="D70" s="19">
         <f t="shared" si="15"/>
         <v>100</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G70" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H71" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A71)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="H70" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A70)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B71" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C72">
-        <v>1</v>
-      </c>
-      <c r="D72">
+      <c r="C71" s="19">
+        <v>1</v>
+      </c>
+      <c r="D71" s="19">
         <f t="shared" si="15"/>
         <v>0.01</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G71" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H72" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A72)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="H71" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A71)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B72" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C73">
-        <v>1</v>
-      </c>
-      <c r="D73">
+      <c r="C72" s="19">
+        <v>1</v>
+      </c>
+      <c r="D72" s="19">
         <f t="shared" si="15"/>
         <v>0.01</v>
       </c>
-      <c r="G73" t="s">
+      <c r="G72" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H73" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A73)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="H72" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A72)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B73" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C74">
-        <v>1</v>
-      </c>
-      <c r="D74">
+      <c r="C73" s="19">
+        <v>1</v>
+      </c>
+      <c r="D73" s="19">
         <f t="shared" si="15"/>
         <v>0.01</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G73" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H74" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A74)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="H73" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A73)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B74" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C75">
-        <v>1</v>
-      </c>
-      <c r="D75">
+      <c r="C74" s="19">
+        <v>1</v>
+      </c>
+      <c r="D74" s="19">
         <f t="shared" si="15"/>
         <v>0.01</v>
       </c>
-      <c r="G75" t="s">
+      <c r="G74" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H75" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A75)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="H74" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A74)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B75" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C76">
-        <v>1</v>
-      </c>
-      <c r="D76">
+      <c r="C75" s="19">
+        <v>1</v>
+      </c>
+      <c r="D75" s="19">
         <f t="shared" si="15"/>
         <v>0.01</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G75" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H76" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A76)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="H75" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A75)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B76" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C77">
+      <c r="C76" s="19">
         <v>300</v>
       </c>
-      <c r="D77">
+      <c r="D76" s="19">
         <f t="shared" si="15"/>
         <v>3</v>
       </c>
-      <c r="G77" t="s">
+      <c r="G76" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H77" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A77)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="H76" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A76)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B77" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C78">
+      <c r="C77" s="19">
         <v>300</v>
       </c>
-      <c r="D78">
+      <c r="D77" s="19">
         <f t="shared" si="15"/>
         <v>3</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G77" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H78" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A78)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="H77" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A77)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B78" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C79">
+      <c r="C78" s="19">
         <v>300</v>
       </c>
-      <c r="D79">
+      <c r="D78" s="19">
         <f t="shared" si="15"/>
         <v>3</v>
       </c>
-      <c r="G79" t="s">
+      <c r="G78" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H79" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A79)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="H78" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A78)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B79" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C80">
+      <c r="C79" s="19">
         <v>300</v>
       </c>
-      <c r="D80">
+      <c r="D79" s="19">
         <f t="shared" si="15"/>
         <v>3</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G79" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H80" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A80)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="H79" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A79)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B80" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C81">
+      <c r="C80" s="19">
         <v>300</v>
       </c>
-      <c r="D81">
+      <c r="D80" s="19">
         <f t="shared" si="15"/>
         <v>3</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G80" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H81" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A81)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="H80" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A80)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B81" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C82">
-        <v>1</v>
-      </c>
-      <c r="D82">
+      <c r="C81" s="19">
+        <v>1</v>
+      </c>
+      <c r="D81" s="19">
         <f t="shared" si="15"/>
         <v>0.01</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G81" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H82" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A82)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="H81" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A81)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B82" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C83">
-        <v>1</v>
-      </c>
-      <c r="D83">
+      <c r="C82" s="19">
+        <v>1</v>
+      </c>
+      <c r="D82" s="19">
         <f t="shared" si="15"/>
         <v>0.01</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G82" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H83" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A83)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="H82" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A82)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B83" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C84">
-        <v>1</v>
-      </c>
-      <c r="D84">
+      <c r="C83" s="19">
+        <v>1</v>
+      </c>
+      <c r="D83" s="19">
         <f t="shared" si="15"/>
         <v>0.01</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G83" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H84" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A84)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="H83" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A83)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B84" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C85">
-        <v>1</v>
-      </c>
-      <c r="D85">
+      <c r="C84" s="19">
+        <v>1</v>
+      </c>
+      <c r="D84" s="19">
         <f t="shared" si="15"/>
         <v>0.01</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G84" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H85" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A85)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="H84" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A84)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B85" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C86">
-        <v>1</v>
-      </c>
-      <c r="D86">
+      <c r="C85" s="19">
+        <v>1</v>
+      </c>
+      <c r="D85" s="19">
         <f t="shared" si="15"/>
         <v>0.01</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G85" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H86" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A86)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="H85" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A85)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B86" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C87">
+      <c r="C86" s="19">
         <v>8</v>
       </c>
-      <c r="D87">
+      <c r="D86" s="19">
         <f t="shared" si="15"/>
         <v>0.08</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G86" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H87" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A87)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="H86" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A86)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B87" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C88">
+      <c r="C87" s="19">
         <v>0.5</v>
       </c>
-      <c r="D88">
+      <c r="D87" s="19">
         <f t="shared" si="15"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G87" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H88" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A88)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>257</v>
-      </c>
-      <c r="B89" t="s">
+      <c r="H87" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A87)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="B88" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C89">
-        <v>800</v>
-      </c>
-      <c r="D89">
-        <f t="shared" si="15"/>
-        <v>8</v>
-      </c>
-      <c r="G89" t="s">
-        <v>12</v>
-      </c>
-      <c r="H89" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A89)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>260</v>
-      </c>
-      <c r="B90" t="s">
-        <v>65</v>
-      </c>
-      <c r="C90">
-        <v>1</v>
-      </c>
-      <c r="D90">
+      <c r="C88" s="19">
+        <v>1</v>
+      </c>
+      <c r="D88" s="19">
         <f t="shared" si="15"/>
         <v>0.01</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G88" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H90" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A90)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>261</v>
-      </c>
-      <c r="B91" t="s">
+      <c r="H88" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A88)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="B89" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C91">
+      <c r="C89" s="19">
         <v>7</v>
       </c>
-      <c r="D91">
+      <c r="D89" s="19">
         <f t="shared" si="15"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G89" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H91" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A91)&gt;0,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>267</v>
-      </c>
-      <c r="B92" t="s">
+      <c r="H89" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A89)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B90" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C92">
+      <c r="C90" s="19">
         <f>0.0005/2</f>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D92">
+      <c r="D90" s="19">
         <f t="shared" si="15"/>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G90" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H92" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A92)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>268</v>
-      </c>
-      <c r="B93" t="s">
+      <c r="H90" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A90)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="B91" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C93">
-        <f t="shared" ref="C93:C107" si="16">0.0005/2</f>
+      <c r="C91" s="19">
+        <f t="shared" ref="C91:C105" si="16">0.0005/2</f>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D93">
+      <c r="D91" s="19">
         <f t="shared" si="15"/>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G91" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H93" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A93)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>269</v>
-      </c>
-      <c r="B94" t="s">
+      <c r="H91" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A91)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="B92" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C94">
+      <c r="C92" s="19">
         <f t="shared" si="16"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D94">
+      <c r="D92" s="19">
         <f t="shared" si="15"/>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G92" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H94" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A94)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>270</v>
-      </c>
-      <c r="B95" t="s">
+      <c r="H92" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A92)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="B93" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C95">
+      <c r="C93" s="19">
         <f t="shared" si="16"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D95">
+      <c r="D93" s="19">
         <f t="shared" si="15"/>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G93" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H95" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A95)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>271</v>
-      </c>
-      <c r="B96" t="s">
+      <c r="H93" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A93)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="B94" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C96">
+      <c r="C94" s="19">
         <f t="shared" si="16"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D96">
-        <f t="shared" ref="D96:D108" si="17">C96*0.01</f>
+      <c r="D94" s="19">
+        <f t="shared" ref="D94:D106" si="17">C94*0.01</f>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G94" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H96" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A96)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>272</v>
-      </c>
-      <c r="B97" t="s">
+      <c r="H94" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A94)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="B95" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C97">
+      <c r="C95" s="19">
         <f t="shared" si="16"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D97">
+      <c r="D95" s="19">
         <f t="shared" si="17"/>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G97" t="s">
+      <c r="G95" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H97" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A97)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>273</v>
-      </c>
-      <c r="B98" t="s">
+      <c r="H95" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A95)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="B96" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C98">
+      <c r="C96" s="19">
         <f t="shared" si="16"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D98">
+      <c r="D96" s="19">
         <f t="shared" si="17"/>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G96" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H98" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A98)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>274</v>
-      </c>
-      <c r="B99" t="s">
+      <c r="H96" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A96)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="B97" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C99">
+      <c r="C97" s="19">
         <f t="shared" si="16"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D99">
+      <c r="D97" s="19">
         <f t="shared" si="17"/>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G97" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H99" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A99)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>275</v>
-      </c>
-      <c r="B100" t="s">
+      <c r="H97" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A97)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="B98" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C100">
+      <c r="C98" s="19">
         <f t="shared" si="16"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D100">
+      <c r="D98" s="19">
         <f t="shared" si="17"/>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G100" t="s">
+      <c r="G98" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H100" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A100)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>276</v>
-      </c>
-      <c r="B101" t="s">
+      <c r="H98" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A98)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="B99" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C101">
+      <c r="C99" s="19">
         <f t="shared" si="16"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D101">
+      <c r="D99" s="19">
         <f t="shared" si="17"/>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G101" t="s">
+      <c r="G99" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H101" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A101)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>277</v>
-      </c>
-      <c r="B102" t="s">
+      <c r="H99" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A99)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="B100" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C102">
+      <c r="C100" s="19">
         <f t="shared" si="16"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D102">
+      <c r="D100" s="19">
         <f t="shared" si="17"/>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G102" t="s">
+      <c r="G100" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H102" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A102)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>278</v>
-      </c>
-      <c r="B103" t="s">
+      <c r="H100" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A100)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="B101" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C103">
+      <c r="C101" s="19">
         <f t="shared" si="16"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D103">
+      <c r="D101" s="19">
         <f t="shared" si="17"/>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G103" t="s">
+      <c r="G101" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H103" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A103)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>279</v>
-      </c>
-      <c r="B104" t="s">
+      <c r="H101" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A101)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="B102" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C104">
+      <c r="C102" s="19">
         <f t="shared" si="16"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D104">
+      <c r="D102" s="19">
         <f t="shared" si="17"/>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G104" t="s">
+      <c r="G102" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H104" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A104)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>280</v>
-      </c>
-      <c r="B105" t="s">
+      <c r="H102" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A102)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="B103" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C105">
+      <c r="C103" s="19">
         <f t="shared" si="16"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D105">
+      <c r="D103" s="19">
         <f t="shared" si="17"/>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G105" t="s">
+      <c r="G103" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H105" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A105)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>281</v>
-      </c>
-      <c r="B106" t="s">
+      <c r="H103" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A103)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="B104" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C106">
+      <c r="C104" s="19">
         <f t="shared" si="16"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D106">
+      <c r="D104" s="19">
         <f t="shared" si="17"/>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G106" t="s">
+      <c r="G104" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H106" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A106)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>282</v>
-      </c>
-      <c r="B107" t="s">
+      <c r="H104" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A104)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="B105" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C107">
+      <c r="C105" s="19">
         <f t="shared" si="16"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D107">
+      <c r="D105" s="19">
         <f t="shared" si="17"/>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G107" t="s">
+      <c r="G105" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H107" t="b">
-        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A107)&gt;0,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>264</v>
-      </c>
-      <c r="B108" t="s">
+      <c r="H105" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A105)&gt;0,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="B106" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C108">
+      <c r="C106" s="19">
         <v>1000</v>
       </c>
-      <c r="D108">
+      <c r="D106" s="19">
         <f t="shared" si="17"/>
         <v>10</v>
       </c>
-      <c r="G108" t="s">
+      <c r="G106" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H108" t="b">
+      <c r="H106" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A106)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="B107" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C107" s="19">
+        <v>1000</v>
+      </c>
+      <c r="D107" s="19">
+        <f t="shared" ref="D107:D108" si="18">C107*0.01</f>
+        <v>10</v>
+      </c>
+      <c r="G107" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H107" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A107)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="B108" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C108" s="19">
+        <v>0</v>
+      </c>
+      <c r="D108" s="19">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G108" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H108" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A108)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="A109" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C109">
-        <v>1000</v>
-      </c>
-      <c r="D109">
-        <f t="shared" ref="D109:D110" si="18">C109*0.01</f>
-        <v>10</v>
-      </c>
-      <c r="G109" t="s">
-        <v>12</v>
-      </c>
-      <c r="H109" t="b">
+      <c r="C109" s="19">
+        <v>0</v>
+      </c>
+      <c r="D109" s="19">
+        <f t="shared" ref="D109:D110" si="19">C109*0.01</f>
+        <v>0</v>
+      </c>
+      <c r="G109" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H109" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A109)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>264</v>
-      </c>
-      <c r="B110" t="s">
-        <v>65</v>
-      </c>
-      <c r="C110">
-        <v>0</v>
-      </c>
-      <c r="D110">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="G110" t="s">
-        <v>283</v>
-      </c>
-      <c r="H110" t="b">
+        <v>302</v>
+      </c>
+      <c r="B110" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="C110" s="19">
+        <v>1000</v>
+      </c>
+      <c r="D110" s="19">
+        <f t="shared" si="19"/>
+        <v>10</v>
+      </c>
+      <c r="E110" s="19">
+        <v>0</v>
+      </c>
+      <c r="F110" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="G110" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H110" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A110)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>195</v>
-      </c>
-      <c r="B111" t="s">
-        <v>65</v>
-      </c>
-      <c r="C111">
-        <v>0</v>
-      </c>
-      <c r="D111">
-        <f t="shared" ref="D111" si="19">C111*0.01</f>
-        <v>0</v>
-      </c>
-      <c r="G111" t="s">
-        <v>283</v>
-      </c>
-      <c r="H111" t="b">
+        <v>303</v>
+      </c>
+      <c r="B111" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="C111" s="19">
+        <v>1000</v>
+      </c>
+      <c r="D111" s="19">
+        <f t="shared" ref="D111:D113" si="20">C111*0.01</f>
+        <v>10</v>
+      </c>
+      <c r="E111" s="19">
+        <v>0</v>
+      </c>
+      <c r="F111" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="G111" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H111" s="19" t="b">
         <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A111)&gt;0,FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>304</v>
+      </c>
+      <c r="B112" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="C112" s="19">
+        <v>1000</v>
+      </c>
+      <c r="D112" s="19">
+        <f t="shared" si="20"/>
+        <v>10</v>
+      </c>
+      <c r="E112" s="19">
+        <v>0</v>
+      </c>
+      <c r="F112" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="G112" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H112" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A112)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>302</v>
+      </c>
+      <c r="B113" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="C113" s="19">
+        <v>1000</v>
+      </c>
+      <c r="D113" s="19">
+        <f t="shared" si="20"/>
+        <v>10</v>
+      </c>
+      <c r="E113" s="19">
+        <v>0</v>
+      </c>
+      <c r="F113" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="G113" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H113" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A113)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>303</v>
+      </c>
+      <c r="B114" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="C114" s="19">
+        <v>1000</v>
+      </c>
+      <c r="D114" s="19">
+        <f t="shared" ref="D114:D115" si="21">C114*0.01</f>
+        <v>10</v>
+      </c>
+      <c r="E114" s="19">
+        <v>0</v>
+      </c>
+      <c r="F114" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="G114" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H114" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A114)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>304</v>
+      </c>
+      <c r="B115" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="C115" s="19">
+        <v>1000</v>
+      </c>
+      <c r="D115" s="19">
+        <f t="shared" si="21"/>
+        <v>10</v>
+      </c>
+      <c r="E115" s="19">
+        <v>0</v>
+      </c>
+      <c r="F115" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="G115" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H115" s="19" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A115)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G54" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A1:G53" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -6257,87 +6408,87 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -6362,13 +6513,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6398,7 +6549,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -6410,7 +6561,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -6422,7 +6573,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -6434,7 +6585,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6455,7 +6606,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6467,7 +6618,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -6479,7 +6630,7 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -6491,7 +6642,7 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -6503,7 +6654,7 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -6598,7 +6749,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B24" t="b">
         <f>FALSE</f>
@@ -6607,7 +6758,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B25" t="b">
         <f>FALSE</f>
@@ -6622,10 +6773,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E230"/>
+  <dimension ref="A1:E228"/>
   <sheetViews>
-    <sheetView topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="B155" sqref="B155:B156"/>
+    <sheetView topLeftCell="A203" workbookViewId="0">
+      <selection activeCell="B215" sqref="B215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6648,10 +6799,10 @@
         <v>79</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6699,7 +6850,7 @@
         <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C4" t="b">
         <f>TRUE</f>
@@ -6719,7 +6870,7 @@
         <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C5" t="b">
         <f>TRUE</f>
@@ -6739,7 +6890,7 @@
         <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C6" t="b">
         <f>TRUE</f>
@@ -6759,7 +6910,7 @@
         <v>101</v>
       </c>
       <c r="B7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C7" t="b">
         <f>TRUE</f>
@@ -6779,7 +6930,7 @@
         <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C8" t="b">
         <f>TRUE</f>
@@ -6799,7 +6950,7 @@
         <v>101</v>
       </c>
       <c r="B9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C9" t="b">
         <f>TRUE</f>
@@ -6819,7 +6970,7 @@
         <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C10" t="b">
         <f>TRUE</f>
@@ -6839,7 +6990,7 @@
         <v>101</v>
       </c>
       <c r="B11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C11" t="b">
         <f>TRUE</f>
@@ -6859,7 +7010,7 @@
         <v>101</v>
       </c>
       <c r="B12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C12" t="b">
         <f>TRUE</f>
@@ -6879,7 +7030,7 @@
         <v>101</v>
       </c>
       <c r="B13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C13" t="b">
         <f>TRUE</f>
@@ -6899,7 +7050,7 @@
         <v>101</v>
       </c>
       <c r="B14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C14" t="b">
         <f>TRUE</f>
@@ -6919,7 +7070,7 @@
         <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C15" t="b">
         <f>TRUE</f>
@@ -6939,7 +7090,7 @@
         <v>101</v>
       </c>
       <c r="B16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C16" t="b">
         <f>TRUE</f>
@@ -6959,7 +7110,7 @@
         <v>101</v>
       </c>
       <c r="B17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C17" t="b">
         <f>TRUE</f>
@@ -6979,7 +7130,7 @@
         <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C18" t="b">
         <f>TRUE</f>
@@ -6999,7 +7150,7 @@
         <v>101</v>
       </c>
       <c r="B19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C19" t="b">
         <f>TRUE</f>
@@ -9739,7 +9890,7 @@
         <v>198</v>
       </c>
       <c r="B156" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C156" t="b">
         <f>TRUE</f>
@@ -10778,7 +10929,7 @@
         <v>254</v>
       </c>
       <c r="B208" t="s">
-        <v>255</v>
+        <v>302</v>
       </c>
       <c r="C208" t="b">
         <f>TRUE</f>
@@ -10798,7 +10949,7 @@
         <v>254</v>
       </c>
       <c r="B209" t="s">
-        <v>256</v>
+        <v>303</v>
       </c>
       <c r="C209" t="b">
         <f>TRUE</f>
@@ -10895,10 +11046,10 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="B214" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C214" t="b">
         <f>TRUE</f>
@@ -10915,10 +11066,10 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B215" t="s">
-        <v>260</v>
+        <v>304</v>
       </c>
       <c r="C215" t="b">
         <f>TRUE</f>
@@ -10935,10 +11086,10 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B216" t="s">
-        <v>261</v>
+        <v>117</v>
       </c>
       <c r="C216" t="b">
         <f>TRUE</f>
@@ -10955,10 +11106,10 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B217" t="s">
-        <v>257</v>
+        <v>118</v>
       </c>
       <c r="C217" t="b">
         <f>TRUE</f>
@@ -10975,14 +11126,14 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>262</v>
+        <v>285</v>
       </c>
       <c r="B218" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C218" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D218" t="b">
         <f>VLOOKUP(A218,Módulos!A:B,2,FALSE)</f>
@@ -10990,19 +11141,19 @@
       </c>
       <c r="E218" t="str">
         <f>IF(C218,"Nenhuma",VLOOKUP(B218,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_beneficios_inss</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>262</v>
+        <v>285</v>
       </c>
       <c r="B219" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C219" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D219" t="b">
         <f>VLOOKUP(A219,Módulos!A:B,2,FALSE)</f>
@@ -11010,15 +11161,15 @@
       </c>
       <c r="E219" t="str">
         <f>IF(C219,"Nenhuma",VLOOKUP(B219,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
+        <v>calcular_beneficios_inss</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B220" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C220" t="b">
         <f>FALSE</f>
@@ -11035,10 +11186,10 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B221" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C221" t="b">
         <f>FALSE</f>
@@ -11055,14 +11206,14 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B222" t="s">
-        <v>128</v>
+        <v>240</v>
       </c>
       <c r="C222" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D222" t="b">
         <f>VLOOKUP(A222,Módulos!A:B,2,FALSE)</f>
@@ -11070,19 +11221,19 @@
       </c>
       <c r="E222" t="str">
         <f>IF(C222,"Nenhuma",VLOOKUP(B222,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_beneficios_inss</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B223" t="s">
-        <v>129</v>
+        <v>241</v>
       </c>
       <c r="C223" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="D223" t="b">
         <f>VLOOKUP(A223,Módulos!A:B,2,FALSE)</f>
@@ -11090,15 +11241,15 @@
       </c>
       <c r="E223" t="str">
         <f>IF(C223,"Nenhuma",VLOOKUP(B223,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>calcular_beneficios_inss</v>
+        <v>Nenhuma</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B224" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C224" t="b">
         <f>TRUE</f>
@@ -11115,10 +11266,10 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B225" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C225" t="b">
         <f>TRUE</f>
@@ -11135,10 +11286,10 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B226" t="s">
-        <v>242</v>
+        <v>2</v>
       </c>
       <c r="C226" t="b">
         <f>TRUE</f>
@@ -11155,10 +11306,10 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B227" t="s">
-        <v>243</v>
+        <v>1</v>
       </c>
       <c r="C227" t="b">
         <f>TRUE</f>
@@ -11175,14 +11326,14 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B228" t="s">
-        <v>2</v>
+        <v>175</v>
       </c>
       <c r="C228" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="D228" t="b">
         <f>VLOOKUP(A228,Módulos!A:B,2,FALSE)</f>
@@ -11190,51 +11341,11 @@
       </c>
       <c r="E228" t="str">
         <f>IF(C228,"Nenhuma",VLOOKUP(B228,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
-        <v>286</v>
-      </c>
-      <c r="B229" t="s">
-        <v>1</v>
-      </c>
-      <c r="C229" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="D229" t="b">
-        <f>VLOOKUP(A229,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="E229" t="str">
-        <f>IF(C229,"Nenhuma",VLOOKUP(B229,Funcoes_Outputs!B:D,3,FALSE))</f>
-        <v>Nenhuma</v>
-      </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>286</v>
-      </c>
-      <c r="B230" t="s">
-        <v>175</v>
-      </c>
-      <c r="C230" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="D230" t="b">
-        <f>VLOOKUP(A230,Módulos!A:B,2,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="E230" t="str">
-        <f>IF(C230,"Nenhuma",VLOOKUP(B230,Funcoes_Outputs!B:D,3,FALSE))</f>
         <v>calcular_turnovergeral</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E219" xr:uid="{D8C2AD8A-D29B-4ECE-B686-2DDAE10A4D17}"/>
+  <autoFilter ref="A1:E217" xr:uid="{D8C2AD8A-D29B-4ECE-B686-2DDAE10A4D17}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Poisson: Ajuste realizado para prever variáveis não relativizadas
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="295">
   <si>
     <t>Ano</t>
   </si>
@@ -958,6 +958,9 @@
   </si>
   <si>
     <t>poisson</t>
+  </si>
+  <si>
+    <t>poisson_percentual_eventos</t>
   </si>
 </sst>
 </file>
@@ -2812,7 +2815,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3734,14 +3739,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="20" customWidth="1"/>
     <col min="5" max="6" width="13.5703125" style="20" bestFit="1" customWidth="1"/>
@@ -4528,15 +4531,12 @@
       <c r="A36" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="B36" s="20" t="s">
-        <v>49</v>
+      <c r="B36" s="17" t="s">
+        <v>293</v>
       </c>
       <c r="C36" s="20">
-        <v>2</v>
-      </c>
-      <c r="D36" s="20">
-        <f t="shared" ref="D36:D37" si="12">C36*0.01</f>
-        <v>0.02</v>
+        <f>1/10</f>
+        <v>0.1</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>266</v>
@@ -4557,7 +4557,7 @@
         <v>10</v>
       </c>
       <c r="D37" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="D36:D37" si="12">C37*0.01</f>
         <v>0.1</v>
       </c>
       <c r="G37" s="20" t="s">
@@ -4661,7 +4661,7 @@
         <v>254</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C42" s="20">
         <f>1/20</f>
@@ -5669,15 +5669,12 @@
       <c r="A88" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="B88" s="20" t="s">
-        <v>49</v>
+      <c r="B88" s="17" t="s">
+        <v>293</v>
       </c>
       <c r="C88" s="20">
-        <v>1</v>
-      </c>
-      <c r="D88" s="20">
-        <f t="shared" si="15"/>
-        <v>0.01</v>
+        <f>1/10</f>
+        <v>0.1</v>
       </c>
       <c r="G88" s="20" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Verificação Inicial de Inputs está configurada.
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -945,7 +945,7 @@
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1025,6 +1025,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1049,7 +1064,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1090,6 +1105,13 @@
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -1413,50 +1435,51 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="28" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="26" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="28">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="28">
         <v>200</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="26">
         <v>2017</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="27">
         <f>AVERAGE(Dados_Projetados!B1:B10)</f>
         <v>3000</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="27">
         <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C3" s="1"/>
+      <c r="C3" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Criado arquivo de teste
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="749" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="749" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ParametrosSemSeedFixa" sheetId="33" state="hidden" r:id="rId1"/>
@@ -18199,8 +18199,8 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19056,14 +19056,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:M325"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="E333" sqref="E333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19121,7 +19121,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="72" t="s">
         <v>72</v>
       </c>
@@ -19159,7 +19159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="72" t="s">
         <v>76</v>
       </c>
@@ -19204,7 +19204,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="72" t="s">
         <v>89</v>
       </c>
@@ -19238,7 +19238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="72" t="s">
         <v>86</v>
       </c>
@@ -19280,7 +19280,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="72" t="s">
         <v>110</v>
       </c>
@@ -19314,7 +19314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="72" t="s">
         <v>115</v>
       </c>
@@ -19356,7 +19356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="72" t="s">
         <v>117</v>
       </c>
@@ -19391,7 +19391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="72" t="s">
         <v>122</v>
       </c>
@@ -19426,7 +19426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="72" t="s">
         <v>144</v>
       </c>
@@ -19460,7 +19460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="72" t="s">
         <v>145</v>
       </c>
@@ -19494,7 +19494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="72" t="s">
         <v>158</v>
       </c>
@@ -19529,7 +19529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="72" t="s">
         <v>159</v>
       </c>
@@ -19564,7 +19564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="72" t="s">
         <v>165</v>
       </c>
@@ -19599,7 +19599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="72" t="s">
         <v>175</v>
       </c>
@@ -19633,7 +19633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="72" t="s">
         <v>179</v>
       </c>
@@ -19667,7 +19667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="72" t="s">
         <v>84</v>
       </c>
@@ -19700,7 +19700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="72" t="s">
         <v>191</v>
       </c>
@@ -19733,7 +19733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="72" t="s">
         <v>192</v>
       </c>
@@ -19766,7 +19766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="72" t="s">
         <v>193</v>
       </c>
@@ -19799,7 +19799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="72" t="s">
         <v>194</v>
       </c>
@@ -19832,7 +19832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="72" t="s">
         <v>182</v>
       </c>
@@ -19865,7 +19865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="72" t="s">
         <v>187</v>
       </c>
@@ -19898,7 +19898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="72" t="s">
         <v>188</v>
       </c>
@@ -19931,7 +19931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="72" t="s">
         <v>189</v>
       </c>
@@ -19964,7 +19964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="72" t="s">
         <v>190</v>
       </c>
@@ -19997,7 +19997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="72" t="s">
         <v>81</v>
       </c>
@@ -20030,7 +20030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="72" t="s">
         <v>183</v>
       </c>
@@ -20063,7 +20063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="72" t="s">
         <v>184</v>
       </c>
@@ -20096,7 +20096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="72" t="s">
         <v>185</v>
       </c>
@@ -20129,7 +20129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="72" t="s">
         <v>186</v>
       </c>
@@ -20162,7 +20162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="72" t="s">
         <v>226</v>
       </c>
@@ -20199,7 +20199,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="72" t="s">
         <v>206</v>
       </c>
@@ -20239,7 +20239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="72" t="s">
         <v>207</v>
       </c>
@@ -20279,7 +20279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="72" t="s">
         <v>208</v>
       </c>
@@ -20319,7 +20319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="72" t="s">
         <v>209</v>
       </c>
@@ -20359,7 +20359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="72" t="s">
         <v>241</v>
       </c>
@@ -20400,7 +20400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="72" t="s">
         <v>245</v>
       </c>
@@ -20441,7 +20441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="72" t="s">
         <v>233</v>
       </c>
@@ -20482,23 +20482,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="72" t="s">
         <v>237</v>
       </c>
-      <c r="B40" s="72" t="s">
-        <v>466</v>
+      <c r="B40" s="37" t="s">
+        <v>501</v>
       </c>
       <c r="C40" s="72">
         <f>1/20</f>
         <v>0.05</v>
       </c>
-      <c r="D40" s="72">
-        <v>0</v>
-      </c>
-      <c r="E40" s="75">
-        <v>1.0869565217391304E-3</v>
-      </c>
+      <c r="E40" s="75"/>
       <c r="G40" s="72" t="s">
         <v>249</v>
       </c>
@@ -20508,7 +20503,7 @@
       </c>
       <c r="I40" s="72" t="str">
         <f t="shared" si="0"/>
-        <v>Dados Incorretos</v>
+        <v>OK</v>
       </c>
       <c r="J40" s="72" t="str">
         <f>VLOOKUP(B40,Distribuições!$A$1:$F$13,6,FALSE)</f>
@@ -20519,7 +20514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="72" t="s">
         <v>242</v>
       </c>
@@ -20560,7 +20555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="72" t="s">
         <v>246</v>
       </c>
@@ -20601,7 +20596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="72" t="s">
         <v>234</v>
       </c>
@@ -20642,7 +20637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="72" t="s">
         <v>238</v>
       </c>
@@ -20683,7 +20678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="72" t="s">
         <v>243</v>
       </c>
@@ -20724,7 +20719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="72" t="s">
         <v>247</v>
       </c>
@@ -20765,7 +20760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="72" t="s">
         <v>235</v>
       </c>
@@ -20806,7 +20801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="72" t="s">
         <v>239</v>
       </c>
@@ -20847,7 +20842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="72" t="s">
         <v>244</v>
       </c>
@@ -20888,7 +20883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="72" t="s">
         <v>248</v>
       </c>
@@ -20929,7 +20924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="72" t="s">
         <v>236</v>
       </c>
@@ -20970,7 +20965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="72" t="s">
         <v>240</v>
       </c>
@@ -21011,7 +21006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="72" t="s">
         <v>52</v>
       </c>
@@ -21053,7 +21048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="72" t="s">
         <v>150</v>
       </c>
@@ -21087,7 +21082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="72" t="s">
         <v>151</v>
       </c>
@@ -21121,7 +21116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="72" t="s">
         <v>152</v>
       </c>
@@ -21155,7 +21150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="72" t="s">
         <v>167</v>
       </c>
@@ -21189,7 +21184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="72" t="s">
         <v>170</v>
       </c>
@@ -21223,7 +21218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="72" t="s">
         <v>168</v>
       </c>
@@ -21257,7 +21252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="72" t="s">
         <v>169</v>
       </c>
@@ -21291,7 +21286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="72" t="s">
         <v>171</v>
       </c>
@@ -21325,7 +21320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="72" t="s">
         <v>211</v>
       </c>
@@ -21364,7 +21359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="72" t="s">
         <v>215</v>
       </c>
@@ -21398,7 +21393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="72" t="s">
         <v>210</v>
       </c>
@@ -21432,7 +21427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="72" t="s">
         <v>212</v>
       </c>
@@ -21466,7 +21461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="72" t="s">
         <v>213</v>
       </c>
@@ -21500,7 +21495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="72" t="s">
         <v>214</v>
       </c>
@@ -21534,7 +21529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="72" t="s">
         <v>129</v>
       </c>
@@ -21568,7 +21563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="72" t="s">
         <v>132</v>
       </c>
@@ -21602,7 +21597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="72" t="s">
         <v>130</v>
       </c>
@@ -21636,7 +21631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="72" t="s">
         <v>131</v>
       </c>
@@ -21670,7 +21665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="72" t="s">
         <v>72</v>
       </c>
@@ -21703,7 +21698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="72" t="s">
         <v>76</v>
       </c>
@@ -21748,7 +21743,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="74" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="72" t="s">
         <v>89</v>
       </c>
@@ -21781,7 +21776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="72" t="s">
         <v>86</v>
       </c>
@@ -21823,7 +21818,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="76" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="72" t="s">
         <v>110</v>
       </c>
@@ -21856,7 +21851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="72" t="s">
         <v>115</v>
       </c>
@@ -21896,7 +21891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="72" t="s">
         <v>117</v>
       </c>
@@ -21929,7 +21924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="72" t="s">
         <v>122</v>
       </c>
@@ -21962,7 +21957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="72" t="s">
         <v>144</v>
       </c>
@@ -21995,7 +21990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="72" t="s">
         <v>145</v>
       </c>
@@ -22028,7 +22023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="72" t="s">
         <v>158</v>
       </c>
@@ -22061,7 +22056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="72" t="s">
         <v>159</v>
       </c>
@@ -22094,7 +22089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="72" t="s">
         <v>165</v>
       </c>
@@ -22127,7 +22122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="72" t="s">
         <v>175</v>
       </c>
@@ -22160,7 +22155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="72" t="s">
         <v>179</v>
       </c>
@@ -22193,7 +22188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="72" t="s">
         <v>84</v>
       </c>
@@ -22226,7 +22221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="72" t="s">
         <v>191</v>
       </c>
@@ -22259,7 +22254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="72" t="s">
         <v>192</v>
       </c>
@@ -22292,7 +22287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="72" t="s">
         <v>193</v>
       </c>
@@ -22325,7 +22320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="72" t="s">
         <v>194</v>
       </c>
@@ -22358,7 +22353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="72" t="s">
         <v>182</v>
       </c>
@@ -22391,7 +22386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="72" t="s">
         <v>187</v>
       </c>
@@ -22424,7 +22419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="72" t="s">
         <v>188</v>
       </c>
@@ -22457,7 +22452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="72" t="s">
         <v>189</v>
       </c>
@@ -22490,7 +22485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="72" t="s">
         <v>190</v>
       </c>
@@ -22523,7 +22518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="72" t="s">
         <v>81</v>
       </c>
@@ -22556,7 +22551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="72" t="s">
         <v>183</v>
       </c>
@@ -22589,7 +22584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="72" t="s">
         <v>184</v>
       </c>
@@ -22622,7 +22617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="72" t="s">
         <v>185</v>
       </c>
@@ -22655,7 +22650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="72" t="s">
         <v>186</v>
       </c>
@@ -22688,7 +22683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="72" t="s">
         <v>226</v>
       </c>
@@ -22725,7 +22720,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="103" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="72" t="s">
         <v>206</v>
       </c>
@@ -22765,7 +22760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="72" t="s">
         <v>207</v>
       </c>
@@ -22805,7 +22800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="72" t="s">
         <v>208</v>
       </c>
@@ -22845,7 +22840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="72" t="s">
         <v>209</v>
       </c>
@@ -22885,7 +22880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="72" t="s">
         <v>241</v>
       </c>
@@ -22924,7 +22919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="72" t="s">
         <v>245</v>
       </c>
@@ -22963,7 +22958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="72" t="s">
         <v>233</v>
       </c>
@@ -23002,23 +22997,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="72" t="s">
         <v>237</v>
       </c>
-      <c r="B110" s="72" t="s">
-        <v>466</v>
+      <c r="B110" s="37" t="s">
+        <v>501</v>
       </c>
       <c r="C110" s="72">
         <f>1/40</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D110" s="72">
-        <v>0</v>
-      </c>
-      <c r="E110" s="72">
-        <v>1.0869565217391304E-3</v>
-      </c>
       <c r="G110" s="72" t="s">
         <v>10</v>
       </c>
@@ -23028,7 +23017,7 @@
       </c>
       <c r="I110" s="72" t="str">
         <f t="shared" si="7"/>
-        <v>Dados Incorretos</v>
+        <v>OK</v>
       </c>
       <c r="J110" s="72" t="str">
         <f>VLOOKUP(B110,Distribuições!$A$1:$F$13,6,FALSE)</f>
@@ -23039,7 +23028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="72" t="s">
         <v>242</v>
       </c>
@@ -23078,7 +23067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="72" t="s">
         <v>246</v>
       </c>
@@ -23117,7 +23106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="72" t="s">
         <v>234</v>
       </c>
@@ -23156,7 +23145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="72" t="s">
         <v>238</v>
       </c>
@@ -23195,7 +23184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="72" t="s">
         <v>243</v>
       </c>
@@ -23234,7 +23223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="72" t="s">
         <v>247</v>
       </c>
@@ -23273,7 +23262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="72" t="s">
         <v>235</v>
       </c>
@@ -23312,7 +23301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="72" t="s">
         <v>239</v>
       </c>
@@ -23351,7 +23340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="72" t="s">
         <v>244</v>
       </c>
@@ -23390,7 +23379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="72" t="s">
         <v>248</v>
       </c>
@@ -23429,7 +23418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="72" t="s">
         <v>236</v>
       </c>
@@ -23473,7 +23462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="72" t="s">
         <v>240</v>
       </c>
@@ -23512,7 +23501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="72" t="s">
         <v>52</v>
       </c>
@@ -23552,7 +23541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="72" t="s">
         <v>150</v>
       </c>
@@ -23585,7 +23574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="72" t="s">
         <v>151</v>
       </c>
@@ -23618,7 +23607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="72" t="s">
         <v>152</v>
       </c>
@@ -23651,7 +23640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="72" t="s">
         <v>167</v>
       </c>
@@ -23684,7 +23673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="72" t="s">
         <v>170</v>
       </c>
@@ -23717,7 +23706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="72" t="s">
         <v>168</v>
       </c>
@@ -23750,7 +23739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="72" t="s">
         <v>169</v>
       </c>
@@ -23783,7 +23772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="72" t="s">
         <v>171</v>
       </c>
@@ -23816,7 +23805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="72" t="s">
         <v>211</v>
       </c>
@@ -23849,7 +23838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="72" t="s">
         <v>215</v>
       </c>
@@ -23882,7 +23871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="72" t="s">
         <v>210</v>
       </c>
@@ -23915,7 +23904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="72" t="s">
         <v>212</v>
       </c>
@@ -23948,7 +23937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="72" t="s">
         <v>213</v>
       </c>
@@ -23981,7 +23970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="72" t="s">
         <v>214</v>
       </c>
@@ -24014,7 +24003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="72" t="s">
         <v>129</v>
       </c>
@@ -24047,7 +24036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="72" t="s">
         <v>132</v>
       </c>
@@ -24080,7 +24069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="72" t="s">
         <v>130</v>
       </c>
@@ -24113,7 +24102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="72" t="s">
         <v>131</v>
       </c>
@@ -24146,7 +24135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="72" t="s">
         <v>72</v>
       </c>
@@ -24179,7 +24168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="72" t="s">
         <v>76</v>
       </c>
@@ -24224,7 +24213,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="144" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="72" t="s">
         <v>89</v>
       </c>
@@ -24257,7 +24246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="72" t="s">
         <v>86</v>
       </c>
@@ -24299,7 +24288,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="146" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="72" t="s">
         <v>110</v>
       </c>
@@ -24332,7 +24321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="72" t="s">
         <v>115</v>
       </c>
@@ -24372,7 +24361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="72" t="s">
         <v>117</v>
       </c>
@@ -24405,7 +24394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="72" t="s">
         <v>122</v>
       </c>
@@ -24438,7 +24427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="72" t="s">
         <v>144</v>
       </c>
@@ -24471,7 +24460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="72" t="s">
         <v>145</v>
       </c>
@@ -24504,7 +24493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="72" t="s">
         <v>158</v>
       </c>
@@ -24537,7 +24526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="72" t="s">
         <v>159</v>
       </c>
@@ -24570,7 +24559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="72" t="s">
         <v>165</v>
       </c>
@@ -24603,7 +24592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="72" t="s">
         <v>175</v>
       </c>
@@ -24636,7 +24625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="72" t="s">
         <v>179</v>
       </c>
@@ -24669,7 +24658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="72" t="s">
         <v>84</v>
       </c>
@@ -24702,7 +24691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="72" t="s">
         <v>191</v>
       </c>
@@ -24735,7 +24724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="72" t="s">
         <v>192</v>
       </c>
@@ -24768,7 +24757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="72" t="s">
         <v>193</v>
       </c>
@@ -24801,7 +24790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="72" t="s">
         <v>194</v>
       </c>
@@ -24834,7 +24823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="72" t="s">
         <v>182</v>
       </c>
@@ -24867,7 +24856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="72" t="s">
         <v>187</v>
       </c>
@@ -24900,7 +24889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="72" t="s">
         <v>188</v>
       </c>
@@ -24933,7 +24922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="72" t="s">
         <v>189</v>
       </c>
@@ -24966,7 +24955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="72" t="s">
         <v>190</v>
       </c>
@@ -24999,7 +24988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="72" t="s">
         <v>81</v>
       </c>
@@ -25032,7 +25021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="72" t="s">
         <v>183</v>
       </c>
@@ -25065,7 +25054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="72" t="s">
         <v>184</v>
       </c>
@@ -25098,7 +25087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="72" t="s">
         <v>185</v>
       </c>
@@ -25131,7 +25120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="72" t="s">
         <v>186</v>
       </c>
@@ -25164,7 +25153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="72" t="s">
         <v>226</v>
       </c>
@@ -25201,7 +25190,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="173" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="72" t="s">
         <v>206</v>
       </c>
@@ -25241,7 +25230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="72" t="s">
         <v>207</v>
       </c>
@@ -25281,7 +25270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="72" t="s">
         <v>208</v>
       </c>
@@ -25321,7 +25310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="72" t="s">
         <v>209</v>
       </c>
@@ -25361,7 +25350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="72" t="s">
         <v>241</v>
       </c>
@@ -25400,7 +25389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="72" t="s">
         <v>245</v>
       </c>
@@ -25439,7 +25428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="72" t="s">
         <v>233</v>
       </c>
@@ -25478,25 +25467,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:11" s="72" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" s="72" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="72" t="s">
         <v>237</v>
       </c>
-      <c r="B180" s="72" t="s">
-        <v>466</v>
+      <c r="B180" s="37" t="s">
+        <v>501</v>
       </c>
       <c r="C180" s="72">
         <f>1/20</f>
         <v>0.05</v>
-      </c>
-      <c r="D180" s="72">
-        <v>0</v>
-      </c>
-      <c r="E180" s="72">
-        <v>0</v>
-      </c>
-      <c r="F180" s="72">
-        <v>1</v>
       </c>
       <c r="G180" s="72" t="s">
         <v>21</v>
@@ -25512,7 +25492,7 @@
 IF(AND(B180="normaltruncada",NOT(COUNT(C180:F180)=4)),"Dados Incorretos",
 IF(AND(B180="uniforme",NOT(COUNT(C180:D180)=2)),"Dados Incorretos",
 IF(AND(B180="poisson_percentual_eventos",NOT(COUNT(C180:D180)=1)),"Dados Incorretos","OK"))))))</f>
-        <v>Dados Incorretos</v>
+        <v>OK</v>
       </c>
       <c r="J180" s="72" t="str">
         <f>VLOOKUP(B180,Distribuições!$A$1:$F$13,6,FALSE)</f>
@@ -25523,7 +25503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="72" t="s">
         <v>242</v>
       </c>
@@ -25562,7 +25542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="72" t="s">
         <v>246</v>
       </c>
@@ -25601,7 +25581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="72" t="s">
         <v>234</v>
       </c>
@@ -25640,7 +25620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="72" t="s">
         <v>238</v>
       </c>
@@ -25679,7 +25659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="72" t="s">
         <v>243</v>
       </c>
@@ -25718,7 +25698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="72" t="s">
         <v>247</v>
       </c>
@@ -25757,7 +25737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="72" t="s">
         <v>235</v>
       </c>
@@ -25796,7 +25776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="72" t="s">
         <v>239</v>
       </c>
@@ -25835,7 +25815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="72" t="s">
         <v>244</v>
       </c>
@@ -25874,7 +25854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="72" t="s">
         <v>248</v>
       </c>
@@ -25913,7 +25893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="72" t="s">
         <v>236</v>
       </c>
@@ -25952,7 +25932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="72" t="s">
         <v>240</v>
       </c>
@@ -25991,7 +25971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="72" t="s">
         <v>52</v>
       </c>
@@ -26031,7 +26011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="72" t="s">
         <v>150</v>
       </c>
@@ -26064,7 +26044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="72" t="s">
         <v>151</v>
       </c>
@@ -26097,7 +26077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="72" t="s">
         <v>152</v>
       </c>
@@ -26130,7 +26110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" s="72" t="s">
         <v>167</v>
       </c>
@@ -26163,7 +26143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" s="72" t="s">
         <v>170</v>
       </c>
@@ -26196,7 +26176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="72" t="s">
         <v>168</v>
       </c>
@@ -26229,7 +26209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" s="72" t="s">
         <v>169</v>
       </c>
@@ -26262,7 +26242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" s="72" t="s">
         <v>171</v>
       </c>
@@ -26295,7 +26275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" s="72" t="s">
         <v>211</v>
       </c>
@@ -26328,7 +26308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" s="72" t="s">
         <v>215</v>
       </c>
@@ -26361,7 +26341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" s="72" t="s">
         <v>210</v>
       </c>
@@ -26394,7 +26374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" s="72" t="s">
         <v>212</v>
       </c>
@@ -26427,7 +26407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" s="72" t="s">
         <v>213</v>
       </c>
@@ -26460,7 +26440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" s="72" t="s">
         <v>214</v>
       </c>
@@ -26493,7 +26473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" s="72" t="s">
         <v>129</v>
       </c>
@@ -26526,7 +26506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" s="72" t="s">
         <v>132</v>
       </c>
@@ -26559,7 +26539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="72" t="s">
         <v>130</v>
       </c>
@@ -26592,7 +26572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" s="72" t="s">
         <v>131</v>
       </c>
@@ -26625,7 +26605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" s="72" t="s">
         <v>72</v>
       </c>
@@ -26658,7 +26638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" s="72" t="s">
         <v>76</v>
       </c>
@@ -26703,7 +26683,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="214" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" s="72" t="s">
         <v>89</v>
       </c>
@@ -26736,7 +26716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" s="72" t="s">
         <v>86</v>
       </c>
@@ -26778,7 +26758,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="216" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" s="72" t="s">
         <v>110</v>
       </c>
@@ -26811,7 +26791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" s="72" t="s">
         <v>115</v>
       </c>
@@ -26851,7 +26831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" s="72" t="s">
         <v>117</v>
       </c>
@@ -26884,7 +26864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" s="72" t="s">
         <v>122</v>
       </c>
@@ -26917,7 +26897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" s="72" t="s">
         <v>144</v>
       </c>
@@ -26950,7 +26930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" s="72" t="s">
         <v>145</v>
       </c>
@@ -26983,7 +26963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" s="72" t="s">
         <v>158</v>
       </c>
@@ -27016,7 +26996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" s="72" t="s">
         <v>159</v>
       </c>
@@ -27049,7 +27029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" s="72" t="s">
         <v>165</v>
       </c>
@@ -27082,7 +27062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" s="72" t="s">
         <v>175</v>
       </c>
@@ -27115,7 +27095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" s="72" t="s">
         <v>179</v>
       </c>
@@ -27148,7 +27128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" s="72" t="s">
         <v>84</v>
       </c>
@@ -27181,7 +27161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" s="72" t="s">
         <v>191</v>
       </c>
@@ -27214,7 +27194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" s="72" t="s">
         <v>192</v>
       </c>
@@ -27247,7 +27227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" s="72" t="s">
         <v>193</v>
       </c>
@@ -27280,7 +27260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" s="72" t="s">
         <v>194</v>
       </c>
@@ -27313,7 +27293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" s="72" t="s">
         <v>182</v>
       </c>
@@ -27346,7 +27326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" s="72" t="s">
         <v>187</v>
       </c>
@@ -27379,7 +27359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" s="72" t="s">
         <v>188</v>
       </c>
@@ -27412,7 +27392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" s="72" t="s">
         <v>189</v>
       </c>
@@ -27445,7 +27425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" s="72" t="s">
         <v>190</v>
       </c>
@@ -27478,7 +27458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" s="72" t="s">
         <v>81</v>
       </c>
@@ -27511,7 +27491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" s="72" t="s">
         <v>183</v>
       </c>
@@ -27544,7 +27524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" s="72" t="s">
         <v>184</v>
       </c>
@@ -27577,7 +27557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" s="72" t="s">
         <v>185</v>
       </c>
@@ -27610,7 +27590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" s="72" t="s">
         <v>186</v>
       </c>
@@ -27643,7 +27623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" s="72" t="s">
         <v>226</v>
       </c>
@@ -27685,7 +27665,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="243" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" s="72" t="s">
         <v>206</v>
       </c>
@@ -27718,7 +27698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" s="72" t="s">
         <v>207</v>
       </c>
@@ -27751,7 +27731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" s="72" t="s">
         <v>208</v>
       </c>
@@ -27784,7 +27764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" s="72" t="s">
         <v>209</v>
       </c>
@@ -27817,7 +27797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" s="72" t="s">
         <v>241</v>
       </c>
@@ -27856,7 +27836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" s="72" t="s">
         <v>245</v>
       </c>
@@ -27895,7 +27875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" s="72" t="s">
         <v>233</v>
       </c>
@@ -27934,26 +27914,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:13" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A250" s="72" t="s">
         <v>237</v>
       </c>
-      <c r="B250" s="72" t="s">
-        <v>466</v>
+      <c r="B250" s="37" t="s">
+        <v>501</v>
       </c>
       <c r="C250" s="72">
         <f>1/20</f>
         <v>0.05</v>
       </c>
-      <c r="D250" s="72">
-        <v>0</v>
-      </c>
-      <c r="E250" s="72">
-        <v>0</v>
-      </c>
-      <c r="F250" s="72">
-        <v>1</v>
-      </c>
       <c r="G250" s="72" t="s">
         <v>22</v>
       </c>
@@ -27963,7 +27934,7 @@
       </c>
       <c r="I250" s="72" t="str">
         <f t="shared" si="12"/>
-        <v>Dados Incorretos</v>
+        <v>OK</v>
       </c>
       <c r="J250" s="72" t="str">
         <f>VLOOKUP(B250,Distribuições!$A$1:$F$13,6,FALSE)</f>
@@ -27974,7 +27945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" s="72" t="s">
         <v>242</v>
       </c>
@@ -28013,7 +27984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" s="72" t="s">
         <v>246</v>
       </c>
@@ -28052,7 +28023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" s="72" t="s">
         <v>234</v>
       </c>
@@ -28091,7 +28062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" s="72" t="s">
         <v>238</v>
       </c>
@@ -28130,7 +28101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" s="72" t="s">
         <v>243</v>
       </c>
@@ -28169,7 +28140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:13" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:13" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" s="72" t="s">
         <v>247</v>
       </c>
@@ -28208,7 +28179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" s="72" t="s">
         <v>235</v>
       </c>
@@ -28247,7 +28218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" s="72" t="s">
         <v>239</v>
       </c>
@@ -28286,7 +28257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" s="72" t="s">
         <v>244</v>
       </c>
@@ -28325,7 +28296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" s="72" t="s">
         <v>248</v>
       </c>
@@ -28364,7 +28335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" s="72" t="s">
         <v>236</v>
       </c>
@@ -28403,7 +28374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" s="72" t="s">
         <v>240</v>
       </c>
@@ -28442,7 +28413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" s="72" t="s">
         <v>52</v>
       </c>
@@ -28482,7 +28453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" s="72" t="s">
         <v>150</v>
       </c>
@@ -28515,7 +28486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" s="72" t="s">
         <v>151</v>
       </c>
@@ -28548,7 +28519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" s="72" t="s">
         <v>152</v>
       </c>
@@ -28581,7 +28552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" s="72" t="s">
         <v>167</v>
       </c>
@@ -28614,7 +28585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" s="72" t="s">
         <v>170</v>
       </c>
@@ -28647,7 +28618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" s="72" t="s">
         <v>168</v>
       </c>
@@ -28680,7 +28651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" s="72" t="s">
         <v>169</v>
       </c>
@@ -28713,7 +28684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" s="72" t="s">
         <v>171</v>
       </c>
@@ -28746,7 +28717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" s="72" t="s">
         <v>211</v>
       </c>
@@ -28779,7 +28750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" s="72" t="s">
         <v>215</v>
       </c>
@@ -28812,7 +28783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" s="72" t="s">
         <v>210</v>
       </c>
@@ -28845,7 +28816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" s="72" t="s">
         <v>212</v>
       </c>
@@ -28878,7 +28849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" s="72" t="s">
         <v>213</v>
       </c>
@@ -28911,7 +28882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" s="72" t="s">
         <v>214</v>
       </c>
@@ -28944,7 +28915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" s="72" t="s">
         <v>129</v>
       </c>
@@ -28977,7 +28948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" s="72" t="s">
         <v>132</v>
       </c>
@@ -29010,7 +28981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" s="72" t="s">
         <v>130</v>
       </c>
@@ -29043,7 +29014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" s="72" t="s">
         <v>131</v>
       </c>
@@ -29076,7 +29047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" s="72" t="s">
         <v>230</v>
       </c>
@@ -29115,7 +29086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" s="72" t="s">
         <v>161</v>
       </c>
@@ -29148,7 +29119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" s="72" t="s">
         <v>230</v>
       </c>
@@ -29182,7 +29153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" s="72" t="s">
         <v>161</v>
       </c>
@@ -29216,7 +29187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" s="72" t="s">
         <v>230</v>
       </c>
@@ -29250,7 +29221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" s="72" t="s">
         <v>161</v>
       </c>
@@ -29284,7 +29255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" s="72" t="s">
         <v>230</v>
       </c>
@@ -29318,7 +29289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:11" s="72" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:11" s="72" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" s="72" t="s">
         <v>161</v>
       </c>
@@ -29352,7 +29323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="77" t="s">
         <v>471</v>
       </c>
@@ -29391,7 +29362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="77" t="s">
         <v>472</v>
       </c>
@@ -29435,7 +29406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="77" t="s">
         <v>473</v>
       </c>
@@ -29474,7 +29445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="77" t="s">
         <v>474</v>
       </c>
@@ -29513,7 +29484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="77" t="s">
         <v>471</v>
       </c>
@@ -29552,7 +29523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="77" t="s">
         <v>472</v>
       </c>
@@ -29591,7 +29562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="77" t="s">
         <v>473</v>
       </c>
@@ -29630,7 +29601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="77" t="s">
         <v>474</v>
       </c>
@@ -29669,7 +29640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="77" t="s">
         <v>471</v>
       </c>
@@ -29708,7 +29679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="77" t="s">
         <v>472</v>
       </c>
@@ -29747,7 +29718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="77" t="s">
         <v>473</v>
       </c>
@@ -29786,7 +29757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="77" t="s">
         <v>474</v>
       </c>
@@ -29825,7 +29796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="77" t="s">
         <v>471</v>
       </c>
@@ -29864,7 +29835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="77" t="s">
         <v>472</v>
       </c>
@@ -29903,7 +29874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="77" t="s">
         <v>473</v>
       </c>
@@ -29942,7 +29913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="77" t="s">
         <v>474</v>
       </c>
@@ -29981,7 +29952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="77" t="s">
         <v>479</v>
       </c>
@@ -30019,7 +29990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="77" t="s">
         <v>480</v>
       </c>
@@ -30052,7 +30023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="77" t="s">
         <v>481</v>
       </c>
@@ -30085,7 +30056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="77" t="s">
         <v>483</v>
       </c>
@@ -30118,7 +30089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="77" t="s">
         <v>482</v>
       </c>
@@ -30151,7 +30122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="77" t="s">
         <v>479</v>
       </c>
@@ -30184,7 +30155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="77" t="s">
         <v>480</v>
       </c>
@@ -30217,7 +30188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="77" t="s">
         <v>481</v>
       </c>
@@ -30250,7 +30221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="77" t="s">
         <v>483</v>
       </c>
@@ -30283,7 +30254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="77" t="s">
         <v>482</v>
       </c>
@@ -30316,7 +30287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="77" t="s">
         <v>479</v>
       </c>
@@ -30349,7 +30320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="77" t="s">
         <v>480</v>
       </c>
@@ -30382,7 +30353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="77" t="s">
         <v>481</v>
       </c>
@@ -30415,7 +30386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="77" t="s">
         <v>483</v>
       </c>
@@ -30448,7 +30419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="77" t="s">
         <v>482</v>
       </c>
@@ -30481,7 +30452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="77" t="s">
         <v>479</v>
       </c>
@@ -30514,7 +30485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="77" t="s">
         <v>480</v>
       </c>
@@ -30547,7 +30518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="77" t="s">
         <v>481</v>
       </c>
@@ -30580,7 +30551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="77" t="s">
         <v>483</v>
       </c>
@@ -30613,7 +30584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="77" t="s">
         <v>482</v>
       </c>
@@ -30647,7 +30618,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K325" xr:uid="{7B5D6D09-2AF2-4F78-B88B-F79D6D3ADDAA}"/>
+  <autoFilter ref="A1:K325" xr:uid="{7B5D6D09-2AF2-4F78-B88B-F79D6D3ADDAA}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="poisson_percentual_eventos"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -30658,7 +30635,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aplicando verificação dos Betas1 ao Plano de Saúde.
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -2076,7 +2076,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2216,6 +2216,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -2717,7 +2718,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D83D282-F75C-4952-B6E5-FA904FFBD51F}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3460,11 +3463,11 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="83" t="s">
+      <c r="A62" s="95" t="s">
         <v>147</v>
       </c>
-      <c r="B62" s="83">
-        <v>1.5491573940793143E-3</v>
+      <c r="B62" s="95">
+        <v>0</v>
       </c>
       <c r="C62" s="83" t="str">
         <f>IF(VLOOKUP(A62,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3472,11 +3475,11 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="83" t="s">
+      <c r="A63" s="95" t="s">
         <v>148</v>
       </c>
-      <c r="B63" s="83">
-        <v>-4.399566149642267E-3</v>
+      <c r="B63" s="95">
+        <v>0</v>
       </c>
       <c r="C63" s="83" t="str">
         <f>IF(VLOOKUP(A63,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>

</xml_diff>

<commit_message>
Verificação dos Betas - Regressão de Desligamentos Voluntários
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -39,7 +39,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Cenarios!$A$1:$C$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Constantes!$A$1:$C$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Constantes!$A$1:$C$84</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">Custos!$A$1:$D$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Eventos_Inic!$A$2:$L$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Funcoes_Inputs!$A$1:$I$250</definedName>
@@ -2210,13 +2210,13 @@
     <xf numFmtId="10" fontId="28" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="28" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -2718,8 +2718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D83D282-F75C-4952-B6E5-FA904FFBD51F}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3463,10 +3463,10 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="95" t="s">
+      <c r="A62" s="93" t="s">
         <v>147</v>
       </c>
-      <c r="B62" s="95">
+      <c r="B62" s="93">
         <v>0</v>
       </c>
       <c r="C62" s="83" t="str">
@@ -3475,10 +3475,10 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="95" t="s">
+      <c r="A63" s="93" t="s">
         <v>148</v>
       </c>
-      <c r="B63" s="95">
+      <c r="B63" s="93">
         <v>0</v>
       </c>
       <c r="C63" s="83" t="str">
@@ -3739,7 +3739,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C29" xr:uid="{E72623EE-AF76-4665-8E1C-61480EAE2A81}"/>
+  <autoFilter ref="A1:C84" xr:uid="{E72623EE-AF76-4665-8E1C-61480EAE2A81}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -10900,28 +10900,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="95" t="s">
         <v>255</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="94" t="s">
         <v>441</v>
       </c>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93" t="s">
+      <c r="C1" s="94"/>
+      <c r="D1" s="94" t="s">
         <v>442</v>
       </c>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93" t="s">
+      <c r="E1" s="94"/>
+      <c r="F1" s="94" t="s">
         <v>443</v>
       </c>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="94"/>
+      <c r="A2" s="95"/>
       <c r="B2" s="55" t="s">
         <v>439</v>
       </c>

</xml_diff>

<commit_message>
Gráfico box plot por iniciativa
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7470" tabRatio="749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7470" tabRatio="749" firstSheet="5" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constantes" sheetId="36" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2889" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2891" uniqueCount="554">
   <si>
     <t>Ano</t>
   </si>
@@ -1765,6 +1765,12 @@
   </si>
   <si>
     <t>AnosDelay</t>
+  </si>
+  <si>
+    <t>Multas1</t>
+  </si>
+  <si>
+    <t>DespesaExposicaoMulta1</t>
   </si>
 </sst>
 </file>
@@ -2718,8 +2724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D83D282-F75C-4952-B6E5-FA904FFBD51F}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E100" sqref="E100"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14124,10 +14130,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:I250"/>
+  <dimension ref="A1:I253"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A229" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F233" sqref="F233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23134,6 +23140,16 @@
       <c r="I250" s="67">
         <f t="shared" si="15"/>
         <v>9</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B252" s="11" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B253" s="11" t="s">
+        <v>552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualizando versão e adicionando verificação de inputs inconsistentes
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7470" tabRatio="749" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7470" tabRatio="749" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constantes" sheetId="36" r:id="rId1"/>
@@ -23415,9 +23415,9 @@
   </sheetPr>
   <dimension ref="A1:P145"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A145" sqref="A145"/>
+      <selection pane="bottomLeft" activeCell="B142" sqref="B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37773,8 +37773,8 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37809,7 +37809,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="70">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="C2" s="68">
         <v>2017</v>

</xml_diff>

<commit_message>
Implementaçao genérica dos batentes, e aplicação à todas as regressões
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7470" tabRatio="749" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7470" tabRatio="749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constantes" sheetId="36" r:id="rId1"/>
@@ -2748,8 +2748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D83D282-F75C-4952-B6E5-FA904FFBD51F}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37773,8 +37773,8 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ajustando arquivo app e arquivo de dados
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -39,7 +39,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Cenarios!$A$1:$C$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Constantes!$A$1:$C$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Constantes!$A$1:$C$55</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">Custos!$A$1:$D$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Eventos_Inic!$A$2:$L$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Funcoes_Inputs!$A$1:$I$226</definedName>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2955" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2988" uniqueCount="562">
   <si>
     <t>Ano</t>
   </si>
@@ -2106,7 +2106,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2247,6 +2247,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -2746,10 +2747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D83D282-F75C-4952-B6E5-FA904FFBD51F}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3110,10 +3111,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="83" t="s">
-        <v>175</v>
+        <v>202</v>
       </c>
       <c r="B30" s="83">
-        <v>0</v>
+        <v>2289.12</v>
       </c>
       <c r="C30" s="83" t="str">
         <f>IF(VLOOKUP(A30,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3122,10 +3123,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="83" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B31" s="83">
-        <v>2289.12</v>
+        <v>419405.11</v>
       </c>
       <c r="C31" s="83" t="str">
         <f>IF(VLOOKUP(A31,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3134,10 +3135,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="83" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B32" s="83">
-        <v>419405.11</v>
+        <v>178766</v>
       </c>
       <c r="C32" s="83" t="str">
         <f>IF(VLOOKUP(A32,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3146,10 +3147,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="83" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B33" s="83">
-        <v>178766</v>
+        <v>277966.82127272728</v>
       </c>
       <c r="C33" s="83" t="str">
         <f>IF(VLOOKUP(A33,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3158,10 +3159,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="83" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="B34" s="83">
-        <v>277966.82127272728</v>
+        <v>0.2044537027147259</v>
       </c>
       <c r="C34" s="83" t="str">
         <f>IF(VLOOKUP(A34,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3169,11 +3170,11 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="83" t="s">
-        <v>146</v>
-      </c>
-      <c r="B35" s="83">
-        <v>0.2044537027147259</v>
+      <c r="A35" s="93" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" s="93">
+        <v>0</v>
       </c>
       <c r="C35" s="83" t="str">
         <f>IF(VLOOKUP(A35,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3182,7 +3183,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="93" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B36" s="93">
         <v>0</v>
@@ -3193,10 +3194,10 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="93" t="s">
-        <v>148</v>
-      </c>
-      <c r="B37" s="93">
+      <c r="A37" s="83" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" s="83">
         <v>0</v>
       </c>
       <c r="C37" s="83" t="str">
@@ -3206,7 +3207,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="83" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B38" s="83">
         <v>0</v>
@@ -3218,7 +3219,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="83" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B39" s="83">
         <v>0</v>
@@ -3230,7 +3231,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="83" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B40" s="83">
         <v>0</v>
@@ -3242,10 +3243,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="83" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B41" s="83">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="C41" s="83" t="str">
         <f>IF(VLOOKUP(A41,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3254,10 +3255,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="83" t="s">
-        <v>167</v>
+        <v>207</v>
       </c>
       <c r="B42" s="83">
-        <v>32</v>
+        <v>7.8975872998198113</v>
       </c>
       <c r="C42" s="83" t="str">
         <f>IF(VLOOKUP(A42,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3266,10 +3267,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="83" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B43" s="83">
-        <v>7.8975872998198113</v>
+        <v>0.62289934258889479</v>
       </c>
       <c r="C43" s="83" t="str">
         <f>IF(VLOOKUP(A43,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3278,10 +3279,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="83" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B44" s="83">
-        <v>0.62289934258889479</v>
+        <v>9.0134963707211782</v>
       </c>
       <c r="C44" s="83" t="str">
         <f>IF(VLOOKUP(A44,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3290,10 +3291,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="83" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B45" s="83">
-        <v>9.0134963707211782</v>
+        <v>11.225658326292109</v>
       </c>
       <c r="C45" s="83" t="str">
         <f>IF(VLOOKUP(A45,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3302,10 +3303,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="83" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B46" s="83">
-        <v>11.225658326292109</v>
+        <v>16.96052253162523</v>
       </c>
       <c r="C46" s="83" t="str">
         <f>IF(VLOOKUP(A46,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3314,10 +3315,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="83" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B47" s="83">
-        <v>16.96052253162523</v>
+        <v>7.038585793358461</v>
       </c>
       <c r="C47" s="83" t="str">
         <f>IF(VLOOKUP(A47,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3326,10 +3327,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="83" t="s">
-        <v>210</v>
+        <v>125</v>
       </c>
       <c r="B48" s="83">
-        <v>7.038585793358461</v>
+        <v>0</v>
       </c>
       <c r="C48" s="83" t="str">
         <f>IF(VLOOKUP(A48,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3338,7 +3339,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="83" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B49" s="83">
         <v>0</v>
@@ -3350,7 +3351,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="83" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B50" s="83">
         <v>0</v>
@@ -3362,7 +3363,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="83" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B51" s="83">
         <v>0</v>
@@ -3374,10 +3375,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="83" t="s">
-        <v>127</v>
+        <v>465</v>
       </c>
       <c r="B52" s="83">
-        <v>0</v>
+        <v>2.2111111111111108</v>
       </c>
       <c r="C52" s="83" t="str">
         <f>IF(VLOOKUP(A52,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3386,10 +3387,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="83" t="s">
-        <v>226</v>
+        <v>466</v>
       </c>
       <c r="B53" s="83">
-        <v>0</v>
+        <v>5.5555555555555558E-3</v>
       </c>
       <c r="C53" s="83" t="str">
         <f>IF(VLOOKUP(A53,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3398,10 +3399,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="83" t="s">
-        <v>157</v>
+        <v>467</v>
       </c>
       <c r="B54" s="83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54" s="83" t="str">
         <f>IF(VLOOKUP(A54,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3410,54 +3411,18 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="83" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="B55" s="83">
-        <v>2.2111111111111108</v>
+        <v>7.2222222222222229E-2</v>
       </c>
       <c r="C55" s="83" t="str">
         <f>IF(VLOOKUP(A55,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
         <v>Sim</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="83" t="s">
-        <v>466</v>
-      </c>
-      <c r="B56" s="83">
-        <v>5.5555555555555558E-3</v>
-      </c>
-      <c r="C56" s="83" t="str">
-        <f>IF(VLOOKUP(A56,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
-        <v>Sim</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="83" t="s">
-        <v>467</v>
-      </c>
-      <c r="B57" s="83">
-        <v>1</v>
-      </c>
-      <c r="C57" s="83" t="str">
-        <f>IF(VLOOKUP(A57,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
-        <v>Sim</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="83" t="s">
-        <v>468</v>
-      </c>
-      <c r="B58" s="83">
-        <v>7.2222222222222229E-2</v>
-      </c>
-      <c r="C58" s="83" t="str">
-        <f>IF(VLOOKUP(A58,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
-        <v>Sim</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C58" xr:uid="{E72623EE-AF76-4665-8E1C-61480EAE2A81}"/>
+  <autoFilter ref="A1:C55" xr:uid="{E72623EE-AF76-4665-8E1C-61480EAE2A81}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -23413,11 +23378,11 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:P145"/>
+  <dimension ref="A1:P157"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B142" sqref="B142"/>
+      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30424,6 +30389,539 @@
       </c>
       <c r="P145" s="86" t="b">
         <f>COUNTIF(Constantes!$A:$A,Parametros!A145)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A146" s="83" t="s">
+        <v>175</v>
+      </c>
+      <c r="B146" s="86" t="str">
+        <f>IF(VLOOKUP(A146,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
+        <v>Sim</v>
+      </c>
+      <c r="C146" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D146" s="96">
+        <v>200</v>
+      </c>
+      <c r="E146" s="85">
+        <v>0</v>
+      </c>
+      <c r="H146" s="86">
+        <v>0</v>
+      </c>
+      <c r="I146" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="J146" s="86" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A146)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="K146" s="86" t="str">
+        <f t="shared" ref="K146:K157" si="8">IF(AND(C146="normal",NOT(COUNT(D146:E146)=2)),"Dados Incorretos",
+IF(AND(C146="triangular",NOT(COUNT(D146:F146)=3)),"Dados Incorretos",
+IF(AND(C146="poisson",NOT(COUNT(D146:E146)=1)),"Dados Incorretos",
+IF(AND(C146="normaltruncada",NOT(COUNT(D146:G146)=4)),"Dados Incorretos",
+IF(AND(C146="uniforme",NOT(COUNT(D146:E146)=2)),"Dados Incorretos",
+IF(AND(C146="poisson_percentual_eventos",NOT(COUNT(D146:E146)=1)),"Dados Incorretos","OK"))))))</f>
+        <v>OK</v>
+      </c>
+      <c r="L146" s="86" t="str">
+        <f>VLOOKUP(C146,Distribuições!$A$1:$F$13,6,FALSE)</f>
+        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+      </c>
+      <c r="M146" s="86">
+        <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A146)</f>
+        <v>1</v>
+      </c>
+      <c r="P146" s="86" t="b">
+        <f>COUNTIF(Constantes!$A:$A,Parametros!A146)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A147" s="83" t="s">
+        <v>175</v>
+      </c>
+      <c r="B147" s="86" t="str">
+        <f>IF(VLOOKUP(A147,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
+        <v>Sim</v>
+      </c>
+      <c r="C147" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D147" s="96">
+        <v>200</v>
+      </c>
+      <c r="E147" s="85">
+        <v>0</v>
+      </c>
+      <c r="H147" s="86">
+        <v>0</v>
+      </c>
+      <c r="I147" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J147" s="86" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A147)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="K147" s="86" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="L147" s="86" t="str">
+        <f>VLOOKUP(C147,Distribuições!$A$1:$F$13,6,FALSE)</f>
+        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+      </c>
+      <c r="M147" s="86">
+        <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A147)</f>
+        <v>1</v>
+      </c>
+      <c r="P147" s="86" t="b">
+        <f>COUNTIF(Constantes!$A:$A,Parametros!A147)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A148" s="83" t="s">
+        <v>175</v>
+      </c>
+      <c r="B148" s="86" t="str">
+        <f>IF(VLOOKUP(A148,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
+        <v>Sim</v>
+      </c>
+      <c r="C148" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D148" s="96">
+        <v>200</v>
+      </c>
+      <c r="E148" s="85">
+        <v>0</v>
+      </c>
+      <c r="H148" s="86">
+        <v>0</v>
+      </c>
+      <c r="I148" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="J148" s="86" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A148)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="K148" s="86" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="L148" s="86" t="str">
+        <f>VLOOKUP(C148,Distribuições!$A$1:$F$13,6,FALSE)</f>
+        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+      </c>
+      <c r="M148" s="86">
+        <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A148)</f>
+        <v>1</v>
+      </c>
+      <c r="P148" s="86" t="b">
+        <f>COUNTIF(Constantes!$A:$A,Parametros!A148)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A149" s="83" t="s">
+        <v>175</v>
+      </c>
+      <c r="B149" s="86" t="str">
+        <f>IF(VLOOKUP(A149,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
+        <v>Sim</v>
+      </c>
+      <c r="C149" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D149" s="96">
+        <v>200</v>
+      </c>
+      <c r="E149" s="85">
+        <v>0</v>
+      </c>
+      <c r="H149" s="86">
+        <v>0</v>
+      </c>
+      <c r="I149" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J149" s="86" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A149)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="K149" s="86" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="L149" s="86" t="str">
+        <f>VLOOKUP(C149,Distribuições!$A$1:$F$13,6,FALSE)</f>
+        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+      </c>
+      <c r="M149" s="86">
+        <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A149)</f>
+        <v>1</v>
+      </c>
+      <c r="P149" s="86" t="b">
+        <f>COUNTIF(Constantes!$A:$A,Parametros!A149)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A150" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="B150" s="86" t="str">
+        <f>IF(VLOOKUP(A150,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
+        <v>Sim</v>
+      </c>
+      <c r="C150" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D150" s="96">
+        <v>200</v>
+      </c>
+      <c r="E150" s="85">
+        <v>0</v>
+      </c>
+      <c r="H150" s="86">
+        <v>0</v>
+      </c>
+      <c r="I150" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="J150" s="86" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A150)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="K150" s="86" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="L150" s="86" t="str">
+        <f>VLOOKUP(C150,Distribuições!$A$1:$F$13,6,FALSE)</f>
+        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+      </c>
+      <c r="M150" s="86">
+        <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A150)</f>
+        <v>1</v>
+      </c>
+      <c r="P150" s="86" t="b">
+        <f>COUNTIF(Constantes!$A:$A,Parametros!A150)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A151" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="B151" s="86" t="str">
+        <f>IF(VLOOKUP(A151,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
+        <v>Sim</v>
+      </c>
+      <c r="C151" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D151" s="96">
+        <v>200</v>
+      </c>
+      <c r="E151" s="85">
+        <v>0</v>
+      </c>
+      <c r="H151" s="86">
+        <v>0</v>
+      </c>
+      <c r="I151" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J151" s="86" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A151)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="K151" s="86" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="L151" s="86" t="str">
+        <f>VLOOKUP(C151,Distribuições!$A$1:$F$13,6,FALSE)</f>
+        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+      </c>
+      <c r="M151" s="86">
+        <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A151)</f>
+        <v>1</v>
+      </c>
+      <c r="P151" s="86" t="b">
+        <f>COUNTIF(Constantes!$A:$A,Parametros!A151)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A152" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="B152" s="86" t="str">
+        <f>IF(VLOOKUP(A152,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
+        <v>Sim</v>
+      </c>
+      <c r="C152" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D152" s="96">
+        <v>200</v>
+      </c>
+      <c r="E152" s="85">
+        <v>0</v>
+      </c>
+      <c r="H152" s="86">
+        <v>0</v>
+      </c>
+      <c r="I152" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="J152" s="86" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A152)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="K152" s="86" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="L152" s="86" t="str">
+        <f>VLOOKUP(C152,Distribuições!$A$1:$F$13,6,FALSE)</f>
+        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+      </c>
+      <c r="M152" s="86">
+        <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A152)</f>
+        <v>1</v>
+      </c>
+      <c r="P152" s="86" t="b">
+        <f>COUNTIF(Constantes!$A:$A,Parametros!A152)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A153" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="B153" s="86" t="str">
+        <f>IF(VLOOKUP(A153,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
+        <v>Sim</v>
+      </c>
+      <c r="C153" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D153" s="96">
+        <v>200</v>
+      </c>
+      <c r="E153" s="85">
+        <v>0</v>
+      </c>
+      <c r="H153" s="86">
+        <v>0</v>
+      </c>
+      <c r="I153" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J153" s="86" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A153)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="K153" s="86" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="L153" s="86" t="str">
+        <f>VLOOKUP(C153,Distribuições!$A$1:$F$13,6,FALSE)</f>
+        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+      </c>
+      <c r="M153" s="86">
+        <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A153)</f>
+        <v>1</v>
+      </c>
+      <c r="P153" s="86" t="b">
+        <f>COUNTIF(Constantes!$A:$A,Parametros!A153)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A154" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B154" s="86" t="str">
+        <f>IF(VLOOKUP(A154,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
+        <v>Sim</v>
+      </c>
+      <c r="C154" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D154" s="96">
+        <v>200</v>
+      </c>
+      <c r="E154" s="85">
+        <v>0</v>
+      </c>
+      <c r="H154" s="86">
+        <v>0</v>
+      </c>
+      <c r="I154" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="J154" s="86" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A154)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="K154" s="86" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="L154" s="86" t="str">
+        <f>VLOOKUP(C154,Distribuições!$A$1:$F$13,6,FALSE)</f>
+        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+      </c>
+      <c r="M154" s="86">
+        <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A154)</f>
+        <v>1</v>
+      </c>
+      <c r="P154" s="86" t="b">
+        <f>COUNTIF(Constantes!$A:$A,Parametros!A154)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A155" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B155" s="86" t="str">
+        <f>IF(VLOOKUP(A155,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
+        <v>Sim</v>
+      </c>
+      <c r="C155" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D155" s="96">
+        <v>200</v>
+      </c>
+      <c r="E155" s="85">
+        <v>0</v>
+      </c>
+      <c r="H155" s="86">
+        <v>0</v>
+      </c>
+      <c r="I155" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J155" s="86" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A155)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="K155" s="86" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="L155" s="86" t="str">
+        <f>VLOOKUP(C155,Distribuições!$A$1:$F$13,6,FALSE)</f>
+        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+      </c>
+      <c r="M155" s="86">
+        <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A155)</f>
+        <v>1</v>
+      </c>
+      <c r="P155" s="86" t="b">
+        <f>COUNTIF(Constantes!$A:$A,Parametros!A155)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A156" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B156" s="86" t="str">
+        <f>IF(VLOOKUP(A156,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
+        <v>Sim</v>
+      </c>
+      <c r="C156" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D156" s="96">
+        <v>200</v>
+      </c>
+      <c r="E156" s="85">
+        <v>0</v>
+      </c>
+      <c r="H156" s="86">
+        <v>0</v>
+      </c>
+      <c r="I156" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="J156" s="86" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A156)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="K156" s="86" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="L156" s="86" t="str">
+        <f>VLOOKUP(C156,Distribuições!$A$1:$F$13,6,FALSE)</f>
+        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+      </c>
+      <c r="M156" s="86">
+        <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A156)</f>
+        <v>1</v>
+      </c>
+      <c r="P156" s="86" t="b">
+        <f>COUNTIF(Constantes!$A:$A,Parametros!A156)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A157" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B157" s="86" t="str">
+        <f>IF(VLOOKUP(A157,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
+        <v>Sim</v>
+      </c>
+      <c r="C157" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D157" s="96">
+        <v>200</v>
+      </c>
+      <c r="E157" s="85">
+        <v>0</v>
+      </c>
+      <c r="H157" s="86">
+        <v>0</v>
+      </c>
+      <c r="I157" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J157" s="86" t="b">
+        <f>IF(COUNTIF(ParametrosSemSeedFixa!$A:$A,Parametros!A157)&gt;0,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="K157" s="86" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="L157" s="86" t="str">
+        <f>VLOOKUP(C157,Distribuições!$A$1:$F$13,6,FALSE)</f>
+        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+      </c>
+      <c r="M157" s="86">
+        <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A157)</f>
+        <v>1</v>
+      </c>
+      <c r="P157" s="86" t="b">
+        <f>COUNTIF(Constantes!$A:$A,Parametros!A157)&gt;0</f>
         <v>0</v>
       </c>
     </row>
@@ -36017,7 +36515,7 @@
       </c>
       <c r="E67" s="77">
         <f>COUNTIF(Parametros!A:A,Verificação_Parametros!A67)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F67" s="77" t="b">
         <f t="shared" si="2"/>
@@ -36025,7 +36523,7 @@
       </c>
       <c r="G67" s="77">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H67" s="77" t="s">
         <v>456</v>
@@ -37073,7 +37571,7 @@
       </c>
       <c r="E100" s="77">
         <f>COUNTIF(Parametros!A:A,Verificação_Parametros!A100)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F100" s="77" t="b">
         <f t="shared" si="2"/>
@@ -37081,7 +37579,7 @@
       </c>
       <c r="G100" s="77">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H100" s="77" t="s">
         <v>456</v>
@@ -37105,7 +37603,7 @@
       </c>
       <c r="E101" s="77">
         <f>COUNTIF(Parametros!A:A,Verificação_Parametros!A101)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F101" s="77" t="b">
         <f t="shared" si="2"/>
@@ -37113,7 +37611,7 @@
       </c>
       <c r="G101" s="77">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H101" s="77" t="s">
         <v>456</v>

</xml_diff>

<commit_message>
Alterando Dados de Entrada
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -2241,13 +2241,13 @@
     <xf numFmtId="43" fontId="28" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -2749,8 +2749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D83D282-F75C-4952-B6E5-FA904FFBD51F}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3246,7 +3246,7 @@
         <v>167</v>
       </c>
       <c r="B41" s="83">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="C41" s="83" t="str">
         <f>IF(VLOOKUP(A41,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -10583,28 +10583,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="96" t="s">
         <v>255</v>
       </c>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="95" t="s">
         <v>441</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94" t="s">
+      <c r="C1" s="95"/>
+      <c r="D1" s="95" t="s">
         <v>442</v>
       </c>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94" t="s">
+      <c r="E1" s="95"/>
+      <c r="F1" s="95" t="s">
         <v>443</v>
       </c>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95"/>
+      <c r="A2" s="96"/>
       <c r="B2" s="55" t="s">
         <v>439</v>
       </c>
@@ -30403,7 +30403,7 @@
       <c r="C146" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D146" s="96">
+      <c r="D146" s="94">
         <v>200</v>
       </c>
       <c r="E146" s="85">
@@ -30452,7 +30452,7 @@
       <c r="C147" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D147" s="96">
+      <c r="D147" s="94">
         <v>200</v>
       </c>
       <c r="E147" s="85">
@@ -30496,7 +30496,7 @@
       <c r="C148" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D148" s="96">
+      <c r="D148" s="94">
         <v>200</v>
       </c>
       <c r="E148" s="85">
@@ -30540,7 +30540,7 @@
       <c r="C149" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D149" s="96">
+      <c r="D149" s="94">
         <v>200</v>
       </c>
       <c r="E149" s="85">
@@ -30584,7 +30584,7 @@
       <c r="C150" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D150" s="96">
+      <c r="D150" s="94">
         <v>200</v>
       </c>
       <c r="E150" s="85">
@@ -30628,7 +30628,7 @@
       <c r="C151" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D151" s="96">
+      <c r="D151" s="94">
         <v>200</v>
       </c>
       <c r="E151" s="85">
@@ -30672,7 +30672,7 @@
       <c r="C152" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D152" s="96">
+      <c r="D152" s="94">
         <v>200</v>
       </c>
       <c r="E152" s="85">
@@ -30716,7 +30716,7 @@
       <c r="C153" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D153" s="96">
+      <c r="D153" s="94">
         <v>200</v>
       </c>
       <c r="E153" s="85">
@@ -30760,7 +30760,7 @@
       <c r="C154" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D154" s="96">
+      <c r="D154" s="94">
         <v>200</v>
       </c>
       <c r="E154" s="85">
@@ -30804,7 +30804,7 @@
       <c r="C155" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D155" s="96">
+      <c r="D155" s="94">
         <v>200</v>
       </c>
       <c r="E155" s="85">
@@ -30848,7 +30848,7 @@
       <c r="C156" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D156" s="96">
+      <c r="D156" s="94">
         <v>200</v>
       </c>
       <c r="E156" s="85">
@@ -30892,7 +30892,7 @@
       <c r="C157" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D157" s="96">
+      <c r="D157" s="94">
         <v>200</v>
       </c>
       <c r="E157" s="85">

</xml_diff>

<commit_message>
Adicionando rotinas para tratamento de dados
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7470" tabRatio="749" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7470" tabRatio="749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constantes" sheetId="36" r:id="rId1"/>
@@ -39,7 +39,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Cenarios!$A$1:$C$13</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Constantes!$A$1:$C$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Constantes!$A$1:$C$52</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">Custos!$A$1:$D$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Eventos_Inic!$A$2:$L$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Funcoes_Inputs!$A$1:$I$226</definedName>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3010" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3007" uniqueCount="564">
   <si>
     <t>Ano</t>
   </si>
@@ -2753,9 +2753,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D83D282-F75C-4952-B6E5-FA904FFBD51F}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2851,7 +2851,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="83" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="B8" s="83">
         <v>0</v>
@@ -2863,10 +2863,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B9" s="83">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="83" t="str">
         <f>IF(VLOOKUP(A9,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="83" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B10" s="83">
         <v>0</v>
@@ -2887,7 +2887,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="83" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B11" s="83">
         <v>0</v>
@@ -2899,10 +2899,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="83" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="B12" s="83">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="C12" s="83" t="str">
         <f>IF(VLOOKUP(A12,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -2911,10 +2911,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="83" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
       <c r="B13" s="83">
-        <v>0</v>
+        <v>2522743.88</v>
       </c>
       <c r="C13" s="83" t="str">
         <f>IF(VLOOKUP(A13,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -2923,10 +2923,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="83" t="s">
-        <v>126</v>
+        <v>466</v>
       </c>
       <c r="B14" s="83">
-        <v>0.01</v>
+        <v>10000</v>
       </c>
       <c r="C14" s="83" t="str">
         <f>IF(VLOOKUP(A14,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -2935,10 +2935,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="83" t="s">
-        <v>132</v>
+        <v>468</v>
       </c>
       <c r="B15" s="83">
-        <v>300</v>
+        <v>10000</v>
       </c>
       <c r="C15" s="83" t="str">
         <f>IF(VLOOKUP(A15,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -2947,10 +2947,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="83" t="s">
-        <v>142</v>
+        <v>540</v>
       </c>
       <c r="B16" s="83">
-        <v>2522743.88</v>
+        <v>1</v>
       </c>
       <c r="C16" s="83" t="str">
         <f>IF(VLOOKUP(A16,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -2959,10 +2959,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="83" t="s">
-        <v>466</v>
+        <v>69</v>
       </c>
       <c r="B17" s="83">
-        <v>10000</v>
+        <v>6475</v>
       </c>
       <c r="C17" s="83" t="str">
         <f>IF(VLOOKUP(A17,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -2971,10 +2971,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="83" t="s">
-        <v>468</v>
+        <v>86</v>
       </c>
       <c r="B18" s="83">
-        <v>10000</v>
+        <v>2.976190476190476E-3</v>
       </c>
       <c r="C18" s="83" t="str">
         <f>IF(VLOOKUP(A18,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -2983,10 +2983,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="83" t="s">
-        <v>540</v>
+        <v>103</v>
       </c>
       <c r="B19" s="83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="83" t="str">
         <f>IF(VLOOKUP(A19,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -2995,10 +2995,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="83" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="B20" s="83">
-        <v>6475</v>
+        <v>0</v>
       </c>
       <c r="C20" s="83" t="str">
         <f>IF(VLOOKUP(A20,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3007,10 +3007,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="83" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="B21" s="83">
-        <v>2.976190476190476E-3</v>
+        <v>0</v>
       </c>
       <c r="C21" s="83" t="str">
         <f>IF(VLOOKUP(A21,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3019,10 +3019,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="83" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="B22" s="83">
-        <v>0</v>
+        <v>2.8854037747524753E-2</v>
       </c>
       <c r="C22" s="83" t="str">
         <f>IF(VLOOKUP(A22,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3031,10 +3031,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="83" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="B23" s="83">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="C23" s="83" t="str">
         <f>IF(VLOOKUP(A23,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3043,7 +3043,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="83" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="B24" s="83">
         <v>0</v>
@@ -3055,10 +3055,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="83" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="B25" s="83">
-        <v>2.8854037747524753E-2</v>
+        <v>0</v>
       </c>
       <c r="C25" s="83" t="str">
         <f>IF(VLOOKUP(A25,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3067,10 +3067,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="83" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="B26" s="83">
-        <v>6000</v>
+        <v>23.90625</v>
       </c>
       <c r="C26" s="83" t="str">
         <f>IF(VLOOKUP(A26,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3079,10 +3079,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="83" t="s">
-        <v>151</v>
+        <v>199</v>
       </c>
       <c r="B27" s="83">
-        <v>0</v>
+        <v>2289.12</v>
       </c>
       <c r="C27" s="83" t="str">
         <f>IF(VLOOKUP(A27,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3091,10 +3091,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="83" t="s">
-        <v>152</v>
+        <v>200</v>
       </c>
       <c r="B28" s="83">
-        <v>0</v>
+        <v>419405.11</v>
       </c>
       <c r="C28" s="83" t="str">
         <f>IF(VLOOKUP(A28,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3103,10 +3103,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="83" t="s">
-        <v>168</v>
+        <v>201</v>
       </c>
       <c r="B29" s="83">
-        <v>23.90625</v>
+        <v>178766</v>
       </c>
       <c r="C29" s="83" t="str">
         <f>IF(VLOOKUP(A29,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3115,10 +3115,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="83" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B30" s="83">
-        <v>2289.12</v>
+        <v>277966.82127272728</v>
       </c>
       <c r="C30" s="83" t="str">
         <f>IF(VLOOKUP(A30,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3127,10 +3127,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="83" t="s">
-        <v>200</v>
+        <v>143</v>
       </c>
       <c r="B31" s="83">
-        <v>419405.11</v>
+        <v>0.2044537027147259</v>
       </c>
       <c r="C31" s="83" t="str">
         <f>IF(VLOOKUP(A31,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3138,11 +3138,11 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="83" t="s">
-        <v>201</v>
-      </c>
-      <c r="B32" s="83">
-        <v>178766</v>
+      <c r="A32" s="93" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" s="93">
+        <v>0</v>
       </c>
       <c r="C32" s="83" t="str">
         <f>IF(VLOOKUP(A32,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3150,11 +3150,11 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="83" t="s">
-        <v>202</v>
-      </c>
-      <c r="B33" s="83">
-        <v>277966.82127272728</v>
+      <c r="A33" s="93" t="s">
+        <v>145</v>
+      </c>
+      <c r="B33" s="93">
+        <v>0</v>
       </c>
       <c r="C33" s="83" t="str">
         <f>IF(VLOOKUP(A33,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3163,10 +3163,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="83" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="B34" s="83">
-        <v>0.2044537027147259</v>
+        <v>0</v>
       </c>
       <c r="C34" s="83" t="str">
         <f>IF(VLOOKUP(A34,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3174,10 +3174,10 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="93" t="s">
-        <v>144</v>
-      </c>
-      <c r="B35" s="93">
+      <c r="A35" s="83" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="83">
         <v>0</v>
       </c>
       <c r="C35" s="83" t="str">
@@ -3186,10 +3186,10 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="93" t="s">
-        <v>145</v>
-      </c>
-      <c r="B36" s="93">
+      <c r="A36" s="83" t="s">
+        <v>161</v>
+      </c>
+      <c r="B36" s="83">
         <v>0</v>
       </c>
       <c r="C36" s="83" t="str">
@@ -3199,7 +3199,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="83" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B37" s="83">
         <v>0</v>
@@ -3211,7 +3211,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="83" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B38" s="83">
         <v>0</v>
@@ -3223,10 +3223,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="83" t="s">
-        <v>161</v>
+        <v>204</v>
       </c>
       <c r="B39" s="83">
-        <v>0</v>
+        <v>7.8975872998198113</v>
       </c>
       <c r="C39" s="83" t="str">
         <f>IF(VLOOKUP(A39,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3235,10 +3235,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="83" t="s">
-        <v>162</v>
+        <v>208</v>
       </c>
       <c r="B40" s="83">
-        <v>0</v>
+        <v>0.62289934258889479</v>
       </c>
       <c r="C40" s="83" t="str">
         <f>IF(VLOOKUP(A40,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3247,10 +3247,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="83" t="s">
-        <v>164</v>
+        <v>203</v>
       </c>
       <c r="B41" s="83">
-        <v>0</v>
+        <v>9.0134963707211782</v>
       </c>
       <c r="C41" s="83" t="str">
         <f>IF(VLOOKUP(A41,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3259,10 +3259,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="83" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B42" s="83">
-        <v>7.8975872998198113</v>
+        <v>11.225658326292109</v>
       </c>
       <c r="C42" s="83" t="str">
         <f>IF(VLOOKUP(A42,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3271,10 +3271,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="83" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B43" s="83">
-        <v>0.62289934258889479</v>
+        <v>16.96052253162523</v>
       </c>
       <c r="C43" s="83" t="str">
         <f>IF(VLOOKUP(A43,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3283,10 +3283,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="83" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B44" s="83">
-        <v>9.0134963707211782</v>
+        <v>7.038585793358461</v>
       </c>
       <c r="C44" s="83" t="str">
         <f>IF(VLOOKUP(A44,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3295,10 +3295,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="83" t="s">
-        <v>205</v>
+        <v>122</v>
       </c>
       <c r="B45" s="83">
-        <v>11.225658326292109</v>
+        <v>0</v>
       </c>
       <c r="C45" s="83" t="str">
         <f>IF(VLOOKUP(A45,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3307,10 +3307,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="83" t="s">
-        <v>206</v>
+        <v>125</v>
       </c>
       <c r="B46" s="83">
-        <v>16.96052253162523</v>
+        <v>0</v>
       </c>
       <c r="C46" s="83" t="str">
         <f>IF(VLOOKUP(A46,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3319,10 +3319,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="83" t="s">
-        <v>207</v>
+        <v>123</v>
       </c>
       <c r="B47" s="83">
-        <v>7.038585793358461</v>
+        <v>0</v>
       </c>
       <c r="C47" s="83" t="str">
         <f>IF(VLOOKUP(A47,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3331,7 +3331,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="83" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B48" s="83">
         <v>0</v>
@@ -3343,10 +3343,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="83" t="s">
-        <v>125</v>
+        <v>461</v>
       </c>
       <c r="B49" s="83">
-        <v>0</v>
+        <v>2.2111111111111108</v>
       </c>
       <c r="C49" s="83" t="str">
         <f>IF(VLOOKUP(A49,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3355,10 +3355,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="83" t="s">
-        <v>123</v>
+        <v>462</v>
       </c>
       <c r="B50" s="83">
-        <v>0</v>
+        <v>5.5555555555555558E-3</v>
       </c>
       <c r="C50" s="83" t="str">
         <f>IF(VLOOKUP(A50,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3367,10 +3367,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="83" t="s">
-        <v>124</v>
+        <v>463</v>
       </c>
       <c r="B51" s="83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51" s="83" t="str">
         <f>IF(VLOOKUP(A51,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
@@ -3379,54 +3379,18 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="83" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="B52" s="83">
-        <v>2.2111111111111108</v>
+        <v>7.2222222222222229E-2</v>
       </c>
       <c r="C52" s="83" t="str">
         <f>IF(VLOOKUP(A52,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
         <v>Sim</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="83" t="s">
-        <v>462</v>
-      </c>
-      <c r="B53" s="83">
-        <v>5.5555555555555558E-3</v>
-      </c>
-      <c r="C53" s="83" t="str">
-        <f>IF(VLOOKUP(A53,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
-        <v>Sim</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="83" t="s">
-        <v>463</v>
-      </c>
-      <c r="B54" s="83">
-        <v>1</v>
-      </c>
-      <c r="C54" s="83" t="str">
-        <f>IF(VLOOKUP(A54,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
-        <v>Sim</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="83" t="s">
-        <v>464</v>
-      </c>
-      <c r="B55" s="83">
-        <v>7.2222222222222229E-2</v>
-      </c>
-      <c r="C55" s="83" t="str">
-        <f>IF(VLOOKUP(A55,Verificação_Parametros!$A:$B,2,FALSE),"Sim","Não")</f>
-        <v>Sim</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C55" xr:uid="{E72623EE-AF76-4665-8E1C-61480EAE2A81}"/>
+  <autoFilter ref="A1:C52" xr:uid="{E72623EE-AF76-4665-8E1C-61480EAE2A81}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -38317,7 +38281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Função para criar template de entrada de dados
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3007" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3009" uniqueCount="566">
   <si>
     <t>Ano</t>
   </si>
@@ -1801,6 +1801,12 @@
   </si>
   <si>
     <t>Obrigatorio</t>
+  </si>
+  <si>
+    <t>NomeAnalista</t>
+  </si>
+  <si>
+    <t>Pedro Lima</t>
   </si>
 </sst>
 </file>
@@ -2112,7 +2118,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2248,6 +2254,9 @@
     <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2755,7 +2764,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D83D282-F75C-4952-B6E5-FA904FFBD51F}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10549,28 +10560,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>251</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="96" t="s">
         <v>437</v>
       </c>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95" t="s">
+      <c r="C1" s="96"/>
+      <c r="D1" s="96" t="s">
         <v>438</v>
       </c>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95" t="s">
+      <c r="E1" s="96"/>
+      <c r="F1" s="96" t="s">
         <v>439</v>
       </c>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96"/>
+      <c r="A2" s="97"/>
       <c r="B2" s="55" t="s">
         <v>435</v>
       </c>
@@ -21924,9 +21935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A87" sqref="A86:A87"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -23348,7 +23357,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C159" sqref="C159"/>
+      <selection pane="bottomLeft" activeCell="C152" sqref="C152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38233,7 +38242,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -38242,10 +38251,11 @@
     <col min="1" max="1" width="11.42578125" style="70" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="69" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" style="69" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="69"/>
+    <col min="4" max="4" width="13.7109375" style="69" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="69"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
         <v>3</v>
       </c>
@@ -38255,8 +38265,11 @@
       <c r="C1" s="68" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="95" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="68">
         <v>2017</v>
       </c>
@@ -38266,8 +38279,11 @@
       <c r="C2" s="69">
         <v>1800</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="11" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="68"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Usando média como parâmetro das constantes
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7470" tabRatio="749" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7470" tabRatio="749" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constantes" sheetId="36" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2982" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2984" uniqueCount="568">
   <si>
     <t>Ano</t>
   </si>
@@ -1807,16 +1807,23 @@
   </si>
   <si>
     <t>DifPorIniciativa</t>
+  </si>
+  <si>
+    <t>Verificação Normal Truncada</t>
+  </si>
+  <si>
+    <t>Verificação Triangular</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="29" x14ac:knownFonts="1">
     <font>
@@ -2118,7 +2125,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2256,13 +2263,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -10582,28 +10590,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>251</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="96" t="s">
         <v>437</v>
       </c>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95" t="s">
+      <c r="C1" s="96"/>
+      <c r="D1" s="96" t="s">
         <v>438</v>
       </c>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95" t="s">
+      <c r="E1" s="96"/>
+      <c r="F1" s="96" t="s">
         <v>439</v>
       </c>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96"/>
+      <c r="A2" s="97"/>
       <c r="B2" s="55" t="s">
         <v>435</v>
       </c>
@@ -23375,18 +23383,18 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:Q149"/>
+  <dimension ref="A1:S149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" style="85" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="85" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="85" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="85" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" style="85" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="85" customWidth="1"/>
     <col min="6" max="7" width="13.5703125" style="85" bestFit="1" customWidth="1"/>
@@ -23398,10 +23406,12 @@
     <col min="13" max="13" width="76.42578125" style="85" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="9.140625" style="85"/>
     <col min="17" max="17" width="21" style="85" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="85"/>
+    <col min="18" max="18" width="28.42578125" style="85" customWidth="1"/>
+    <col min="19" max="19" width="26.85546875" style="85" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="85"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="84" t="s">
         <v>4</v>
       </c>
@@ -23432,7 +23442,7 @@
       <c r="J1" s="84" t="s">
         <v>455</v>
       </c>
-      <c r="K1" s="97" t="s">
+      <c r="K1" s="95" t="s">
         <v>565</v>
       </c>
       <c r="L1" s="84" t="s">
@@ -23453,8 +23463,14 @@
       <c r="Q1" s="84" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R1" s="95" t="s">
+        <v>566</v>
+      </c>
+      <c r="S1" s="95" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="86" t="s">
         <v>83</v>
       </c>
@@ -23466,7 +23482,7 @@
         <v>453</v>
       </c>
       <c r="D2" s="86">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="E2" s="86">
         <v>5.0000000000000001E-3</v>
@@ -23518,8 +23534,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A2)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R2" s="86" t="b">
+        <f>AND(G2&gt;D2,F2 &lt; D2)</f>
+        <v>1</v>
+      </c>
+      <c r="S2" s="86" t="b">
+        <f>AND(F2&gt;E2,D2 &lt; E2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="86" t="s">
         <v>219</v>
       </c>
@@ -23570,8 +23594,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A3)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R3" s="86" t="b">
+        <f t="shared" ref="R3:R66" si="1">AND(G3&gt;D3,F3 &lt; D3)</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="86" t="b">
+        <f t="shared" ref="S3:S66" si="2">AND(F3&gt;E3,D3 &lt; E3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="86" t="s">
         <v>232</v>
       </c>
@@ -23626,8 +23658,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A4)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R4" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S4" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="86" t="s">
         <v>236</v>
       </c>
@@ -23682,8 +23722,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A5)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R5" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S5" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="86" t="s">
         <v>224</v>
       </c>
@@ -23738,8 +23786,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A6)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R6" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S6" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="86" t="s">
         <v>228</v>
       </c>
@@ -23785,8 +23841,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A7)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R7" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S7" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="86" t="s">
         <v>233</v>
       </c>
@@ -23841,8 +23905,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A8)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R8" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S8" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="86" t="s">
         <v>237</v>
       </c>
@@ -23897,8 +23969,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A9)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R9" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S9" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="86" t="s">
         <v>225</v>
       </c>
@@ -23953,8 +24033,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A10)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R10" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S10" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="86" t="s">
         <v>229</v>
       </c>
@@ -24009,8 +24097,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A11)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R11" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S11" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="86" t="s">
         <v>234</v>
       </c>
@@ -24065,8 +24161,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A12)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R12" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S12" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="86" t="s">
         <v>238</v>
       </c>
@@ -24121,8 +24225,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A13)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R13" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S13" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="86" t="s">
         <v>226</v>
       </c>
@@ -24177,8 +24289,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A14)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R14" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S14" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="86" t="s">
         <v>230</v>
       </c>
@@ -24233,8 +24353,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A15)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R15" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S15" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="86" t="s">
         <v>235</v>
       </c>
@@ -24289,8 +24417,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A16)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R16" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S16" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="86" t="s">
         <v>239</v>
       </c>
@@ -24345,8 +24481,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A17)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R17" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S17" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="86" t="s">
         <v>227</v>
       </c>
@@ -24401,8 +24545,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A18)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R18" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S18" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="86" t="s">
         <v>231</v>
       </c>
@@ -24457,8 +24609,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A19)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R19" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S19" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="86" t="s">
         <v>49</v>
       </c>
@@ -24514,8 +24674,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A20)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R20" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S20" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="86" t="s">
         <v>83</v>
       </c>
@@ -24546,7 +24714,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="86" t="str">
-        <f t="shared" ref="L21:L36" si="1">IF(AND(C21="normal",NOT(COUNT(D21:E21)=2)),"Dados Incorretos",
+        <f t="shared" ref="L21:L36" si="3">IF(AND(C21="normal",NOT(COUNT(D21:E21)=2)),"Dados Incorretos",
 IF(AND(C21="triangular",NOT(COUNT(D21:F21)=3)),"Dados Incorretos",
 IF(AND(C21="poisson",NOT(COUNT(D21:E21)=1)),"Dados Incorretos",
 IF(AND(C21="normaltruncada",NOT(COUNT(D21:G21)=4)),"Dados Incorretos",
@@ -24572,8 +24740,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A21)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R21" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S21" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="86" t="s">
         <v>219</v>
       </c>
@@ -24599,7 +24775,7 @@
         <v>1</v>
       </c>
       <c r="L22" s="86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="M22" s="86" t="str">
@@ -24620,8 +24796,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A22)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R22" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S22" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="86" t="s">
         <v>232</v>
       </c>
@@ -24655,7 +24839,7 @@
         <v>1</v>
       </c>
       <c r="L23" s="86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="M23" s="86" t="str">
@@ -24670,8 +24854,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A23)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R23" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S23" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="86" t="s">
         <v>236</v>
       </c>
@@ -24705,7 +24897,7 @@
         <v>1</v>
       </c>
       <c r="L24" s="86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="M24" s="86" t="str">
@@ -24720,8 +24912,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A24)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R24" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S24" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="86" t="s">
         <v>224</v>
       </c>
@@ -24755,7 +24955,7 @@
         <v>1</v>
       </c>
       <c r="L25" s="86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="M25" s="86" t="str">
@@ -24770,8 +24970,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A25)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R25" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S25" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="86" t="s">
         <v>228</v>
       </c>
@@ -24797,7 +25005,7 @@
         <v>1</v>
       </c>
       <c r="L26" s="86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="M26" s="86" t="str">
@@ -24812,8 +25020,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A26)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R26" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S26" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="86" t="s">
         <v>233</v>
       </c>
@@ -24847,7 +25063,7 @@
         <v>1</v>
       </c>
       <c r="L27" s="86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="M27" s="86" t="str">
@@ -24862,8 +25078,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A27)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R27" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S27" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="86" t="s">
         <v>237</v>
       </c>
@@ -24897,7 +25121,7 @@
         <v>1</v>
       </c>
       <c r="L28" s="86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="M28" s="86" t="str">
@@ -24912,8 +25136,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A28)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R28" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S28" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="86" t="s">
         <v>225</v>
       </c>
@@ -24947,7 +25179,7 @@
         <v>1</v>
       </c>
       <c r="L29" s="86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="M29" s="86" t="str">
@@ -24962,8 +25194,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A29)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R29" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S29" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="86" t="s">
         <v>229</v>
       </c>
@@ -24997,7 +25237,7 @@
         <v>1</v>
       </c>
       <c r="L30" s="86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="M30" s="86" t="str">
@@ -25012,8 +25252,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A30)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R30" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S30" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="86" t="s">
         <v>234</v>
       </c>
@@ -25047,7 +25295,7 @@
         <v>1</v>
       </c>
       <c r="L31" s="86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="M31" s="86" t="str">
@@ -25062,8 +25310,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A31)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R31" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S31" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="86" t="s">
         <v>238</v>
       </c>
@@ -25097,7 +25353,7 @@
         <v>1</v>
       </c>
       <c r="L32" s="86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="M32" s="86" t="str">
@@ -25112,8 +25368,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A32)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R32" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S32" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="86" t="s">
         <v>226</v>
       </c>
@@ -25147,7 +25411,7 @@
         <v>1</v>
       </c>
       <c r="L33" s="86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="M33" s="86" t="str">
@@ -25162,8 +25426,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A33)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R33" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S33" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="86" t="s">
         <v>230</v>
       </c>
@@ -25197,7 +25469,7 @@
         <v>1</v>
       </c>
       <c r="L34" s="86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="M34" s="86" t="str">
@@ -25212,8 +25484,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A34)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R34" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S34" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="86" t="s">
         <v>235</v>
       </c>
@@ -25247,7 +25527,7 @@
         <v>1</v>
       </c>
       <c r="L35" s="86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="M35" s="86" t="str">
@@ -25262,8 +25542,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A35)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R35" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S35" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="86" t="s">
         <v>239</v>
       </c>
@@ -25297,7 +25585,7 @@
         <v>1</v>
       </c>
       <c r="L36" s="86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="M36" s="86" t="str">
@@ -25312,8 +25600,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A36)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R36" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S36" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="86" t="s">
         <v>227</v>
       </c>
@@ -25347,7 +25643,7 @@
         <v>1</v>
       </c>
       <c r="L37" s="86" t="str">
-        <f t="shared" ref="L37:L44" si="2">IF(AND(C37="normal",NOT(COUNT(D37:E37)=2)),"Dados Incorretos",
+        <f t="shared" ref="L37:L44" si="4">IF(AND(C37="normal",NOT(COUNT(D37:E37)=2)),"Dados Incorretos",
 IF(AND(C37="triangular",NOT(COUNT(D37:F37)=3)),"Dados Incorretos",
 IF(AND(C37="poisson",NOT(COUNT(D37:E37)=1)),"Dados Incorretos",
 IF(AND(C37="normaltruncada",NOT(COUNT(D37:G37)=4)),"Dados Incorretos",
@@ -25367,8 +25663,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A37)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R37" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S37" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="86" t="s">
         <v>231</v>
       </c>
@@ -25402,7 +25706,7 @@
         <v>1</v>
       </c>
       <c r="L38" s="86" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>OK</v>
       </c>
       <c r="M38" s="86" t="str">
@@ -25417,8 +25721,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A38)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R38" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S38" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="86" t="s">
         <v>49</v>
       </c>
@@ -25453,7 +25765,7 @@
         <v>1</v>
       </c>
       <c r="L39" s="86" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>OK</v>
       </c>
       <c r="M39" s="86" t="str">
@@ -25468,8 +25780,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A39)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R39" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S39" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="86" t="s">
         <v>83</v>
       </c>
@@ -25500,7 +25820,7 @@
         <v>1</v>
       </c>
       <c r="L40" s="86" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>OK</v>
       </c>
       <c r="M40" s="86" t="str">
@@ -25521,8 +25841,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A40)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R40" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S40" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="86" t="s">
         <v>219</v>
       </c>
@@ -25548,7 +25876,7 @@
         <v>1</v>
       </c>
       <c r="L41" s="86" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>OK</v>
       </c>
       <c r="M41" s="86" t="str">
@@ -25569,8 +25897,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A41)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R41" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S41" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="86" t="s">
         <v>232</v>
       </c>
@@ -25604,7 +25940,7 @@
         <v>1</v>
       </c>
       <c r="L42" s="86" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>OK</v>
       </c>
       <c r="M42" s="86" t="str">
@@ -25619,8 +25955,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A42)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R42" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S42" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="86" t="s">
         <v>236</v>
       </c>
@@ -25654,7 +25998,7 @@
         <v>1</v>
       </c>
       <c r="L43" s="86" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>OK</v>
       </c>
       <c r="M43" s="86" t="str">
@@ -25669,8 +26013,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A43)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R43" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S43" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="86" t="s">
         <v>224</v>
       </c>
@@ -25704,7 +26056,7 @@
         <v>1</v>
       </c>
       <c r="L44" s="86" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>OK</v>
       </c>
       <c r="M44" s="86" t="str">
@@ -25719,8 +26071,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A44)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" s="86" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R44" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S44" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" s="86" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="86" t="s">
         <v>228</v>
       </c>
@@ -25746,7 +26106,7 @@
         <v>1</v>
       </c>
       <c r="L45" s="86" t="str">
-        <f t="shared" ref="L45:L59" si="3">IF(AND(C45="normal",NOT(COUNT(D45:E45)=2)),"Dados Incorretos",
+        <f t="shared" ref="L45:L59" si="5">IF(AND(C45="normal",NOT(COUNT(D45:E45)=2)),"Dados Incorretos",
 IF(AND(C45="triangular",NOT(COUNT(D45:F45)=3)),"Dados Incorretos",
 IF(AND(C45="poisson",NOT(COUNT(D45:E45)=1)),"Dados Incorretos",
 IF(AND(C45="normaltruncada",NOT(COUNT(D45:G45)=4)),"Dados Incorretos",
@@ -25766,8 +26126,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A45)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R45" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S45" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="86" t="s">
         <v>233</v>
       </c>
@@ -25801,7 +26169,7 @@
         <v>1</v>
       </c>
       <c r="L46" s="86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="M46" s="86" t="str">
@@ -25816,8 +26184,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A46)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R46" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S46" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="86" t="s">
         <v>237</v>
       </c>
@@ -25851,7 +26227,7 @@
         <v>1</v>
       </c>
       <c r="L47" s="86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="M47" s="86" t="str">
@@ -25866,8 +26242,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A47)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R47" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S47" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="86" t="s">
         <v>225</v>
       </c>
@@ -25901,7 +26285,7 @@
         <v>1</v>
       </c>
       <c r="L48" s="86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="M48" s="86" t="str">
@@ -25916,8 +26300,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A48)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R48" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S48" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="86" t="s">
         <v>229</v>
       </c>
@@ -25951,7 +26343,7 @@
         <v>1</v>
       </c>
       <c r="L49" s="86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="M49" s="86" t="str">
@@ -25966,8 +26358,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A49)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R49" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S49" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="86" t="s">
         <v>234</v>
       </c>
@@ -26001,7 +26401,7 @@
         <v>1</v>
       </c>
       <c r="L50" s="86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="M50" s="86" t="str">
@@ -26016,8 +26416,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A50)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R50" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S50" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="86" t="s">
         <v>238</v>
       </c>
@@ -26051,7 +26459,7 @@
         <v>1</v>
       </c>
       <c r="L51" s="86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="M51" s="86" t="str">
@@ -26066,8 +26474,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A51)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R51" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S51" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="86" t="s">
         <v>226</v>
       </c>
@@ -26101,7 +26517,7 @@
         <v>1</v>
       </c>
       <c r="L52" s="86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="M52" s="86" t="str">
@@ -26116,8 +26532,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A52)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R52" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S52" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="86" t="s">
         <v>230</v>
       </c>
@@ -26151,7 +26575,7 @@
         <v>1</v>
       </c>
       <c r="L53" s="86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="M53" s="86" t="str">
@@ -26166,8 +26590,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A53)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R53" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S53" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="86" t="s">
         <v>235</v>
       </c>
@@ -26201,7 +26633,7 @@
         <v>1</v>
       </c>
       <c r="L54" s="86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="M54" s="86" t="str">
@@ -26216,8 +26648,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A54)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R54" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S54" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="86" t="s">
         <v>239</v>
       </c>
@@ -26251,7 +26691,7 @@
         <v>1</v>
       </c>
       <c r="L55" s="86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="M55" s="86" t="str">
@@ -26266,8 +26706,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A55)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R55" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S55" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="86" t="s">
         <v>227</v>
       </c>
@@ -26301,7 +26749,7 @@
         <v>1</v>
       </c>
       <c r="L56" s="86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="M56" s="86" t="str">
@@ -26316,8 +26764,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A56)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R56" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S56" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="86" t="s">
         <v>231</v>
       </c>
@@ -26351,7 +26807,7 @@
         <v>1</v>
       </c>
       <c r="L57" s="86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="M57" s="86" t="str">
@@ -26366,8 +26822,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A57)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R57" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S57" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="86" t="s">
         <v>49</v>
       </c>
@@ -26402,7 +26866,7 @@
         <v>1</v>
       </c>
       <c r="L58" s="86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="M58" s="86" t="str">
@@ -26417,8 +26881,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A58)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R58" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S58" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="86" t="s">
         <v>83</v>
       </c>
@@ -26449,7 +26921,7 @@
         <v>1</v>
       </c>
       <c r="L59" s="86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="M59" s="86" t="str">
@@ -26470,8 +26942,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A59)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R59" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S59" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="86" t="s">
         <v>219</v>
       </c>
@@ -26497,7 +26977,7 @@
         <v>1</v>
       </c>
       <c r="L60" s="86" t="str">
-        <f t="shared" ref="L60:L77" si="4">IF(AND(C60="normal",NOT(COUNT(D60:E60)=2)),"Dados Incorretos",
+        <f t="shared" ref="L60:L77" si="6">IF(AND(C60="normal",NOT(COUNT(D60:E60)=2)),"Dados Incorretos",
 IF(AND(C60="triangular",NOT(COUNT(D60:F60)=3)),"Dados Incorretos",
 IF(AND(C60="poisson",NOT(COUNT(D60:E60)=1)),"Dados Incorretos",
 IF(AND(C60="normaltruncada",NOT(COUNT(D60:G60)=4)),"Dados Incorretos",
@@ -26523,8 +27003,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A60)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R60" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S60" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="86" t="s">
         <v>232</v>
       </c>
@@ -26558,7 +27046,7 @@
         <v>1</v>
       </c>
       <c r="L61" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M61" s="86" t="str">
@@ -26573,8 +27061,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A61)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R61" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S61" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="86" t="s">
         <v>236</v>
       </c>
@@ -26608,7 +27104,7 @@
         <v>1</v>
       </c>
       <c r="L62" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M62" s="86" t="str">
@@ -26623,8 +27119,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A62)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R62" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S62" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="86" t="s">
         <v>224</v>
       </c>
@@ -26658,7 +27162,7 @@
         <v>1</v>
       </c>
       <c r="L63" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M63" s="86" t="str">
@@ -26673,8 +27177,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A63)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R63" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S63" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="86" t="s">
         <v>228</v>
       </c>
@@ -26700,7 +27212,7 @@
         <v>1</v>
       </c>
       <c r="L64" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M64" s="86" t="str">
@@ -26715,8 +27227,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A64)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R64" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S64" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="86" t="s">
         <v>233</v>
       </c>
@@ -26750,7 +27270,7 @@
         <v>1</v>
       </c>
       <c r="L65" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M65" s="86" t="str">
@@ -26765,8 +27285,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A65)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R65" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S65" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="86" t="s">
         <v>237</v>
       </c>
@@ -26800,7 +27328,7 @@
         <v>1</v>
       </c>
       <c r="L66" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M66" s="86" t="str">
@@ -26815,8 +27343,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A66)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R66" s="86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S66" s="86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="86" t="s">
         <v>225</v>
       </c>
@@ -26850,7 +27386,7 @@
         <v>1</v>
       </c>
       <c r="L67" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M67" s="86" t="str">
@@ -26865,8 +27401,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A67)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R67" s="86" t="b">
+        <f t="shared" ref="R67:R130" si="7">AND(G67&gt;D67,F67 &lt; D67)</f>
+        <v>1</v>
+      </c>
+      <c r="S67" s="86" t="b">
+        <f t="shared" ref="S67:S130" si="8">AND(F67&gt;E67,D67 &lt; E67)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="86" t="s">
         <v>229</v>
       </c>
@@ -26900,7 +27444,7 @@
         <v>1</v>
       </c>
       <c r="L68" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M68" s="86" t="str">
@@ -26915,8 +27459,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A68)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R68" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S68" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="86" t="s">
         <v>234</v>
       </c>
@@ -26950,7 +27502,7 @@
         <v>1</v>
       </c>
       <c r="L69" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M69" s="86" t="str">
@@ -26965,8 +27517,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A69)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R69" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S69" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="86" t="s">
         <v>238</v>
       </c>
@@ -27000,7 +27560,7 @@
         <v>1</v>
       </c>
       <c r="L70" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M70" s="86" t="str">
@@ -27015,8 +27575,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A70)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R70" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S70" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="86" t="s">
         <v>226</v>
       </c>
@@ -27050,7 +27618,7 @@
         <v>1</v>
       </c>
       <c r="L71" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M71" s="86" t="str">
@@ -27065,8 +27633,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A71)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R71" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S71" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="86" t="s">
         <v>230</v>
       </c>
@@ -27100,7 +27676,7 @@
         <v>1</v>
       </c>
       <c r="L72" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M72" s="86" t="str">
@@ -27115,8 +27691,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A72)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R72" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S72" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="86" t="s">
         <v>235</v>
       </c>
@@ -27150,7 +27734,7 @@
         <v>1</v>
       </c>
       <c r="L73" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M73" s="86" t="str">
@@ -27165,8 +27749,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A73)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R73" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S73" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="86" t="s">
         <v>239</v>
       </c>
@@ -27200,7 +27792,7 @@
         <v>1</v>
       </c>
       <c r="L74" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M74" s="86" t="str">
@@ -27215,8 +27807,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A74)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R74" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S74" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="86" t="s">
         <v>227</v>
       </c>
@@ -27250,7 +27850,7 @@
         <v>1</v>
       </c>
       <c r="L75" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M75" s="86" t="str">
@@ -27265,8 +27865,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A75)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R75" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S75" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="86" t="s">
         <v>231</v>
       </c>
@@ -27300,7 +27908,7 @@
         <v>1</v>
       </c>
       <c r="L76" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M76" s="86" t="str">
@@ -27315,8 +27923,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A76)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:17" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="R76" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S76" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" s="86" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="86" t="s">
         <v>49</v>
       </c>
@@ -27351,7 +27967,7 @@
         <v>1</v>
       </c>
       <c r="L77" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>OK</v>
       </c>
       <c r="M77" s="86" t="str">
@@ -27366,8 +27982,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A77)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R77" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S77" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="88" t="s">
         <v>469</v>
       </c>
@@ -27406,7 +28030,7 @@
         <v>0</v>
       </c>
       <c r="L78" s="86" t="str">
-        <f t="shared" ref="L78:L97" si="5">IF(AND(C78="normal",NOT(COUNT(D78:E78)=2)),"Dados Incorretos",
+        <f t="shared" ref="L78:L97" si="9">IF(AND(C78="normal",NOT(COUNT(D78:E78)=2)),"Dados Incorretos",
 IF(AND(C78="triangular",NOT(COUNT(D78:F78)=3)),"Dados Incorretos",
 IF(AND(C78="poisson",NOT(COUNT(D78:E78)=1)),"Dados Incorretos",
 IF(AND(C78="normaltruncada",NOT(COUNT(D78:G78)=4)),"Dados Incorretos",
@@ -27426,8 +28050,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A78)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R78" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S78" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="88" t="s">
         <v>470</v>
       </c>
@@ -27466,7 +28098,7 @@
         <v>0</v>
       </c>
       <c r="L79" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M79" s="86" t="str">
@@ -27481,8 +28113,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A79)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R79" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S79" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="88" t="s">
         <v>471</v>
       </c>
@@ -27521,7 +28161,7 @@
         <v>0</v>
       </c>
       <c r="L80" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M80" s="86" t="str">
@@ -27536,8 +28176,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A80)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R80" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S80" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="88" t="s">
         <v>473</v>
       </c>
@@ -27575,7 +28223,7 @@
         <v>0</v>
       </c>
       <c r="L81" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M81" s="86" t="str">
@@ -27590,8 +28238,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A81)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R81" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S81" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="88" t="s">
         <v>472</v>
       </c>
@@ -27602,11 +28258,16 @@
       <c r="C82" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="D82" s="91">
-        <v>0</v>
-      </c>
-      <c r="E82" s="91">
-        <v>0</v>
+      <c r="D82" s="98">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E82" s="98">
+        <f>D82*1.1</f>
+        <v>1.1000000000000001E-5</v>
+      </c>
+      <c r="F82" s="98">
+        <f>E82*1.1</f>
+        <v>1.2100000000000003E-5</v>
       </c>
       <c r="H82" s="86">
         <v>0</v>
@@ -27623,8 +28284,8 @@
         <v>1</v>
       </c>
       <c r="L82" s="86" t="str">
-        <f t="shared" si="5"/>
-        <v>Dados Incorretos</v>
+        <f t="shared" si="9"/>
+        <v>OK</v>
       </c>
       <c r="M82" s="86" t="str">
         <f>VLOOKUP(C82,Distribuições!$A$1:$F$13,6,FALSE)</f>
@@ -27638,8 +28299,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A82)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R82" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S82" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="88" t="s">
         <v>469</v>
       </c>
@@ -27668,7 +28337,7 @@
       </c>
       <c r="K83" s="86"/>
       <c r="L83" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M83" s="86" t="str">
@@ -27683,8 +28352,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A83)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R83" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S83" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="88" t="s">
         <v>470</v>
       </c>
@@ -27713,7 +28390,7 @@
       </c>
       <c r="K84" s="86"/>
       <c r="L84" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M84" s="86" t="str">
@@ -27728,8 +28405,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A84)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R84" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S84" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="88" t="s">
         <v>471</v>
       </c>
@@ -27758,7 +28443,7 @@
       </c>
       <c r="K85" s="86"/>
       <c r="L85" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M85" s="86" t="str">
@@ -27773,8 +28458,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A85)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R85" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S85" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="88" t="s">
         <v>473</v>
       </c>
@@ -27803,7 +28496,7 @@
       </c>
       <c r="K86" s="86"/>
       <c r="L86" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M86" s="86" t="str">
@@ -27818,8 +28511,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A86)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R86" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S86" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="88" t="s">
         <v>472</v>
       </c>
@@ -27848,7 +28549,7 @@
       </c>
       <c r="K87" s="86"/>
       <c r="L87" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M87" s="86" t="str">
@@ -27863,8 +28564,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A87)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R87" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S87" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="88" t="s">
         <v>469</v>
       </c>
@@ -27893,7 +28602,7 @@
       </c>
       <c r="K88" s="86"/>
       <c r="L88" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M88" s="86" t="str">
@@ -27908,8 +28617,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A88)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R88" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S88" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="88" t="s">
         <v>470</v>
       </c>
@@ -27938,7 +28655,7 @@
       </c>
       <c r="K89" s="86"/>
       <c r="L89" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M89" s="86" t="str">
@@ -27953,8 +28670,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A89)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R89" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S89" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="88" t="s">
         <v>471</v>
       </c>
@@ -27983,7 +28708,7 @@
       </c>
       <c r="K90" s="86"/>
       <c r="L90" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M90" s="86" t="str">
@@ -27998,8 +28723,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A90)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R90" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S90" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="88" t="s">
         <v>473</v>
       </c>
@@ -28028,7 +28761,7 @@
       </c>
       <c r="K91" s="86"/>
       <c r="L91" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M91" s="86" t="str">
@@ -28043,8 +28776,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A91)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R91" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S91" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" s="88" t="s">
         <v>472</v>
       </c>
@@ -28073,7 +28814,7 @@
       </c>
       <c r="K92" s="86"/>
       <c r="L92" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M92" s="86" t="str">
@@ -28088,8 +28829,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A92)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R92" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S92" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" s="88" t="s">
         <v>469</v>
       </c>
@@ -28118,7 +28867,7 @@
       </c>
       <c r="K93" s="86"/>
       <c r="L93" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M93" s="86" t="str">
@@ -28133,8 +28882,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A93)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R93" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S93" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" s="88" t="s">
         <v>470</v>
       </c>
@@ -28163,7 +28920,7 @@
       </c>
       <c r="K94" s="86"/>
       <c r="L94" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M94" s="86" t="str">
@@ -28178,8 +28935,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A94)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R94" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S94" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" s="88" t="s">
         <v>471</v>
       </c>
@@ -28208,7 +28973,7 @@
       </c>
       <c r="K95" s="86"/>
       <c r="L95" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M95" s="86" t="str">
@@ -28223,8 +28988,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A95)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R95" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S95" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" s="88" t="s">
         <v>473</v>
       </c>
@@ -28253,7 +29026,7 @@
       </c>
       <c r="K96" s="86"/>
       <c r="L96" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M96" s="86" t="str">
@@ -28268,8 +29041,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A96)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R96" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S96" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" s="88" t="s">
         <v>472</v>
       </c>
@@ -28298,7 +29079,7 @@
       </c>
       <c r="K97" s="86"/>
       <c r="L97" s="86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>OK</v>
       </c>
       <c r="M97" s="86" t="str">
@@ -28313,8 +29094,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A97)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R97" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S97" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
         <v>548</v>
       </c>
@@ -28352,7 +29141,7 @@
         <v>0</v>
       </c>
       <c r="L98" s="86" t="str">
-        <f t="shared" ref="L98:L117" si="6">IF(AND(C98="normal",NOT(COUNT(D98:E98)=2)),"Dados Incorretos",
+        <f t="shared" ref="L98:L117" si="10">IF(AND(C98="normal",NOT(COUNT(D98:E98)=2)),"Dados Incorretos",
 IF(AND(C98="triangular",NOT(COUNT(D98:F98)=3)),"Dados Incorretos",
 IF(AND(C98="poisson",NOT(COUNT(D98:E98)=1)),"Dados Incorretos",
 IF(AND(C98="normaltruncada",NOT(COUNT(D98:G98)=4)),"Dados Incorretos",
@@ -28372,8 +29161,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A98)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R98" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S98" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
         <v>553</v>
       </c>
@@ -28411,7 +29208,7 @@
         <v>0</v>
       </c>
       <c r="L99" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M99" s="86" t="str">
@@ -28426,8 +29223,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A99)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R99" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S99" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
         <v>554</v>
       </c>
@@ -28465,7 +29270,7 @@
         <v>0</v>
       </c>
       <c r="L100" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M100" s="86" t="str">
@@ -28480,8 +29285,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A100)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R100" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S100" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
         <v>555</v>
       </c>
@@ -28519,7 +29332,7 @@
         <v>0</v>
       </c>
       <c r="L101" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M101" s="86" t="str">
@@ -28534,8 +29347,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A101)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R101" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S101" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
         <v>556</v>
       </c>
@@ -28573,7 +29394,7 @@
         <v>0</v>
       </c>
       <c r="L102" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M102" s="86" t="str">
@@ -28588,8 +29409,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A102)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R102" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S102" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
         <v>547</v>
       </c>
@@ -28619,7 +29448,7 @@
         <v>1</v>
       </c>
       <c r="L103" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M103" s="86" t="str">
@@ -28634,8 +29463,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A103)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R103" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S103" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
         <v>549</v>
       </c>
@@ -28665,7 +29502,7 @@
         <v>1</v>
       </c>
       <c r="L104" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M104" s="86" t="str">
@@ -28680,8 +29517,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A104)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R104" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S104" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
         <v>550</v>
       </c>
@@ -28711,7 +29556,7 @@
         <v>1</v>
       </c>
       <c r="L105" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M105" s="86" t="str">
@@ -28726,8 +29571,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A105)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R105" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S105" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
         <v>551</v>
       </c>
@@ -28757,7 +29610,7 @@
         <v>1</v>
       </c>
       <c r="L106" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M106" s="86" t="str">
@@ -28772,8 +29625,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A106)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R106" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S106" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
         <v>552</v>
       </c>
@@ -28803,7 +29664,7 @@
         <v>1</v>
       </c>
       <c r="L107" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M107" s="86" t="str">
@@ -28818,8 +29679,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A107)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R107" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S107" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
         <v>548</v>
       </c>
@@ -28851,7 +29720,7 @@
       </c>
       <c r="K108" s="86"/>
       <c r="L108" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M108" s="86" t="str">
@@ -28866,8 +29735,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A108)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R108" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S108" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
         <v>553</v>
       </c>
@@ -28899,7 +29776,7 @@
       </c>
       <c r="K109" s="86"/>
       <c r="L109" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M109" s="86" t="str">
@@ -28914,8 +29791,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A109)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R109" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S109" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
         <v>554</v>
       </c>
@@ -28947,7 +29832,7 @@
       </c>
       <c r="K110" s="86"/>
       <c r="L110" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M110" s="86" t="str">
@@ -28962,8 +29847,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A110)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R110" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S110" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
         <v>555</v>
       </c>
@@ -28995,7 +29888,7 @@
       </c>
       <c r="K111" s="86"/>
       <c r="L111" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M111" s="86" t="str">
@@ -29010,8 +29903,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A111)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R111" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S111" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
         <v>556</v>
       </c>
@@ -29043,7 +29944,7 @@
       </c>
       <c r="K112" s="86"/>
       <c r="L112" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M112" s="86" t="str">
@@ -29058,8 +29959,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A112)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R112" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S112" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
         <v>547</v>
       </c>
@@ -29086,7 +29995,7 @@
       </c>
       <c r="K113" s="86"/>
       <c r="L113" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M113" s="86" t="str">
@@ -29101,8 +30010,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A113)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R113" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S113" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
         <v>549</v>
       </c>
@@ -29129,7 +30046,7 @@
       </c>
       <c r="K114" s="86"/>
       <c r="L114" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M114" s="86" t="str">
@@ -29144,8 +30061,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A114)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R114" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S114" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
         <v>550</v>
       </c>
@@ -29172,7 +30097,7 @@
       </c>
       <c r="K115" s="86"/>
       <c r="L115" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M115" s="86" t="str">
@@ -29187,8 +30112,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A115)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R115" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S115" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116" s="11" t="s">
         <v>551</v>
       </c>
@@ -29215,7 +30148,7 @@
       </c>
       <c r="K116" s="86"/>
       <c r="L116" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M116" s="86" t="str">
@@ -29230,8 +30163,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A116)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R116" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S116" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" s="11" t="s">
         <v>552</v>
       </c>
@@ -29258,7 +30199,7 @@
       </c>
       <c r="K117" s="86"/>
       <c r="L117" s="86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>OK</v>
       </c>
       <c r="M117" s="86" t="str">
@@ -29273,8 +30214,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A117)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R117" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S117" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" s="11" t="s">
         <v>548</v>
       </c>
@@ -29306,7 +30255,7 @@
       </c>
       <c r="K118" s="86"/>
       <c r="L118" s="86" t="str">
-        <f t="shared" ref="L118:L137" si="7">IF(AND(C118="normal",NOT(COUNT(D118:E118)=2)),"Dados Incorretos",
+        <f t="shared" ref="L118:L137" si="11">IF(AND(C118="normal",NOT(COUNT(D118:E118)=2)),"Dados Incorretos",
 IF(AND(C118="triangular",NOT(COUNT(D118:F118)=3)),"Dados Incorretos",
 IF(AND(C118="poisson",NOT(COUNT(D118:E118)=1)),"Dados Incorretos",
 IF(AND(C118="normaltruncada",NOT(COUNT(D118:G118)=4)),"Dados Incorretos",
@@ -29326,8 +30275,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A118)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R118" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S118" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" s="11" t="s">
         <v>553</v>
       </c>
@@ -29359,7 +30316,7 @@
       </c>
       <c r="K119" s="86"/>
       <c r="L119" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M119" s="86" t="str">
@@ -29374,8 +30331,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A119)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R119" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S119" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" s="11" t="s">
         <v>554</v>
       </c>
@@ -29407,7 +30372,7 @@
       </c>
       <c r="K120" s="86"/>
       <c r="L120" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M120" s="86" t="str">
@@ -29422,8 +30387,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A120)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R120" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S120" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" s="11" t="s">
         <v>555</v>
       </c>
@@ -29455,7 +30428,7 @@
       </c>
       <c r="K121" s="86"/>
       <c r="L121" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M121" s="86" t="str">
@@ -29470,8 +30443,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A121)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R121" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S121" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" s="11" t="s">
         <v>556</v>
       </c>
@@ -29503,7 +30484,7 @@
       </c>
       <c r="K122" s="86"/>
       <c r="L122" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M122" s="86" t="str">
@@ -29518,8 +30499,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A122)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R122" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S122" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" s="11" t="s">
         <v>547</v>
       </c>
@@ -29546,7 +30535,7 @@
       </c>
       <c r="K123" s="86"/>
       <c r="L123" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M123" s="86" t="str">
@@ -29561,8 +30550,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A123)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R123" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S123" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" s="11" t="s">
         <v>549</v>
       </c>
@@ -29589,7 +30586,7 @@
       </c>
       <c r="K124" s="86"/>
       <c r="L124" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M124" s="86" t="str">
@@ -29604,8 +30601,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A124)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R124" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S124" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" s="11" t="s">
         <v>550</v>
       </c>
@@ -29632,7 +30637,7 @@
       </c>
       <c r="K125" s="86"/>
       <c r="L125" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M125" s="86" t="str">
@@ -29647,8 +30652,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A125)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R125" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S125" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" s="11" t="s">
         <v>551</v>
       </c>
@@ -29675,7 +30688,7 @@
       </c>
       <c r="K126" s="86"/>
       <c r="L126" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M126" s="86" t="str">
@@ -29690,8 +30703,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A126)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R126" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S126" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" s="11" t="s">
         <v>552</v>
       </c>
@@ -29718,7 +30739,7 @@
       </c>
       <c r="K127" s="86"/>
       <c r="L127" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M127" s="86" t="str">
@@ -29733,8 +30754,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A127)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R127" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S127" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128" s="11" t="s">
         <v>548</v>
       </c>
@@ -29766,7 +30795,7 @@
       </c>
       <c r="K128" s="86"/>
       <c r="L128" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M128" s="86" t="str">
@@ -29781,8 +30810,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A128)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R128" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S128" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
         <v>553</v>
       </c>
@@ -29814,7 +30851,7 @@
       </c>
       <c r="K129" s="86"/>
       <c r="L129" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M129" s="86" t="str">
@@ -29829,8 +30866,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A129)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R129" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S129" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" s="11" t="s">
         <v>554</v>
       </c>
@@ -29862,7 +30907,7 @@
       </c>
       <c r="K130" s="86"/>
       <c r="L130" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M130" s="86" t="str">
@@ -29877,8 +30922,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A130)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R130" s="86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S130" s="86" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" s="11" t="s">
         <v>555</v>
       </c>
@@ -29910,7 +30963,7 @@
       </c>
       <c r="K131" s="86"/>
       <c r="L131" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M131" s="86" t="str">
@@ -29925,8 +30978,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A131)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R131" s="86" t="b">
+        <f t="shared" ref="R131:R149" si="12">AND(G131&gt;D131,F131 &lt; D131)</f>
+        <v>0</v>
+      </c>
+      <c r="S131" s="86" t="b">
+        <f t="shared" ref="S131:S149" si="13">AND(F131&gt;E131,D131 &lt; E131)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" s="11" t="s">
         <v>556</v>
       </c>
@@ -29958,7 +31019,7 @@
       </c>
       <c r="K132" s="86"/>
       <c r="L132" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M132" s="86" t="str">
@@ -29973,8 +31034,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A132)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R132" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S132" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" s="11" t="s">
         <v>547</v>
       </c>
@@ -30001,7 +31070,7 @@
       </c>
       <c r="K133" s="86"/>
       <c r="L133" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M133" s="86" t="str">
@@ -30016,8 +31085,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A133)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R133" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S133" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" s="11" t="s">
         <v>549</v>
       </c>
@@ -30044,7 +31121,7 @@
       </c>
       <c r="K134" s="86"/>
       <c r="L134" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M134" s="86" t="str">
@@ -30059,8 +31136,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A134)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R134" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S134" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
         <v>550</v>
       </c>
@@ -30087,7 +31172,7 @@
       </c>
       <c r="K135" s="86"/>
       <c r="L135" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M135" s="86" t="str">
@@ -30102,8 +31187,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A135)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R135" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S135" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" s="11" t="s">
         <v>551</v>
       </c>
@@ -30130,7 +31223,7 @@
       </c>
       <c r="K136" s="86"/>
       <c r="L136" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M136" s="86" t="str">
@@ -30145,8 +31238,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A136)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R136" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S136" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" s="11" t="s">
         <v>552</v>
       </c>
@@ -30173,7 +31274,7 @@
       </c>
       <c r="K137" s="86"/>
       <c r="L137" s="86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M137" s="86" t="str">
@@ -30188,8 +31289,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A137)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R137" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S137" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" s="83" t="s">
         <v>172</v>
       </c>
@@ -30201,10 +31310,13 @@
         <v>36</v>
       </c>
       <c r="D138" s="93">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E138" s="85">
-        <v>0</v>
+        <v>0.01</v>
+      </c>
+      <c r="F138" s="85">
+        <v>0.02</v>
       </c>
       <c r="H138" s="86">
         <v>0</v>
@@ -30221,13 +31333,13 @@
         <v>0</v>
       </c>
       <c r="L138" s="86" t="str">
-        <f t="shared" ref="L138:L149" si="8">IF(AND(C138="normal",NOT(COUNT(D138:E138)=2)),"Dados Incorretos",
+        <f t="shared" ref="L138:L149" si="14">IF(AND(C138="normal",NOT(COUNT(D138:E138)=2)),"Dados Incorretos",
 IF(AND(C138="triangular",NOT(COUNT(D138:F138)=3)),"Dados Incorretos",
 IF(AND(C138="poisson",NOT(COUNT(D138:E138)=1)),"Dados Incorretos",
 IF(AND(C138="normaltruncada",NOT(COUNT(D138:G138)=4)),"Dados Incorretos",
 IF(AND(C138="uniforme",NOT(COUNT(D138:E138)=2)),"Dados Incorretos",
 IF(AND(C138="poisson_percentual_eventos",NOT(COUNT(D138:E138)=1)),"Dados Incorretos","OK"))))))</f>
-        <v>Dados Incorretos</v>
+        <v>OK</v>
       </c>
       <c r="M138" s="86" t="str">
         <f>VLOOKUP(C138,Distribuições!$A$1:$F$13,6,FALSE)</f>
@@ -30241,8 +31353,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A138)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R138" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S138" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139" s="83" t="s">
         <v>172</v>
       </c>
@@ -30251,13 +31371,16 @@
         <v>Sim</v>
       </c>
       <c r="C139" s="65" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D139" s="93">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E139" s="85">
-        <v>0</v>
+        <v>0.01</v>
+      </c>
+      <c r="F139" s="85">
+        <v>0.02</v>
       </c>
       <c r="H139" s="86">
         <v>0</v>
@@ -30271,12 +31394,12 @@
       </c>
       <c r="K139" s="86"/>
       <c r="L139" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>OK</v>
       </c>
       <c r="M139" s="86" t="str">
         <f>VLOOKUP(C139,Distribuições!$A$1:$F$13,6,FALSE)</f>
-        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+        <v>Parametro 1: mínimo, Parametro 2: moda (valor mais provável), Parametro 3: máximo</v>
       </c>
       <c r="N139" s="86">
         <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A139)</f>
@@ -30286,8 +31409,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A139)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R139" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S139" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140" s="83" t="s">
         <v>172</v>
       </c>
@@ -30296,13 +31427,16 @@
         <v>Sim</v>
       </c>
       <c r="C140" s="65" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D140" s="93">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E140" s="85">
-        <v>0</v>
+        <v>0.01</v>
+      </c>
+      <c r="F140" s="85">
+        <v>0.02</v>
       </c>
       <c r="H140" s="86">
         <v>0</v>
@@ -30316,12 +31450,12 @@
       </c>
       <c r="K140" s="86"/>
       <c r="L140" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>OK</v>
       </c>
       <c r="M140" s="86" t="str">
         <f>VLOOKUP(C140,Distribuições!$A$1:$F$13,6,FALSE)</f>
-        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+        <v>Parametro 1: mínimo, Parametro 2: moda (valor mais provável), Parametro 3: máximo</v>
       </c>
       <c r="N140" s="86">
         <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A140)</f>
@@ -30331,8 +31465,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A140)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R140" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S140" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141" s="83" t="s">
         <v>172</v>
       </c>
@@ -30341,13 +31483,16 @@
         <v>Sim</v>
       </c>
       <c r="C141" s="65" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D141" s="93">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E141" s="85">
-        <v>0</v>
+        <v>0.01</v>
+      </c>
+      <c r="F141" s="85">
+        <v>0.02</v>
       </c>
       <c r="H141" s="86">
         <v>0</v>
@@ -30361,12 +31506,12 @@
       </c>
       <c r="K141" s="86"/>
       <c r="L141" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>OK</v>
       </c>
       <c r="M141" s="86" t="str">
         <f>VLOOKUP(C141,Distribuições!$A$1:$F$13,6,FALSE)</f>
-        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+        <v>Parametro 1: mínimo, Parametro 2: moda (valor mais provável), Parametro 3: máximo</v>
       </c>
       <c r="N141" s="86">
         <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A141)</f>
@@ -30376,8 +31521,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A141)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R141" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S141" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A142" s="22" t="s">
         <v>223</v>
       </c>
@@ -30389,10 +31542,13 @@
         <v>36</v>
       </c>
       <c r="D142" s="93">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E142" s="85">
-        <v>0</v>
+        <v>0.01</v>
+      </c>
+      <c r="F142" s="85">
+        <v>0.02</v>
       </c>
       <c r="H142" s="86">
         <v>0</v>
@@ -30409,8 +31565,8 @@
         <v>0</v>
       </c>
       <c r="L142" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v>Dados Incorretos</v>
+        <f t="shared" si="14"/>
+        <v>OK</v>
       </c>
       <c r="M142" s="86" t="str">
         <f>VLOOKUP(C142,Distribuições!$A$1:$F$13,6,FALSE)</f>
@@ -30424,8 +31580,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A142)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R142" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S142" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A143" s="22" t="s">
         <v>223</v>
       </c>
@@ -30434,13 +31598,16 @@
         <v>Sim</v>
       </c>
       <c r="C143" s="65" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D143" s="93">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E143" s="85">
-        <v>0</v>
+        <v>0.01</v>
+      </c>
+      <c r="F143" s="85">
+        <v>0.02</v>
       </c>
       <c r="H143" s="86">
         <v>0</v>
@@ -30454,12 +31621,12 @@
       </c>
       <c r="K143" s="86"/>
       <c r="L143" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>OK</v>
       </c>
       <c r="M143" s="86" t="str">
         <f>VLOOKUP(C143,Distribuições!$A$1:$F$13,6,FALSE)</f>
-        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+        <v>Parametro 1: mínimo, Parametro 2: moda (valor mais provável), Parametro 3: máximo</v>
       </c>
       <c r="N143" s="86">
         <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A143)</f>
@@ -30469,8 +31636,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A143)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R143" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S143" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A144" s="22" t="s">
         <v>223</v>
       </c>
@@ -30479,13 +31654,16 @@
         <v>Sim</v>
       </c>
       <c r="C144" s="65" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D144" s="93">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E144" s="85">
-        <v>0</v>
+        <v>0.01</v>
+      </c>
+      <c r="F144" s="85">
+        <v>0.02</v>
       </c>
       <c r="H144" s="86">
         <v>0</v>
@@ -30499,12 +31677,12 @@
       </c>
       <c r="K144" s="86"/>
       <c r="L144" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>OK</v>
       </c>
       <c r="M144" s="86" t="str">
         <f>VLOOKUP(C144,Distribuições!$A$1:$F$13,6,FALSE)</f>
-        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+        <v>Parametro 1: mínimo, Parametro 2: moda (valor mais provável), Parametro 3: máximo</v>
       </c>
       <c r="N144" s="86">
         <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A144)</f>
@@ -30514,8 +31692,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A144)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R144" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S144" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A145" s="22" t="s">
         <v>223</v>
       </c>
@@ -30524,13 +31710,16 @@
         <v>Sim</v>
       </c>
       <c r="C145" s="65" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D145" s="93">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E145" s="85">
-        <v>0</v>
+        <v>0.01</v>
+      </c>
+      <c r="F145" s="85">
+        <v>0.02</v>
       </c>
       <c r="H145" s="86">
         <v>0</v>
@@ -30544,12 +31733,12 @@
       </c>
       <c r="K145" s="86"/>
       <c r="L145" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>OK</v>
       </c>
       <c r="M145" s="86" t="str">
         <f>VLOOKUP(C145,Distribuições!$A$1:$F$13,6,FALSE)</f>
-        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+        <v>Parametro 1: mínimo, Parametro 2: moda (valor mais provável), Parametro 3: máximo</v>
       </c>
       <c r="N145" s="86">
         <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A145)</f>
@@ -30559,8 +31748,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A145)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R145" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S145" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A146" s="22" t="s">
         <v>154</v>
       </c>
@@ -30572,10 +31769,13 @@
         <v>36</v>
       </c>
       <c r="D146" s="93">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E146" s="85">
-        <v>0</v>
+        <v>0.01</v>
+      </c>
+      <c r="F146" s="85">
+        <v>0.02</v>
       </c>
       <c r="H146" s="86">
         <v>0</v>
@@ -30592,8 +31792,8 @@
         <v>0</v>
       </c>
       <c r="L146" s="86" t="str">
-        <f t="shared" si="8"/>
-        <v>Dados Incorretos</v>
+        <f t="shared" si="14"/>
+        <v>OK</v>
       </c>
       <c r="M146" s="86" t="str">
         <f>VLOOKUP(C146,Distribuições!$A$1:$F$13,6,FALSE)</f>
@@ -30607,8 +31807,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A146)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R146" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S146" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A147" s="22" t="s">
         <v>154</v>
       </c>
@@ -30617,13 +31825,16 @@
         <v>Sim</v>
       </c>
       <c r="C147" s="65" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D147" s="93">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E147" s="85">
-        <v>0</v>
+        <v>0.01</v>
+      </c>
+      <c r="F147" s="85">
+        <v>0.02</v>
       </c>
       <c r="H147" s="86">
         <v>0</v>
@@ -30637,12 +31848,12 @@
       </c>
       <c r="K147" s="86"/>
       <c r="L147" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>OK</v>
       </c>
       <c r="M147" s="86" t="str">
         <f>VLOOKUP(C147,Distribuições!$A$1:$F$13,6,FALSE)</f>
-        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+        <v>Parametro 1: mínimo, Parametro 2: moda (valor mais provável), Parametro 3: máximo</v>
       </c>
       <c r="N147" s="86">
         <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A147)</f>
@@ -30652,8 +31863,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A147)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R147" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S147" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A148" s="22" t="s">
         <v>154</v>
       </c>
@@ -30662,13 +31881,16 @@
         <v>Sim</v>
       </c>
       <c r="C148" s="65" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D148" s="93">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E148" s="85">
-        <v>0</v>
+        <v>0.01</v>
+      </c>
+      <c r="F148" s="85">
+        <v>0.02</v>
       </c>
       <c r="H148" s="86">
         <v>0</v>
@@ -30682,12 +31904,12 @@
       </c>
       <c r="K148" s="86"/>
       <c r="L148" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>OK</v>
       </c>
       <c r="M148" s="86" t="str">
         <f>VLOOKUP(C148,Distribuições!$A$1:$F$13,6,FALSE)</f>
-        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+        <v>Parametro 1: mínimo, Parametro 2: moda (valor mais provável), Parametro 3: máximo</v>
       </c>
       <c r="N148" s="86">
         <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A148)</f>
@@ -30697,8 +31919,16 @@
         <f>COUNTIF(Constantes!$A:$A,Parametros!A148)&gt;0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R148" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S148" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A149" s="22" t="s">
         <v>154</v>
       </c>
@@ -30707,13 +31937,16 @@
         <v>Sim</v>
       </c>
       <c r="C149" s="65" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D149" s="93">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E149" s="85">
-        <v>0</v>
+        <v>0.01</v>
+      </c>
+      <c r="F149" s="85">
+        <v>0.02</v>
       </c>
       <c r="H149" s="86">
         <v>0</v>
@@ -30727,12 +31960,12 @@
       </c>
       <c r="K149" s="86"/>
       <c r="L149" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>OK</v>
       </c>
       <c r="M149" s="86" t="str">
         <f>VLOOKUP(C149,Distribuições!$A$1:$F$13,6,FALSE)</f>
-        <v>Parametro 1: média, Parametro 2: desvio padrão</v>
+        <v>Parametro 1: mínimo, Parametro 2: moda (valor mais provável), Parametro 3: máximo</v>
       </c>
       <c r="N149" s="86">
         <f>COUNTIF(Verificação_Parametros!$A:$A,Parametros!A149)</f>
@@ -30741,6 +31974,14 @@
       <c r="Q149" s="86" t="b">
         <f>COUNTIF(Constantes!$A:$A,Parametros!A149)&gt;0</f>
         <v>0</v>
+      </c>
+      <c r="R149" s="86" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S149" s="86" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -38869,7 +40110,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38936,8 +40177,8 @@
         <v>21</v>
       </c>
       <c r="B5" s="37" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="C5" t="b">
         <f>FALSE</f>

</xml_diff>

<commit_message>
Corrigindo Inconsistência na verificação de dados.
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7470" tabRatio="749" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7470" tabRatio="749" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constantes" sheetId="36" r:id="rId1"/>
@@ -1823,7 +1823,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="29" x14ac:knownFonts="1">
     <font>
@@ -2264,13 +2264,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -10590,28 +10590,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="98" t="s">
         <v>251</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="97" t="s">
         <v>437</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96" t="s">
+      <c r="C1" s="97"/>
+      <c r="D1" s="97" t="s">
         <v>438</v>
       </c>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96" t="s">
+      <c r="E1" s="97"/>
+      <c r="F1" s="97" t="s">
         <v>439</v>
       </c>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="97"/>
+      <c r="A2" s="98"/>
       <c r="B2" s="55" t="s">
         <v>435</v>
       </c>
@@ -23385,9 +23385,9 @@
   </sheetPr>
   <dimension ref="A1:S149"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28258,14 +28258,14 @@
       <c r="C82" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="D82" s="98">
+      <c r="D82" s="96">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="E82" s="98">
+      <c r="E82" s="96">
         <f>D82*1.1</f>
         <v>1.1000000000000001E-5</v>
       </c>
-      <c r="F82" s="98">
+      <c r="F82" s="96">
         <f>E82*1.1</f>
         <v>1.2100000000000003E-5</v>
       </c>
@@ -40109,8 +40109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
alterando arquivo do template
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -51,8 +51,8 @@
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MódulosOpcionais!$A$1:$C$18</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Parametros!$A$1:$R$149</definedName>
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Verificação_Parametros!$A$1:$H$110</definedName>
-    <definedName function="false" hidden="false" name="aaaa" vbProcedure="false">[1]Configs!$D$2</definedName>
-    <definedName function="false" hidden="false" name="AAAAAA" vbProcedure="false">[1]Configs!$C$2</definedName>
+    <definedName function="false" hidden="false" name="aaaa" vbProcedure="false">[4]Configs!$D$2</definedName>
+    <definedName function="false" hidden="false" name="AAAAAA" vbProcedure="false">[4]Configs!$C$2</definedName>
     <definedName function="false" hidden="false" name="Anos_a_Serem_Simulados" vbProcedure="false">configs!#REF!</definedName>
     <definedName function="false" hidden="false" name="Ano_Inicial" vbProcedure="false">Configs!$A$2:$A$2</definedName>
     <definedName function="false" hidden="false" name="CategoriaSAT" vbProcedure="false">configs!#REF!</definedName>
@@ -68,6 +68,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Constantes!$A$1:$C$52</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Constantes!$A$1:$C$52</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Constantes!$A$1:$C$52</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Constantes!$A$1:$C$52</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MódulosOpcionais!$A$1:$C$18</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MódulosOpcionais!$A$1:$C$18</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">MódulosOpcionais!$A$1:$C$18</definedName>
@@ -80,6 +81,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">MódulosOpcionais!$A$1:$C$18</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MódulosOpcionais!$A$1:$C$18</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MódulosOpcionais!$A$1:$C$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MódulosOpcionais!$A$1:$C$18</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Parametros!$A$1:$R$149</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parametros!$A$1:$R$149</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parametros!$A$1:$R$149</definedName>
@@ -92,9 +94,10 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parametros!$A$1:$R$149</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parametros!$A$1:$R$149</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parametros!$A$1:$R$149</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="Anos_a_Serem_Simulados" vbProcedure="false">[2]Configs!$A$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="Ano_Inicial" vbProcedure="false">[2]Configs!$D$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="CategoriaSAT" vbProcedure="false">[2]Configs!$C$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parametros!$A$1:$R$149</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="Anos_a_Serem_Simulados" vbProcedure="false">[5]Configs!$A$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="Ano_Inicial" vbProcedure="false">[5]Configs!$D$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="CategoriaSAT" vbProcedure="false">[5]Configs!$C$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Verificação_Parametros!$A$1:$H$110</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">Verificação_Parametros!$A$1:$H$110</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Verificação_Parametros!$A$1:$H$110</definedName>
@@ -107,6 +110,7 @@
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Verificação_Parametros!$A$1:$H$110</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Verificação_Parametros!$A$1:$H$110</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Verificação_Parametros!$A$1:$H$110</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Verificação_Parametros!$A$1:$H$110</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">Custos!$A$1:$D$18</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">Custos!$A$1:$D$18</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Custos!$A$1:$D$18</definedName>
@@ -119,6 +123,7 @@
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Custos!$A$1:$D$18</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Custos!$A$1:$D$18</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Custos!$A$1:$D$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Custos!$A$1:$D$18</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Modulos!$A$1:$D$26</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">Modulos!$A$1:$D$26</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Modulos!$A$1:$D$26</definedName>
@@ -131,9 +136,10 @@
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Modulos!$A$1:$D$26</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Modulos!$A$1:$D$26</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Modulos!$A$1:$D$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="Anos_a_Serem_Simulados" vbProcedure="false">[3]Configs!$A$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="Ano_Inicial" vbProcedure="false">[3]Configs!$D$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="CategoriaSAT" vbProcedure="false">[3]Configs!$C$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Modulos!$A$1:$D$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="Anos_a_Serem_Simulados" vbProcedure="false">[6]Configs!$A$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="Ano_Inicial" vbProcedure="false">[6]Configs!$D$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="CategoriaSAT" vbProcedure="false">[6]Configs!$C$2</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Cenarios!$A$1:$D$13</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0" vbProcedure="false">Cenarios!$A$1:$D$13</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Cenarios!$A$1:$D$13</definedName>
@@ -146,6 +152,7 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Cenarios!$A$1:$D$13</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Cenarios!$A$1:$D$13</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Cenarios!$A$1:$D$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Cenarios!$A$1:$D$13</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Historico!$A$1:$T$115</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0" vbProcedure="false">Historico!$A$1:$T$115</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Historico!$A$1:$T$115</definedName>
@@ -158,6 +165,7 @@
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Historico!$A$1:$T$115</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Historico!$A$1:$T$115</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Historico!$A$1:$T$115</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Historico!$A$1:$T$115</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">Eventos_Inic!$A$2:$L$19</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0" vbProcedure="false">Eventos_Inic!$A$2:$L$19</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Eventos_Inic!$A$2:$L$19</definedName>
@@ -170,6 +178,7 @@
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Eventos_Inic!$A$2:$L$19</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Eventos_Inic!$A$2:$L$19</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Eventos_Inic!$A$2:$L$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Eventos_Inic!$A$2:$L$19</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">Lista_de_Parâmetros!$A$1:$E$132</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0" vbProcedure="false">Lista_de_Parâmetros!$A$1:$E$132</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Lista_de_Parâmetros!$A$1:$E$132</definedName>
@@ -182,6 +191,7 @@
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Lista_de_Parâmetros!$A$1:$E$132</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Lista_de_Parâmetros!$A$1:$E$132</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Lista_de_Parâmetros!$A$1:$E$132</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Lista_de_Parâmetros!$A$1:$E$132</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase" vbProcedure="false">Funcoes_Inputs!$A$1:$I$226</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0" vbProcedure="false">Funcoes_Inputs!$A$1:$I$226</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Funcoes_Inputs!$A$1:$I$226</definedName>
@@ -194,6 +204,7 @@
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Funcoes_Inputs!$A$1:$I$226</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Funcoes_Inputs!$A$1:$I$226</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Funcoes_Inputs!$A$1:$I$226</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Funcoes_Inputs!$A$1:$I$226</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase" vbProcedure="false">Funcoes_Outputs!$A$1:$C$88</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0" vbProcedure="false">Funcoes_Outputs!$A$1:$C$88</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Funcoes_Outputs!$A$1:$C$88</definedName>
@@ -206,9 +217,10 @@
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Funcoes_Outputs!$A$1:$C$88</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Funcoes_Outputs!$A$1:$C$88</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Funcoes_Outputs!$A$1:$C$88</definedName>
-    <definedName function="false" hidden="false" localSheetId="20" name="Anos_a_Serem_Simulados" vbProcedure="false">[1]Configs!$A$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="20" name="Ano_Inicial" vbProcedure="false">[1]Configs!$D$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="20" name="CategoriaSAT" vbProcedure="false">[1]Configs!$C$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Funcoes_Outputs!$A$1:$C$88</definedName>
+    <definedName function="false" hidden="false" localSheetId="20" name="Anos_a_Serem_Simulados" vbProcedure="false">[4]Configs!$A$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="20" name="Ano_Inicial" vbProcedure="false">[4]Configs!$D$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="20" name="CategoriaSAT" vbProcedure="false">[4]Configs!$C$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2601,19 +2613,19 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -2632,11 +2644,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3472,8 +3484,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3506,11 +3518,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3775,13 +3787,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="78.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="77.6224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3937,20 +3949,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="94.765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="16" min="12" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="93.6836734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="16" min="12" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8685,8 +8697,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10126,25 +10138,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="45" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="45" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="45" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="32" min="23" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="36" min="33" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="37" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="45" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="45" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="45" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.25"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="32" min="23" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="36" min="33" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="37" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10761,19 +10773,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.530612244898"/>
     <col collapsed="false" hidden="true" max="11" min="10" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11605,11 +11617,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="108.668367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="107.454081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14029,16 +14041,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.3673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22196,10 +22208,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23283,10 +23295,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="48.4642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="47.7857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23514,10 +23526,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24268,9 +24280,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24738,8 +24750,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25460,9 +25472,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26146,12 +26158,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26867,27 +26879,27 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.6734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="6" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="76.5408163265306"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="6" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="75.7295918367347"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29897,13 +29909,13 @@
         <v>146</v>
       </c>
       <c r="C36" s="9" t="n">
-        <v>1E-007</v>
+        <v>0</v>
       </c>
       <c r="D36" s="10" t="n">
-        <v>1E-006</v>
+        <v>0</v>
       </c>
       <c r="E36" s="10" t="n">
-        <v>1E-005</v>
+        <v>0</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="1" t="n">
@@ -29942,7 +29954,7 @@
       </c>
       <c r="R36" s="4" t="n">
         <f aca="false">AND(E36&gt;D36,C36 &lt; D36)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29953,13 +29965,13 @@
         <v>146</v>
       </c>
       <c r="C37" s="9" t="n">
-        <v>1E-007</v>
+        <v>0</v>
       </c>
       <c r="D37" s="10" t="n">
-        <v>1E-006</v>
+        <v>0</v>
       </c>
       <c r="E37" s="10" t="n">
-        <v>1E-005</v>
+        <v>0</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="1" t="n">
@@ -29998,7 +30010,7 @@
       </c>
       <c r="R37" s="4" t="n">
         <f aca="false">AND(E37&gt;D37,C37 &lt; D37)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30009,13 +30021,13 @@
         <v>146</v>
       </c>
       <c r="C38" s="9" t="n">
-        <v>1E-007</v>
+        <v>0</v>
       </c>
       <c r="D38" s="10" t="n">
-        <v>1E-006</v>
+        <v>0</v>
       </c>
       <c r="E38" s="10" t="n">
-        <v>1E-005</v>
+        <v>0</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="1" t="n">
@@ -30054,7 +30066,7 @@
       </c>
       <c r="R38" s="4" t="n">
         <f aca="false">AND(E38&gt;D38,C38 &lt; D38)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36366,14 +36378,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="13" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="9" style="13" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="13" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="13" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="13" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="13" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="9" style="13" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="13" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="13" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="13" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36537,12 +36549,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36658,15 +36670,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40562,12 +40574,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40630,11 +40642,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40985,12 +40997,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
função para excluir variáveis não desejadas
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados.xlsx
+++ b/tests/testthat/Dados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Constantes" sheetId="1" state="visible" r:id="rId2"/>
@@ -51,8 +51,8 @@
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MódulosOpcionais!$A$1:$C$18</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Parametros!$A$1:$R$149</definedName>
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Verificação_Parametros!$A$1:$H$110</definedName>
-    <definedName function="false" hidden="false" name="aaaa" vbProcedure="false">[1]Configs!$D$2</definedName>
-    <definedName function="false" hidden="false" name="AAAAAA" vbProcedure="false">[1]Configs!$C$2</definedName>
+    <definedName function="false" hidden="false" name="aaaa" vbProcedure="false">[4]Configs!$D$2</definedName>
+    <definedName function="false" hidden="false" name="AAAAAA" vbProcedure="false">[4]Configs!$C$2</definedName>
     <definedName function="false" hidden="false" name="Anos_a_Serem_Simulados" vbProcedure="false">configs!#REF!</definedName>
     <definedName function="false" hidden="false" name="Ano_Inicial" vbProcedure="false">Configs!$A$2:$A$2</definedName>
     <definedName function="false" hidden="false" name="CategoriaSAT" vbProcedure="false">configs!#REF!</definedName>
@@ -71,6 +71,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Constantes!$A$1:$C$52</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Constantes!$A$1:$C$52</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Constantes!$A$1:$C$52</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Constantes!$A$1:$C$52</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MódulosOpcionais!$A$1:$C$18</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MódulosOpcionais!$A$1:$C$18</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">MódulosOpcionais!$A$1:$C$18</definedName>
@@ -86,6 +87,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MódulosOpcionais!$A$1:$C$18</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MódulosOpcionais!$A$1:$C$18</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MódulosOpcionais!$A$1:$C$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MódulosOpcionais!$A$1:$C$18</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Parametros!$A$1:$R$149</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parametros!$A$1:$R$149</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parametros!$A$1:$R$149</definedName>
@@ -101,9 +103,10 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parametros!$A$1:$R$149</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parametros!$A$1:$R$149</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parametros!$A$1:$R$149</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="Anos_a_Serem_Simulados" vbProcedure="false">[2]Configs!$A$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="Ano_Inicial" vbProcedure="false">[2]Configs!$D$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="CategoriaSAT" vbProcedure="false">[2]Configs!$C$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parametros!$A$1:$R$149</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="Anos_a_Serem_Simulados" vbProcedure="false">[5]Configs!$A$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="Ano_Inicial" vbProcedure="false">[5]Configs!$D$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="CategoriaSAT" vbProcedure="false">[5]Configs!$C$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Verificação_Parametros!$A$1:$H$110</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">Verificação_Parametros!$A$1:$H$110</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Verificação_Parametros!$A$1:$H$110</definedName>
@@ -119,6 +122,7 @@
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Verificação_Parametros!$A$1:$H$110</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Verificação_Parametros!$A$1:$H$110</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Verificação_Parametros!$A$1:$H$110</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Verificação_Parametros!$A$1:$H$110</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">Custos!$A$1:$D$18</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">Custos!$A$1:$D$18</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Custos!$A$1:$D$18</definedName>
@@ -134,6 +138,7 @@
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Custos!$A$1:$D$18</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Custos!$A$1:$D$18</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Custos!$A$1:$D$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Custos!$A$1:$D$18</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Modulos!$A$1:$D$26</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">Modulos!$A$1:$D$26</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Modulos!$A$1:$D$26</definedName>
@@ -149,9 +154,10 @@
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Modulos!$A$1:$D$26</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Modulos!$A$1:$D$26</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Modulos!$A$1:$D$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="Anos_a_Serem_Simulados" vbProcedure="false">[3]Configs!$A$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="Ano_Inicial" vbProcedure="false">[3]Configs!$D$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="CategoriaSAT" vbProcedure="false">[3]Configs!$C$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Modulos!$A$1:$D$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="Anos_a_Serem_Simulados" vbProcedure="false">[6]Configs!$A$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="Ano_Inicial" vbProcedure="false">[6]Configs!$D$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="CategoriaSAT" vbProcedure="false">[6]Configs!$C$2</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Cenarios!$A$1:$D$13</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0" vbProcedure="false">Cenarios!$A$1:$D$13</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Cenarios!$A$1:$D$13</definedName>
@@ -167,6 +173,7 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Cenarios!$A$1:$D$13</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Cenarios!$A$1:$D$13</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Cenarios!$A$1:$D$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Cenarios!$A$1:$D$13</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Historico!$A$1:$T$115</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0" vbProcedure="false">Historico!$A$1:$T$115</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Historico!$A$1:$T$115</definedName>
@@ -182,6 +189,7 @@
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Historico!$A$1:$T$115</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Historico!$A$1:$T$115</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Historico!$A$1:$T$115</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Historico!$A$1:$T$115</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">Eventos_Inic!$A$2:$L$19</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0" vbProcedure="false">Eventos_Inic!$A$2:$L$19</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Eventos_Inic!$A$2:$L$19</definedName>
@@ -197,6 +205,7 @@
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Eventos_Inic!$A$2:$L$19</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Eventos_Inic!$A$2:$L$19</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Eventos_Inic!$A$2:$L$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Eventos_Inic!$A$2:$L$19</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">Lista_de_Parâmetros!$A$1:$E$132</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0" vbProcedure="false">Lista_de_Parâmetros!$A$1:$E$132</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Lista_de_Parâmetros!$A$1:$E$132</definedName>
@@ -212,6 +221,7 @@
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Lista_de_Parâmetros!$A$1:$E$132</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Lista_de_Parâmetros!$A$1:$E$132</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Lista_de_Parâmetros!$A$1:$E$132</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Lista_de_Parâmetros!$A$1:$E$132</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase" vbProcedure="false">Funcoes_Inputs!$A$1:$I$226</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0" vbProcedure="false">Funcoes_Inputs!$A$1:$I$226</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Funcoes_Inputs!$A$1:$I$226</definedName>
@@ -227,6 +237,7 @@
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Funcoes_Inputs!$A$1:$I$226</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Funcoes_Inputs!$A$1:$I$226</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Funcoes_Inputs!$A$1:$I$226</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Funcoes_Inputs!$A$1:$I$226</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase" vbProcedure="false">Funcoes_Outputs!$A$1:$C$88</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0" vbProcedure="false">Funcoes_Outputs!$A$1:$C$88</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Funcoes_Outputs!$A$1:$C$88</definedName>
@@ -242,9 +253,10 @@
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Funcoes_Outputs!$A$1:$C$88</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Funcoes_Outputs!$A$1:$C$88</definedName>
     <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Funcoes_Outputs!$A$1:$C$88</definedName>
-    <definedName function="false" hidden="false" localSheetId="20" name="Anos_a_Serem_Simulados" vbProcedure="false">[1]Configs!$A$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="20" name="Ano_Inicial" vbProcedure="false">[1]Configs!$D$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="20" name="CategoriaSAT" vbProcedure="false">[1]Configs!$C$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="18" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Funcoes_Outputs!$A$1:$C$88</definedName>
+    <definedName function="false" hidden="false" localSheetId="20" name="Anos_a_Serem_Simulados" vbProcedure="false">[4]Configs!$A$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="20" name="Ano_Inicial" vbProcedure="false">[4]Configs!$D$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="20" name="CategoriaSAT" vbProcedure="false">[4]Configs!$C$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2647,19 +2659,19 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -2678,11 +2690,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3518,8 +3530,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3552,11 +3564,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3821,13 +3832,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="75.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="74.9183673469388"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3983,20 +3993,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="91.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="12" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="90.5816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="16" min="12" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8731,8 +8740,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9744897959184"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10172,25 +10180,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="47" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="47" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="47" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="32" min="23" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="36" min="33" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="37" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="47" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="47" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="47" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="32" min="23" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="36" min="33" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="37" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10807,19 +10815,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.1224489795918"/>
     <col collapsed="false" hidden="true" max="11" min="10" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="35.234693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11651,11 +11657,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="105.025510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="103.80612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.0357142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14067,24 +14072,24 @@
   </sheetPr>
   <dimension ref="A1:I226"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A156" activeCellId="0" sqref="A156"/>
+      <selection pane="bottomLeft" activeCell="D44" activeCellId="0" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="34.1530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.75"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15852,8 +15857,7 @@
         <v>529</v>
       </c>
       <c r="C50" s="1" t="n">
-        <f aca="false">1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" s="1" t="n">
         <f aca="false">VLOOKUP(A50,Modulos!A:C,2,0)</f>
@@ -15861,11 +15865,11 @@
       </c>
       <c r="E50" s="1" t="str">
         <f aca="false">IF(C50,"Nenhuma",VLOOKUP(B50,Funcoes_Outputs!B:C,2,0))</f>
-        <v>Nenhuma</v>
+        <v>calcular_turnovergeral</v>
       </c>
       <c r="F50" s="1" t="n">
         <f aca="false">AND(C50,D50)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50" s="1" t="n">
         <f aca="false">VLOOKUP(A50,Modulos!$A:$C,2,0)</f>
@@ -15873,7 +15877,7 @@
       </c>
       <c r="H50" s="1" t="n">
         <f aca="false">AND(G50,C50)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" s="1" t="n">
         <f aca="false">COUNTIF($B:$B,B50)</f>
@@ -19624,7 +19628,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
         <v>80</v>
       </c>
@@ -22242,10 +22246,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23329,10 +23332,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23560,10 +23563,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24314,9 +24316,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24784,8 +24786,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25506,9 +25508,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26192,12 +26194,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26910,30 +26912,30 @@
   </sheetPr>
   <dimension ref="1:149"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="6" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="73.8418367346939"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="6" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="73.030612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36465,14 +36467,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="15" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="15" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="15" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="9" style="15" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="15" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="15" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="15" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="15" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="15" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="15" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="9" style="15" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="15" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="15" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="15" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36636,12 +36638,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="6.75"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36757,15 +36759,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40661,12 +40663,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40729,11 +40731,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="14.5816326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41084,12 +41085,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.1071428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>